<commit_message>
CAN acceptance filter working
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="132">
   <si>
     <t>CAN-Messages</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>40-64</t>
+  </si>
+  <si>
+    <t>Datenbuffergrösse (2550 Byte)</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +512,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -744,6 +753,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,9 +787,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -807,6 +819,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -825,16 +852,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -843,11 +861,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,115 +1186,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
       <c r="AK1" s="9"/>
-      <c r="AL1" s="48" t="s">
+      <c r="AL1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="48"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="48"/>
-      <c r="AY1" s="48"/>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="48"/>
-      <c r="BM1" s="48"/>
-      <c r="BN1" s="48"/>
-      <c r="BO1" s="48"/>
-      <c r="BP1" s="48"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="48"/>
-      <c r="BS1" s="48"/>
-      <c r="BT1" s="48"/>
-      <c r="BU1" s="48"/>
-      <c r="BV1" s="48"/>
-      <c r="BW1" s="48"/>
-      <c r="BX1" s="48"/>
-      <c r="BY1" s="48"/>
-      <c r="BZ1" s="48"/>
-      <c r="CA1" s="48"/>
-      <c r="CB1" s="48"/>
-      <c r="CC1" s="48"/>
-      <c r="CD1" s="48"/>
-      <c r="CE1" s="48"/>
-      <c r="CF1" s="48"/>
-      <c r="CG1" s="48"/>
-      <c r="CH1" s="48"/>
-      <c r="CI1" s="48"/>
-      <c r="CJ1" s="48"/>
-      <c r="CK1" s="48"/>
-      <c r="CL1" s="48"/>
-      <c r="CM1" s="48"/>
-      <c r="CN1" s="48"/>
-      <c r="CO1" s="48"/>
-      <c r="CP1" s="48"/>
-      <c r="CQ1" s="48"/>
-      <c r="CR1" s="48"/>
-      <c r="CS1" s="48"/>
-      <c r="CT1" s="48"/>
-      <c r="CU1" s="48"/>
-      <c r="CV1" s="48"/>
-      <c r="CW1" s="48"/>
+      <c r="AM1" s="49"/>
+      <c r="AN1" s="49"/>
+      <c r="AO1" s="49"/>
+      <c r="AP1" s="49"/>
+      <c r="AQ1" s="49"/>
+      <c r="AR1" s="49"/>
+      <c r="AS1" s="49"/>
+      <c r="AT1" s="49"/>
+      <c r="AU1" s="49"/>
+      <c r="AV1" s="49"/>
+      <c r="AW1" s="49"/>
+      <c r="AX1" s="49"/>
+      <c r="AY1" s="49"/>
+      <c r="AZ1" s="49"/>
+      <c r="BA1" s="49"/>
+      <c r="BB1" s="49"/>
+      <c r="BC1" s="49"/>
+      <c r="BD1" s="49"/>
+      <c r="BE1" s="49"/>
+      <c r="BF1" s="49"/>
+      <c r="BG1" s="49"/>
+      <c r="BH1" s="49"/>
+      <c r="BI1" s="49"/>
+      <c r="BJ1" s="49"/>
+      <c r="BK1" s="49"/>
+      <c r="BL1" s="49"/>
+      <c r="BM1" s="49"/>
+      <c r="BN1" s="49"/>
+      <c r="BO1" s="49"/>
+      <c r="BP1" s="49"/>
+      <c r="BQ1" s="49"/>
+      <c r="BR1" s="49"/>
+      <c r="BS1" s="49"/>
+      <c r="BT1" s="49"/>
+      <c r="BU1" s="49"/>
+      <c r="BV1" s="49"/>
+      <c r="BW1" s="49"/>
+      <c r="BX1" s="49"/>
+      <c r="BY1" s="49"/>
+      <c r="BZ1" s="49"/>
+      <c r="CA1" s="49"/>
+      <c r="CB1" s="49"/>
+      <c r="CC1" s="49"/>
+      <c r="CD1" s="49"/>
+      <c r="CE1" s="49"/>
+      <c r="CF1" s="49"/>
+      <c r="CG1" s="49"/>
+      <c r="CH1" s="49"/>
+      <c r="CI1" s="49"/>
+      <c r="CJ1" s="49"/>
+      <c r="CK1" s="49"/>
+      <c r="CL1" s="49"/>
+      <c r="CM1" s="49"/>
+      <c r="CN1" s="49"/>
+      <c r="CO1" s="49"/>
+      <c r="CP1" s="49"/>
+      <c r="CQ1" s="49"/>
+      <c r="CR1" s="49"/>
+      <c r="CS1" s="49"/>
+      <c r="CT1" s="49"/>
+      <c r="CU1" s="49"/>
+      <c r="CV1" s="49"/>
+      <c r="CW1" s="49"/>
       <c r="CX1" s="1" t="s">
         <v>81</v>
       </c>
@@ -1700,7 +1715,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -1758,41 +1773,82 @@
       <c r="AB4" s="14">
         <v>1</v>
       </c>
-      <c r="AC4" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
-      <c r="AG4" s="44"/>
-      <c r="AH4" s="44"/>
-      <c r="AI4" s="44"/>
-      <c r="AJ4" s="45"/>
+      <c r="AC4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="15">
+        <v>1</v>
+      </c>
       <c r="AK4" s="10"/>
-      <c r="AL4" s="39" t="s">
+      <c r="AL4" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="AM4" s="40"/>
-      <c r="AN4" s="40"/>
-      <c r="AO4" s="40"/>
-      <c r="AP4" s="40"/>
-      <c r="AQ4" s="40"/>
-      <c r="AR4" s="40"/>
-      <c r="AS4" s="40"/>
-      <c r="AU4" s="3"/>
-      <c r="BA4" s="18"/>
-      <c r="BE4" s="3"/>
-      <c r="BI4" s="18"/>
-      <c r="BO4" s="3"/>
-      <c r="BQ4" s="18"/>
-      <c r="BY4" s="20"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="42"/>
+      <c r="AO4" s="42"/>
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="42"/>
+      <c r="AS4" s="42"/>
+      <c r="AT4" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU4" s="72"/>
+      <c r="AV4" s="72"/>
+      <c r="AW4" s="72"/>
+      <c r="AX4" s="72"/>
+      <c r="AY4" s="72"/>
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="72"/>
+      <c r="BE4" s="72"/>
+      <c r="BF4" s="72"/>
+      <c r="BG4" s="72"/>
+      <c r="BH4" s="72"/>
+      <c r="BI4" s="72"/>
+      <c r="BJ4" s="72"/>
+      <c r="BK4" s="72"/>
+      <c r="BL4" s="72"/>
+      <c r="BM4" s="72"/>
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="72"/>
+      <c r="BP4" s="72"/>
+      <c r="BQ4" s="72"/>
+      <c r="BR4" s="72"/>
+      <c r="BS4" s="72"/>
+      <c r="BT4" s="72"/>
+      <c r="BU4" s="72"/>
+      <c r="BV4" s="72"/>
+      <c r="BW4" s="72"/>
+      <c r="BX4" s="72"/>
+      <c r="BY4" s="72"/>
       <c r="CG4" s="18"/>
       <c r="CI4" s="3"/>
       <c r="CO4" s="18"/>
       <c r="CS4" s="3"/>
       <c r="CW4" s="18"/>
       <c r="CX4">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.25">
@@ -1803,7 +1859,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1861,77 +1917,72 @@
       <c r="AB5" s="14">
         <v>1</v>
       </c>
-      <c r="AC5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="15">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="15">
-        <v>1</v>
-      </c>
+      <c r="AC5" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="47"/>
       <c r="AK5" s="10"/>
-      <c r="AL5" s="50" t="s">
+      <c r="AL5" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="51"/>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="51"/>
-      <c r="AS5" s="51"/>
-      <c r="AT5" s="51"/>
-      <c r="AU5" s="51"/>
-      <c r="AV5" s="52" t="s">
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="AW5" s="52"/>
-      <c r="AX5" s="52"/>
-      <c r="AY5" s="52"/>
-      <c r="AZ5" s="52"/>
-      <c r="BA5" s="52"/>
-      <c r="BB5" s="52"/>
-      <c r="BC5" s="52"/>
-      <c r="BD5" s="52"/>
-      <c r="BE5" s="52"/>
-      <c r="BF5" s="53" t="s">
+      <c r="AW5" s="53"/>
+      <c r="AX5" s="53"/>
+      <c r="AY5" s="53"/>
+      <c r="AZ5" s="53"/>
+      <c r="BA5" s="53"/>
+      <c r="BB5" s="53"/>
+      <c r="BC5" s="53"/>
+      <c r="BD5" s="53"/>
+      <c r="BE5" s="53"/>
+      <c r="BF5" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="BG5" s="53"/>
-      <c r="BH5" s="53"/>
-      <c r="BI5" s="53"/>
-      <c r="BJ5" s="53"/>
-      <c r="BK5" s="53"/>
-      <c r="BL5" s="53"/>
-      <c r="BM5" s="53"/>
-      <c r="BN5" s="53"/>
-      <c r="BO5" s="53"/>
-      <c r="BP5" s="53"/>
-      <c r="BQ5" s="53"/>
-      <c r="BY5" s="20"/>
+      <c r="BG5" s="54"/>
+      <c r="BH5" s="54"/>
+      <c r="BI5" s="54"/>
+      <c r="BJ5" s="54"/>
+      <c r="BK5" s="54"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="54"/>
+      <c r="BN5" s="54"/>
+      <c r="BO5" s="54"/>
+      <c r="BP5" s="54"/>
+      <c r="BQ5" s="54"/>
+      <c r="BR5" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="BS5" s="37"/>
+      <c r="BT5" s="37"/>
+      <c r="BU5" s="37"/>
+      <c r="BV5" s="37"/>
+      <c r="BW5" s="37"/>
+      <c r="BX5" s="37"/>
+      <c r="BY5" s="37"/>
       <c r="CG5" s="18"/>
       <c r="CI5" s="3"/>
       <c r="CO5" s="18"/>
       <c r="CS5" s="3"/>
       <c r="CW5" s="18"/>
       <c r="CX5">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.25">
@@ -2000,27 +2051,27 @@
       <c r="AB6" s="14">
         <v>1</v>
       </c>
-      <c r="AC6" s="43" t="s">
+      <c r="AC6" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="44"/>
-      <c r="AG6" s="44"/>
-      <c r="AH6" s="44"/>
-      <c r="AI6" s="44"/>
-      <c r="AJ6" s="45"/>
+      <c r="AD6" s="46"/>
+      <c r="AE6" s="46"/>
+      <c r="AF6" s="46"/>
+      <c r="AG6" s="46"/>
+      <c r="AH6" s="46"/>
+      <c r="AI6" s="46"/>
+      <c r="AJ6" s="47"/>
       <c r="AK6" s="10"/>
-      <c r="AL6" s="39" t="s">
+      <c r="AL6" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="AM6" s="40"/>
-      <c r="AN6" s="40"/>
-      <c r="AO6" s="40"/>
-      <c r="AP6" s="40"/>
-      <c r="AQ6" s="40"/>
-      <c r="AR6" s="40"/>
-      <c r="AS6" s="40"/>
+      <c r="AM6" s="42"/>
+      <c r="AN6" s="42"/>
+      <c r="AO6" s="42"/>
+      <c r="AP6" s="42"/>
+      <c r="AQ6" s="42"/>
+      <c r="AR6" s="42"/>
+      <c r="AS6" s="42"/>
       <c r="AU6" s="3"/>
       <c r="BA6" s="18"/>
       <c r="BE6" s="3"/>
@@ -2103,27 +2154,27 @@
       <c r="AB7" s="14">
         <v>1</v>
       </c>
-      <c r="AC7" s="43" t="s">
+      <c r="AC7" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="AD7" s="44"/>
-      <c r="AE7" s="44"/>
-      <c r="AF7" s="44"/>
-      <c r="AG7" s="44"/>
-      <c r="AH7" s="44"/>
-      <c r="AI7" s="44"/>
-      <c r="AJ7" s="45"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="46"/>
+      <c r="AI7" s="46"/>
+      <c r="AJ7" s="47"/>
       <c r="AK7" s="10"/>
-      <c r="AL7" s="39" t="s">
+      <c r="AL7" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="AM7" s="40"/>
-      <c r="AN7" s="40"/>
-      <c r="AO7" s="40"/>
-      <c r="AP7" s="40"/>
-      <c r="AQ7" s="40"/>
-      <c r="AR7" s="40"/>
-      <c r="AS7" s="40"/>
+      <c r="AM7" s="42"/>
+      <c r="AN7" s="42"/>
+      <c r="AO7" s="42"/>
+      <c r="AP7" s="42"/>
+      <c r="AQ7" s="42"/>
+      <c r="AR7" s="42"/>
+      <c r="AS7" s="42"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="18"/>
       <c r="BE7" s="3"/>
@@ -2174,16 +2225,16 @@
       <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="63" t="s">
+      <c r="M8" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="63"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="14">
         <v>0</v>
       </c>
@@ -2208,35 +2259,35 @@
       <c r="AB8" s="14">
         <v>1</v>
       </c>
-      <c r="AC8" s="43" t="s">
+      <c r="AC8" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="44"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="44"/>
-      <c r="AH8" s="44"/>
-      <c r="AI8" s="44"/>
-      <c r="AJ8" s="45"/>
+      <c r="AD8" s="46"/>
+      <c r="AE8" s="46"/>
+      <c r="AF8" s="46"/>
+      <c r="AG8" s="46"/>
+      <c r="AH8" s="46"/>
+      <c r="AI8" s="46"/>
+      <c r="AJ8" s="47"/>
       <c r="AK8" s="10"/>
-      <c r="AL8" s="40" t="s">
+      <c r="AL8" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="AM8" s="40"/>
-      <c r="AN8" s="40"/>
-      <c r="AO8" s="40"/>
-      <c r="AP8" s="40"/>
-      <c r="AQ8" s="40"/>
-      <c r="AR8" s="40"/>
-      <c r="AS8" s="40"/>
-      <c r="AT8" s="40"/>
-      <c r="AU8" s="40"/>
-      <c r="AV8" s="40"/>
-      <c r="AW8" s="40"/>
-      <c r="AX8" s="40"/>
-      <c r="AY8" s="40"/>
-      <c r="AZ8" s="40"/>
-      <c r="BA8" s="40"/>
+      <c r="AM8" s="42"/>
+      <c r="AN8" s="42"/>
+      <c r="AO8" s="42"/>
+      <c r="AP8" s="42"/>
+      <c r="AQ8" s="42"/>
+      <c r="AR8" s="42"/>
+      <c r="AS8" s="42"/>
+      <c r="AT8" s="42"/>
+      <c r="AU8" s="42"/>
+      <c r="AV8" s="42"/>
+      <c r="AW8" s="42"/>
+      <c r="AX8" s="42"/>
+      <c r="AY8" s="42"/>
+      <c r="AZ8" s="42"/>
+      <c r="BA8" s="42"/>
       <c r="BE8" s="3"/>
       <c r="BI8" s="18"/>
       <c r="BO8" s="3"/>
@@ -2401,16 +2452,30 @@
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
-      <c r="U10" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="58"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="58"/>
-      <c r="AB10" s="59"/>
+      <c r="U10" s="14">
+        <v>0</v>
+      </c>
+      <c r="V10" s="14">
+        <v>0</v>
+      </c>
+      <c r="W10" s="14">
+        <v>0</v>
+      </c>
+      <c r="X10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="14">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="14">
+        <v>0</v>
+      </c>
       <c r="AC10" s="15">
         <v>0</v>
       </c>
@@ -2436,40 +2501,40 @@
         <v>1</v>
       </c>
       <c r="AK10" s="10"/>
-      <c r="AL10" s="39" t="s">
+      <c r="AL10" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="AM10" s="40"/>
-      <c r="AN10" s="40"/>
-      <c r="AO10" s="40"/>
-      <c r="AP10" s="40"/>
-      <c r="AQ10" s="40"/>
-      <c r="AR10" s="40"/>
-      <c r="AS10" s="40"/>
-      <c r="AT10" s="40"/>
-      <c r="AU10" s="40"/>
-      <c r="AV10" s="40"/>
-      <c r="AW10" s="40"/>
-      <c r="AX10" s="40"/>
-      <c r="AY10" s="40"/>
-      <c r="AZ10" s="40"/>
-      <c r="BA10" s="40"/>
-      <c r="BB10" s="40"/>
-      <c r="BC10" s="40"/>
-      <c r="BD10" s="40"/>
-      <c r="BE10" s="40"/>
-      <c r="BF10" s="40"/>
-      <c r="BG10" s="40"/>
-      <c r="BH10" s="40"/>
-      <c r="BI10" s="40"/>
-      <c r="BJ10" s="40"/>
-      <c r="BK10" s="40"/>
-      <c r="BL10" s="40"/>
-      <c r="BM10" s="40"/>
-      <c r="BN10" s="40"/>
-      <c r="BO10" s="40"/>
-      <c r="BP10" s="40"/>
-      <c r="BQ10" s="40"/>
+      <c r="AM10" s="42"/>
+      <c r="AN10" s="42"/>
+      <c r="AO10" s="42"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="42"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="42"/>
+      <c r="AT10" s="42"/>
+      <c r="AU10" s="42"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="42"/>
+      <c r="AX10" s="42"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="42"/>
+      <c r="BA10" s="42"/>
+      <c r="BB10" s="42"/>
+      <c r="BC10" s="42"/>
+      <c r="BD10" s="42"/>
+      <c r="BE10" s="42"/>
+      <c r="BF10" s="42"/>
+      <c r="BG10" s="42"/>
+      <c r="BH10" s="42"/>
+      <c r="BI10" s="42"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="42"/>
+      <c r="BL10" s="42"/>
+      <c r="BM10" s="42"/>
+      <c r="BN10" s="42"/>
+      <c r="BO10" s="42"/>
+      <c r="BP10" s="42"/>
+      <c r="BQ10" s="42"/>
       <c r="BY10" s="20"/>
       <c r="CG10" s="18"/>
       <c r="CI10" s="3"/>
@@ -2517,26 +2582,26 @@
       <c r="L11" s="12">
         <v>1</v>
       </c>
-      <c r="M11" s="64" t="s">
+      <c r="M11" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="57" t="s">
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="V11" s="58"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="58"/>
-      <c r="AB11" s="59"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="64"/>
+      <c r="Y11" s="64"/>
+      <c r="Z11" s="64"/>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="65"/>
       <c r="AC11" s="15">
         <v>0</v>
       </c>
@@ -2562,40 +2627,40 @@
         <v>1</v>
       </c>
       <c r="AK11" s="10"/>
-      <c r="AL11" s="39" t="s">
+      <c r="AL11" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="AM11" s="40"/>
-      <c r="AN11" s="40"/>
-      <c r="AO11" s="40"/>
-      <c r="AP11" s="40"/>
-      <c r="AQ11" s="40"/>
-      <c r="AR11" s="40"/>
-      <c r="AS11" s="40"/>
-      <c r="AT11" s="40"/>
-      <c r="AU11" s="40"/>
-      <c r="AV11" s="40"/>
-      <c r="AW11" s="40"/>
-      <c r="AX11" s="40"/>
-      <c r="AY11" s="40"/>
-      <c r="AZ11" s="40"/>
-      <c r="BA11" s="40"/>
-      <c r="BB11" s="40"/>
-      <c r="BC11" s="40"/>
-      <c r="BD11" s="40"/>
-      <c r="BE11" s="40"/>
-      <c r="BF11" s="40"/>
-      <c r="BG11" s="40"/>
-      <c r="BH11" s="40"/>
-      <c r="BI11" s="40"/>
-      <c r="BJ11" s="40"/>
-      <c r="BK11" s="40"/>
-      <c r="BL11" s="40"/>
-      <c r="BM11" s="40"/>
-      <c r="BN11" s="40"/>
-      <c r="BO11" s="40"/>
-      <c r="BP11" s="40"/>
-      <c r="BQ11" s="40"/>
+      <c r="AM11" s="42"/>
+      <c r="AN11" s="42"/>
+      <c r="AO11" s="42"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="42"/>
+      <c r="AR11" s="42"/>
+      <c r="AS11" s="42"/>
+      <c r="AT11" s="42"/>
+      <c r="AU11" s="42"/>
+      <c r="AV11" s="42"/>
+      <c r="AW11" s="42"/>
+      <c r="AX11" s="42"/>
+      <c r="AY11" s="42"/>
+      <c r="AZ11" s="42"/>
+      <c r="BA11" s="42"/>
+      <c r="BB11" s="42"/>
+      <c r="BC11" s="42"/>
+      <c r="BD11" s="42"/>
+      <c r="BE11" s="42"/>
+      <c r="BF11" s="42"/>
+      <c r="BG11" s="42"/>
+      <c r="BH11" s="42"/>
+      <c r="BI11" s="42"/>
+      <c r="BJ11" s="42"/>
+      <c r="BK11" s="42"/>
+      <c r="BL11" s="42"/>
+      <c r="BM11" s="42"/>
+      <c r="BN11" s="42"/>
+      <c r="BO11" s="42"/>
+      <c r="BP11" s="42"/>
+      <c r="BQ11" s="42"/>
       <c r="BR11" s="69" t="s">
         <v>124</v>
       </c>
@@ -2636,7 +2701,7 @@
       <c r="CU11" s="69"/>
       <c r="CV11" s="69"/>
       <c r="CW11" s="69"/>
-      <c r="CX11" s="70" t="s">
+      <c r="CX11" s="36" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2674,26 +2739,26 @@
       <c r="L12" s="12">
         <v>0</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="M12" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="57" t="s">
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="58"/>
-      <c r="AB12" s="59"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="64"/>
+      <c r="X12" s="64"/>
+      <c r="Y12" s="64"/>
+      <c r="Z12" s="64"/>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="65"/>
       <c r="AC12" s="15">
         <v>0</v>
       </c>
@@ -2799,7 +2864,7 @@
       <c r="CU12" s="69"/>
       <c r="CV12" s="69"/>
       <c r="CW12" s="69"/>
-      <c r="CX12" s="70" t="s">
+      <c r="CX12" s="36" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2837,26 +2902,26 @@
       <c r="L13" s="12">
         <v>1</v>
       </c>
-      <c r="M13" s="64" t="s">
+      <c r="M13" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="65"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="57" t="s">
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="58"/>
-      <c r="AB13" s="59"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="64"/>
+      <c r="X13" s="64"/>
+      <c r="Y13" s="64"/>
+      <c r="Z13" s="64"/>
+      <c r="AA13" s="64"/>
+      <c r="AB13" s="65"/>
       <c r="AC13" s="15">
         <v>0</v>
       </c>
@@ -2882,70 +2947,70 @@
         <v>1</v>
       </c>
       <c r="AK13" s="10"/>
-      <c r="AL13" s="39" t="s">
+      <c r="AL13" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="AM13" s="40"/>
-      <c r="AN13" s="40"/>
-      <c r="AO13" s="40"/>
-      <c r="AP13" s="40"/>
-      <c r="AQ13" s="40"/>
-      <c r="AR13" s="40"/>
-      <c r="AS13" s="40"/>
-      <c r="AT13" s="40"/>
-      <c r="AU13" s="40"/>
-      <c r="AV13" s="40"/>
-      <c r="AW13" s="40"/>
-      <c r="AX13" s="40"/>
-      <c r="AY13" s="40"/>
-      <c r="AZ13" s="40"/>
-      <c r="BA13" s="40"/>
-      <c r="BB13" s="40"/>
-      <c r="BC13" s="40"/>
-      <c r="BD13" s="40"/>
-      <c r="BE13" s="40"/>
-      <c r="BF13" s="40"/>
-      <c r="BG13" s="40"/>
-      <c r="BH13" s="40"/>
-      <c r="BI13" s="40"/>
-      <c r="BJ13" s="40"/>
-      <c r="BK13" s="40"/>
-      <c r="BL13" s="40"/>
-      <c r="BM13" s="40"/>
-      <c r="BN13" s="40"/>
-      <c r="BO13" s="40"/>
-      <c r="BP13" s="40"/>
-      <c r="BQ13" s="40"/>
-      <c r="BR13" s="67" t="s">
+      <c r="AM13" s="42"/>
+      <c r="AN13" s="42"/>
+      <c r="AO13" s="42"/>
+      <c r="AP13" s="42"/>
+      <c r="AQ13" s="42"/>
+      <c r="AR13" s="42"/>
+      <c r="AS13" s="42"/>
+      <c r="AT13" s="42"/>
+      <c r="AU13" s="42"/>
+      <c r="AV13" s="42"/>
+      <c r="AW13" s="42"/>
+      <c r="AX13" s="42"/>
+      <c r="AY13" s="42"/>
+      <c r="AZ13" s="42"/>
+      <c r="BA13" s="42"/>
+      <c r="BB13" s="42"/>
+      <c r="BC13" s="42"/>
+      <c r="BD13" s="42"/>
+      <c r="BE13" s="42"/>
+      <c r="BF13" s="42"/>
+      <c r="BG13" s="42"/>
+      <c r="BH13" s="42"/>
+      <c r="BI13" s="42"/>
+      <c r="BJ13" s="42"/>
+      <c r="BK13" s="42"/>
+      <c r="BL13" s="42"/>
+      <c r="BM13" s="42"/>
+      <c r="BN13" s="42"/>
+      <c r="BO13" s="42"/>
+      <c r="BP13" s="42"/>
+      <c r="BQ13" s="42"/>
+      <c r="BR13" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="BS13" s="67"/>
-      <c r="BT13" s="67"/>
-      <c r="BU13" s="67"/>
-      <c r="BV13" s="67"/>
-      <c r="BW13" s="67"/>
-      <c r="BX13" s="67"/>
-      <c r="BY13" s="67"/>
-      <c r="BZ13" s="68" t="s">
+      <c r="BS13" s="70"/>
+      <c r="BT13" s="70"/>
+      <c r="BU13" s="70"/>
+      <c r="BV13" s="70"/>
+      <c r="BW13" s="70"/>
+      <c r="BX13" s="70"/>
+      <c r="BY13" s="70"/>
+      <c r="BZ13" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="CA13" s="68"/>
-      <c r="CB13" s="68"/>
-      <c r="CC13" s="68"/>
-      <c r="CD13" s="68"/>
-      <c r="CE13" s="68"/>
-      <c r="CF13" s="68"/>
-      <c r="CG13" s="68"/>
-      <c r="CH13" s="53" t="s">
+      <c r="CA13" s="71"/>
+      <c r="CB13" s="71"/>
+      <c r="CC13" s="71"/>
+      <c r="CD13" s="71"/>
+      <c r="CE13" s="71"/>
+      <c r="CF13" s="71"/>
+      <c r="CG13" s="71"/>
+      <c r="CH13" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="CI13" s="53"/>
-      <c r="CJ13" s="53"/>
-      <c r="CK13" s="53"/>
-      <c r="CL13" s="53"/>
-      <c r="CM13" s="53"/>
-      <c r="CN13" s="53"/>
-      <c r="CO13" s="53"/>
+      <c r="CI13" s="54"/>
+      <c r="CJ13" s="54"/>
+      <c r="CK13" s="54"/>
+      <c r="CL13" s="54"/>
+      <c r="CM13" s="54"/>
+      <c r="CN13" s="54"/>
+      <c r="CO13" s="54"/>
       <c r="CS13" s="3"/>
       <c r="CW13" s="18"/>
       <c r="CX13">
@@ -2995,16 +3060,16 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
-      <c r="U14" s="60" t="s">
+      <c r="U14" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="62"/>
+      <c r="V14" s="67"/>
+      <c r="W14" s="67"/>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="67"/>
+      <c r="Z14" s="67"/>
+      <c r="AA14" s="67"/>
+      <c r="AB14" s="68"/>
       <c r="AC14" s="26">
         <v>0</v>
       </c>
@@ -3078,26 +3143,26 @@
       <c r="L15" s="12">
         <v>1</v>
       </c>
-      <c r="M15" s="64" t="s">
+      <c r="M15" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="66"/>
-      <c r="U15" s="57" t="s">
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="58"/>
-      <c r="Z15" s="58"/>
-      <c r="AA15" s="58"/>
-      <c r="AB15" s="59"/>
+      <c r="V15" s="64"/>
+      <c r="W15" s="64"/>
+      <c r="X15" s="64"/>
+      <c r="Y15" s="64"/>
+      <c r="Z15" s="64"/>
+      <c r="AA15" s="64"/>
+      <c r="AB15" s="65"/>
       <c r="AC15" s="15">
         <v>0</v>
       </c>
@@ -3123,42 +3188,42 @@
         <v>1</v>
       </c>
       <c r="AK15" s="10"/>
-      <c r="AL15" s="39" t="s">
+      <c r="AL15" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="AM15" s="40"/>
-      <c r="AN15" s="40"/>
-      <c r="AO15" s="40"/>
-      <c r="AP15" s="40"/>
-      <c r="AQ15" s="40"/>
-      <c r="AR15" s="40"/>
-      <c r="AS15" s="40"/>
-      <c r="AT15" s="53" t="s">
+      <c r="AM15" s="42"/>
+      <c r="AN15" s="42"/>
+      <c r="AO15" s="42"/>
+      <c r="AP15" s="42"/>
+      <c r="AQ15" s="42"/>
+      <c r="AR15" s="42"/>
+      <c r="AS15" s="42"/>
+      <c r="AT15" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="AU15" s="53"/>
-      <c r="AV15" s="53"/>
-      <c r="AW15" s="53"/>
-      <c r="AX15" s="53"/>
-      <c r="AY15" s="53"/>
-      <c r="AZ15" s="53"/>
-      <c r="BA15" s="53"/>
-      <c r="BB15" s="53"/>
-      <c r="BC15" s="53"/>
-      <c r="BD15" s="53"/>
-      <c r="BE15" s="53"/>
-      <c r="BF15" s="53"/>
-      <c r="BG15" s="53"/>
-      <c r="BH15" s="53"/>
-      <c r="BI15" s="53"/>
-      <c r="BJ15" s="53"/>
-      <c r="BK15" s="53"/>
-      <c r="BL15" s="53"/>
-      <c r="BM15" s="53"/>
-      <c r="BN15" s="53"/>
-      <c r="BO15" s="53"/>
-      <c r="BP15" s="53"/>
-      <c r="BQ15" s="53"/>
+      <c r="AU15" s="54"/>
+      <c r="AV15" s="54"/>
+      <c r="AW15" s="54"/>
+      <c r="AX15" s="54"/>
+      <c r="AY15" s="54"/>
+      <c r="AZ15" s="54"/>
+      <c r="BA15" s="54"/>
+      <c r="BB15" s="54"/>
+      <c r="BC15" s="54"/>
+      <c r="BD15" s="54"/>
+      <c r="BE15" s="54"/>
+      <c r="BF15" s="54"/>
+      <c r="BG15" s="54"/>
+      <c r="BH15" s="54"/>
+      <c r="BI15" s="54"/>
+      <c r="BJ15" s="54"/>
+      <c r="BK15" s="54"/>
+      <c r="BL15" s="54"/>
+      <c r="BM15" s="54"/>
+      <c r="BN15" s="54"/>
+      <c r="BO15" s="54"/>
+      <c r="BP15" s="54"/>
+      <c r="BQ15" s="54"/>
       <c r="BY15" s="20"/>
       <c r="CG15" s="18"/>
       <c r="CI15" s="3"/>
@@ -3173,42 +3238,42 @@
       <c r="H16" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="46" t="s">
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="54" t="s">
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
-      <c r="Y16" s="54"/>
-      <c r="Z16" s="54"/>
-      <c r="AA16" s="54"/>
-      <c r="AB16" s="54"/>
-      <c r="AC16" s="55" t="s">
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="55"/>
+      <c r="AA16" s="55"/>
+      <c r="AB16" s="55"/>
+      <c r="AC16" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="AD16" s="55"/>
-      <c r="AE16" s="55"/>
-      <c r="AF16" s="55"/>
-      <c r="AG16" s="55"/>
-      <c r="AH16" s="55"/>
-      <c r="AI16" s="55"/>
-      <c r="AJ16" s="56"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
+      <c r="AH16" s="56"/>
+      <c r="AI16" s="56"/>
+      <c r="AJ16" s="57"/>
       <c r="AS16" s="18"/>
       <c r="AU16" s="3"/>
       <c r="BA16" s="18"/>
@@ -3322,43 +3387,43 @@
       <c r="AK19" s="10"/>
     </row>
     <row r="20" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="H20" s="37">
+      <c r="H20" s="39">
         <v>18</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="42" t="s">
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="42" t="s">
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="38"/>
-      <c r="AC20" s="41" t="s">
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="37"/>
-      <c r="AI20" s="37"/>
-      <c r="AJ20" s="38"/>
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="40"/>
       <c r="AK20" s="10"/>
     </row>
     <row r="21" spans="7:37" x14ac:dyDescent="0.25">
@@ -3455,43 +3520,43 @@
       <c r="AK21" s="10"/>
     </row>
     <row r="22" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="H22" s="37">
+      <c r="H22" s="39">
         <v>18</v>
       </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="42" t="s">
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="42" t="s">
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="38"/>
-      <c r="AC22" s="42" t="s">
+      <c r="V22" s="39"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="39"/>
+      <c r="Y22" s="39"/>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="40"/>
+      <c r="AC22" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="AD22" s="37"/>
-      <c r="AE22" s="37"/>
-      <c r="AF22" s="37"/>
-      <c r="AG22" s="37"/>
-      <c r="AH22" s="37"/>
-      <c r="AI22" s="37"/>
-      <c r="AJ22" s="38"/>
+      <c r="AD22" s="39"/>
+      <c r="AE22" s="39"/>
+      <c r="AF22" s="39"/>
+      <c r="AG22" s="39"/>
+      <c r="AH22" s="39"/>
+      <c r="AI22" s="39"/>
+      <c r="AJ22" s="40"/>
       <c r="AK22" s="10"/>
     </row>
     <row r="23" spans="7:37" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3620,43 +3685,43 @@
       <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="H25" s="37">
+      <c r="H25" s="39">
         <v>18</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="42" t="s">
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="41" t="s">
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="37"/>
-      <c r="AA25" s="37"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="41" t="s">
+      <c r="V25" s="39"/>
+      <c r="W25" s="39"/>
+      <c r="X25" s="39"/>
+      <c r="Y25" s="39"/>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="39"/>
+      <c r="AB25" s="40"/>
+      <c r="AC25" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="AD25" s="37"/>
-      <c r="AE25" s="37"/>
-      <c r="AF25" s="37"/>
-      <c r="AG25" s="37"/>
-      <c r="AH25" s="37"/>
-      <c r="AI25" s="37"/>
-      <c r="AJ25" s="38"/>
+      <c r="AD25" s="39"/>
+      <c r="AE25" s="39"/>
+      <c r="AF25" s="39"/>
+      <c r="AG25" s="39"/>
+      <c r="AH25" s="39"/>
+      <c r="AI25" s="39"/>
+      <c r="AJ25" s="40"/>
       <c r="AK25" s="10"/>
     </row>
     <row r="26" spans="7:37" x14ac:dyDescent="0.25">
@@ -3726,56 +3791,56 @@
       <c r="AB26" s="32">
         <v>1</v>
       </c>
-      <c r="AC26" s="43" t="s">
+      <c r="AC26" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="45"/>
+      <c r="AD26" s="46"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="46"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="47"/>
       <c r="AK26" s="10"/>
     </row>
     <row r="27" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="42" t="s">
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="42" t="s">
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
-      <c r="AA27" s="37"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="41" t="s">
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
+      <c r="AB27" s="40"/>
+      <c r="AC27" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="AD27" s="37"/>
-      <c r="AE27" s="37"/>
-      <c r="AF27" s="37"/>
-      <c r="AG27" s="37"/>
-      <c r="AH27" s="37"/>
-      <c r="AI27" s="37"/>
-      <c r="AJ27" s="38"/>
+      <c r="AD27" s="39"/>
+      <c r="AE27" s="39"/>
+      <c r="AF27" s="39"/>
+      <c r="AG27" s="39"/>
+      <c r="AH27" s="39"/>
+      <c r="AI27" s="39"/>
+      <c r="AJ27" s="40"/>
       <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="7:37" x14ac:dyDescent="0.25">
@@ -3872,43 +3937,43 @@
       <c r="AK28" s="10"/>
     </row>
     <row r="29" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="42" t="s">
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="38"/>
-      <c r="U29" s="42" t="s">
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="37"/>
-      <c r="AB29" s="38"/>
-      <c r="AC29" s="41" t="s">
+      <c r="V29" s="39"/>
+      <c r="W29" s="39"/>
+      <c r="X29" s="39"/>
+      <c r="Y29" s="39"/>
+      <c r="Z29" s="39"/>
+      <c r="AA29" s="39"/>
+      <c r="AB29" s="40"/>
+      <c r="AC29" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="AD29" s="37"/>
-      <c r="AE29" s="37"/>
-      <c r="AF29" s="37"/>
-      <c r="AG29" s="37"/>
-      <c r="AH29" s="37"/>
-      <c r="AI29" s="37"/>
-      <c r="AJ29" s="38"/>
+      <c r="AD29" s="39"/>
+      <c r="AE29" s="39"/>
+      <c r="AF29" s="39"/>
+      <c r="AG29" s="39"/>
+      <c r="AH29" s="39"/>
+      <c r="AI29" s="39"/>
+      <c r="AJ29" s="40"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -3918,41 +3983,40 @@
     <sortCondition ref="K3:K15"/>
     <sortCondition ref="L3:L15"/>
   </sortState>
-  <mergeCells count="71">
+  <mergeCells count="72">
+    <mergeCell ref="AT4:BY4"/>
     <mergeCell ref="BR11:BY11"/>
     <mergeCell ref="BZ11:CG11"/>
     <mergeCell ref="CH11:CO11"/>
     <mergeCell ref="CP11:CW11"/>
     <mergeCell ref="CP12:CW12"/>
+    <mergeCell ref="U13:AB13"/>
+    <mergeCell ref="U14:AB14"/>
+    <mergeCell ref="U15:AB15"/>
+    <mergeCell ref="CH13:CO13"/>
+    <mergeCell ref="BR12:BY12"/>
+    <mergeCell ref="BZ12:CG12"/>
+    <mergeCell ref="CH12:CO12"/>
+    <mergeCell ref="AL12:AS12"/>
     <mergeCell ref="AT12:BA12"/>
     <mergeCell ref="BJ12:BQ12"/>
     <mergeCell ref="BB12:BI12"/>
     <mergeCell ref="BR13:BY13"/>
     <mergeCell ref="BZ13:CG13"/>
-    <mergeCell ref="CH13:CO13"/>
-    <mergeCell ref="BR12:BY12"/>
-    <mergeCell ref="BZ12:CG12"/>
-    <mergeCell ref="CH12:CO12"/>
-    <mergeCell ref="AL12:AS12"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="AL6:AS6"/>
+    <mergeCell ref="AL8:BA8"/>
+    <mergeCell ref="AL11:BQ11"/>
+    <mergeCell ref="M16:T16"/>
     <mergeCell ref="M8:T8"/>
     <mergeCell ref="M15:T15"/>
-    <mergeCell ref="AC4:AJ4"/>
     <mergeCell ref="AC7:AJ7"/>
     <mergeCell ref="AC8:AJ8"/>
-    <mergeCell ref="U10:AB10"/>
     <mergeCell ref="U11:AB11"/>
     <mergeCell ref="M13:T13"/>
     <mergeCell ref="M12:T12"/>
     <mergeCell ref="M11:T11"/>
     <mergeCell ref="U12:AB12"/>
-    <mergeCell ref="U13:AB13"/>
-    <mergeCell ref="U14:AB14"/>
-    <mergeCell ref="U15:AB15"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="AL6:AS6"/>
-    <mergeCell ref="AL8:BA8"/>
-    <mergeCell ref="AL11:BQ11"/>
-    <mergeCell ref="M16:T16"/>
     <mergeCell ref="I16:L16"/>
     <mergeCell ref="AL1:CW1"/>
     <mergeCell ref="A1:F1"/>
@@ -3968,12 +4032,15 @@
     <mergeCell ref="AT15:BQ15"/>
     <mergeCell ref="U16:AB16"/>
     <mergeCell ref="AC16:AJ16"/>
+    <mergeCell ref="AC5:AJ5"/>
+    <mergeCell ref="M20:T20"/>
     <mergeCell ref="M22:T22"/>
     <mergeCell ref="M25:T25"/>
     <mergeCell ref="U25:AB25"/>
     <mergeCell ref="AC25:AJ25"/>
     <mergeCell ref="AC22:AJ22"/>
     <mergeCell ref="U22:AB22"/>
+    <mergeCell ref="BR5:BY5"/>
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="AL10:BQ10"/>
     <mergeCell ref="H20:L20"/>
@@ -3989,7 +4056,6 @@
     <mergeCell ref="AC26:AJ26"/>
     <mergeCell ref="AC20:AJ20"/>
     <mergeCell ref="U20:AB20"/>
-    <mergeCell ref="M20:T20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CAN messages update: Priorities changed
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="128">
   <si>
     <t>CAN-Messages</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Threshold, 0-Level, Sampling-Rate</t>
   </si>
   <si>
-    <t>Timestamp snychronisieren</t>
-  </si>
-  <si>
     <t>Empfänger</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>Modi: Standard, Extended, Rohdaten</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sensor</t>
-  </si>
-  <si>
     <t>Frame Format</t>
   </si>
   <si>
@@ -402,6 +396,9 @@
   </si>
   <si>
     <t>40-64</t>
+  </si>
+  <si>
+    <t>Timestamp synchronisieren</t>
   </si>
 </sst>
 </file>
@@ -507,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -689,11 +686,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -741,6 +749,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,97 +851,34 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1147,7 +1185,7 @@
   <dimension ref="A1:CX31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,117 +1203,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
+      <c r="H1" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
       <c r="AK1" s="9"/>
-      <c r="AL1" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" s="58"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="58"/>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="58"/>
-      <c r="AV1" s="58"/>
-      <c r="AW1" s="58"/>
-      <c r="AX1" s="58"/>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="58"/>
-      <c r="BA1" s="58"/>
-      <c r="BB1" s="58"/>
-      <c r="BC1" s="58"/>
-      <c r="BD1" s="58"/>
-      <c r="BE1" s="58"/>
-      <c r="BF1" s="58"/>
-      <c r="BG1" s="58"/>
-      <c r="BH1" s="58"/>
-      <c r="BI1" s="58"/>
-      <c r="BJ1" s="58"/>
-      <c r="BK1" s="58"/>
-      <c r="BL1" s="58"/>
-      <c r="BM1" s="58"/>
-      <c r="BN1" s="58"/>
-      <c r="BO1" s="58"/>
-      <c r="BP1" s="58"/>
-      <c r="BQ1" s="58"/>
-      <c r="BR1" s="58"/>
-      <c r="BS1" s="58"/>
-      <c r="BT1" s="58"/>
-      <c r="BU1" s="58"/>
-      <c r="BV1" s="58"/>
-      <c r="BW1" s="58"/>
-      <c r="BX1" s="58"/>
-      <c r="BY1" s="58"/>
-      <c r="BZ1" s="58"/>
-      <c r="CA1" s="58"/>
-      <c r="CB1" s="58"/>
-      <c r="CC1" s="58"/>
-      <c r="CD1" s="58"/>
-      <c r="CE1" s="58"/>
-      <c r="CF1" s="58"/>
-      <c r="CG1" s="58"/>
-      <c r="CH1" s="58"/>
-      <c r="CI1" s="58"/>
-      <c r="CJ1" s="58"/>
-      <c r="CK1" s="58"/>
-      <c r="CL1" s="58"/>
-      <c r="CM1" s="58"/>
-      <c r="CN1" s="58"/>
-      <c r="CO1" s="58"/>
-      <c r="CP1" s="58"/>
-      <c r="CQ1" s="58"/>
-      <c r="CR1" s="58"/>
-      <c r="CS1" s="58"/>
-      <c r="CT1" s="58"/>
-      <c r="CU1" s="58"/>
-      <c r="CV1" s="58"/>
-      <c r="CW1" s="58"/>
+      <c r="AL1" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+      <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="48"/>
+      <c r="AZ1" s="48"/>
+      <c r="BA1" s="48"/>
+      <c r="BB1" s="48"/>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="48"/>
+      <c r="BR1" s="48"/>
+      <c r="BS1" s="48"/>
+      <c r="BT1" s="48"/>
+      <c r="BU1" s="48"/>
+      <c r="BV1" s="48"/>
+      <c r="BW1" s="48"/>
+      <c r="BX1" s="48"/>
+      <c r="BY1" s="48"/>
+      <c r="BZ1" s="48"/>
+      <c r="CA1" s="48"/>
+      <c r="CB1" s="48"/>
+      <c r="CC1" s="48"/>
+      <c r="CD1" s="48"/>
+      <c r="CE1" s="48"/>
+      <c r="CF1" s="48"/>
+      <c r="CG1" s="48"/>
+      <c r="CH1" s="48"/>
+      <c r="CI1" s="48"/>
+      <c r="CJ1" s="48"/>
+      <c r="CK1" s="48"/>
+      <c r="CL1" s="48"/>
+      <c r="CM1" s="48"/>
+      <c r="CN1" s="48"/>
+      <c r="CO1" s="48"/>
+      <c r="CP1" s="48"/>
+      <c r="CQ1" s="48"/>
+      <c r="CR1" s="48"/>
+      <c r="CS1" s="48"/>
+      <c r="CT1" s="48"/>
+      <c r="CU1" s="48"/>
+      <c r="CV1" s="48"/>
+      <c r="CW1" s="48"/>
       <c r="CX1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.25">
@@ -1283,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1583,19 +1621,19 @@
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="11">
         <v>0</v>
@@ -1688,13 +1726,13 @@
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -1703,7 +1741,7 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4" s="11">
         <v>0</v>
@@ -1777,16 +1815,16 @@
         <v>1</v>
       </c>
       <c r="AK4" s="10"/>
-      <c r="AL4" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="55"/>
-      <c r="AO4" s="55"/>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="55"/>
-      <c r="AR4" s="55"/>
-      <c r="AS4" s="55"/>
+      <c r="AL4" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="41"/>
+      <c r="AR4" s="41"/>
+      <c r="AS4" s="41"/>
       <c r="AU4" s="3"/>
       <c r="BA4" s="18"/>
       <c r="BE4" s="3"/>
@@ -1805,22 +1843,22 @@
     </row>
     <row r="5" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="H5" s="11">
         <v>0</v>
@@ -1894,44 +1932,13 @@
         <v>1</v>
       </c>
       <c r="AK5" s="10"/>
-      <c r="AL5" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="61"/>
-      <c r="AP5" s="61"/>
-      <c r="AQ5" s="61"/>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="61"/>
-      <c r="AT5" s="61"/>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW5" s="62"/>
-      <c r="AX5" s="62"/>
-      <c r="AY5" s="62"/>
-      <c r="AZ5" s="62"/>
-      <c r="BA5" s="62"/>
-      <c r="BB5" s="62"/>
-      <c r="BC5" s="62"/>
-      <c r="BD5" s="62"/>
-      <c r="BE5" s="62"/>
-      <c r="BF5" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BG5" s="40"/>
-      <c r="BH5" s="40"/>
-      <c r="BI5" s="40"/>
-      <c r="BJ5" s="40"/>
-      <c r="BK5" s="40"/>
-      <c r="BL5" s="40"/>
-      <c r="BM5" s="40"/>
-      <c r="BN5" s="40"/>
-      <c r="BO5" s="40"/>
-      <c r="BP5" s="40"/>
-      <c r="BQ5" s="40"/>
+      <c r="AS5" s="18"/>
+      <c r="AU5" s="3"/>
+      <c r="BA5" s="18"/>
+      <c r="BE5" s="3"/>
+      <c r="BI5" s="18"/>
+      <c r="BO5" s="3"/>
+      <c r="BQ5" s="18"/>
       <c r="BY5" s="20"/>
       <c r="CG5" s="18"/>
       <c r="CI5" s="3"/>
@@ -1939,15 +1946,15 @@
       <c r="CS5" s="3"/>
       <c r="CW5" s="18"/>
       <c r="CX5">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1956,10 +1963,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="H6" s="11">
         <v>0</v>
@@ -1976,14 +1983,16 @@
       <c r="L6" s="12">
         <v>1</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="M6" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
       <c r="U6" s="14">
         <v>0</v>
       </c>
@@ -2008,69 +2017,39 @@
       <c r="AB6" s="14">
         <v>1</v>
       </c>
-      <c r="AC6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="15">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="15">
-        <v>1</v>
-      </c>
+      <c r="AC6" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD6" s="45"/>
+      <c r="AE6" s="45"/>
+      <c r="AF6" s="45"/>
+      <c r="AG6" s="45"/>
+      <c r="AH6" s="45"/>
+      <c r="AI6" s="45"/>
+      <c r="AJ6" s="46"/>
       <c r="AK6" s="10"/>
-      <c r="AL6" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM6" s="61"/>
-      <c r="AN6" s="61"/>
-      <c r="AO6" s="61"/>
-      <c r="AP6" s="61"/>
-      <c r="AQ6" s="61"/>
-      <c r="AR6" s="61"/>
-      <c r="AS6" s="61"/>
-      <c r="AT6" s="61"/>
-      <c r="AU6" s="61"/>
-      <c r="AV6" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW6" s="62"/>
-      <c r="AX6" s="62"/>
-      <c r="AY6" s="62"/>
-      <c r="AZ6" s="62"/>
-      <c r="BA6" s="62"/>
-      <c r="BB6" s="62"/>
-      <c r="BC6" s="62"/>
-      <c r="BD6" s="62"/>
-      <c r="BE6" s="62"/>
-      <c r="BF6" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BG6" s="40"/>
-      <c r="BH6" s="40"/>
-      <c r="BI6" s="40"/>
-      <c r="BJ6" s="40"/>
-      <c r="BK6" s="40"/>
-      <c r="BL6" s="40"/>
-      <c r="BM6" s="40"/>
-      <c r="BN6" s="40"/>
-      <c r="BO6" s="40"/>
-      <c r="BP6" s="40"/>
-      <c r="BQ6" s="40"/>
+      <c r="AL6" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM6" s="41"/>
+      <c r="AN6" s="41"/>
+      <c r="AO6" s="41"/>
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="41"/>
+      <c r="AR6" s="41"/>
+      <c r="AS6" s="41"/>
+      <c r="AT6" s="41"/>
+      <c r="AU6" s="41"/>
+      <c r="AV6" s="41"/>
+      <c r="AW6" s="41"/>
+      <c r="AX6" s="41"/>
+      <c r="AY6" s="41"/>
+      <c r="AZ6" s="41"/>
+      <c r="BA6" s="41"/>
+      <c r="BE6" s="3"/>
+      <c r="BI6" s="18"/>
+      <c r="BO6" s="3"/>
+      <c r="BQ6" s="18"/>
       <c r="BY6" s="20"/>
       <c r="CG6" s="18"/>
       <c r="CI6" s="3"/>
@@ -2078,27 +2057,27 @@
       <c r="CS6" s="3"/>
       <c r="CW6" s="18"/>
       <c r="CX6">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="H7" s="11">
         <v>0</v>
@@ -2147,27 +2126,27 @@
       <c r="AB7" s="14">
         <v>1</v>
       </c>
-      <c r="AC7" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD7" s="46"/>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46"/>
-      <c r="AG7" s="46"/>
-      <c r="AH7" s="46"/>
-      <c r="AI7" s="46"/>
-      <c r="AJ7" s="47"/>
+      <c r="AC7" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD7" s="45"/>
+      <c r="AE7" s="45"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="45"/>
+      <c r="AH7" s="45"/>
+      <c r="AI7" s="45"/>
+      <c r="AJ7" s="46"/>
       <c r="AK7" s="10"/>
-      <c r="AL7" s="54" t="s">
+      <c r="AL7" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="AM7" s="55"/>
-      <c r="AN7" s="55"/>
-      <c r="AO7" s="55"/>
-      <c r="AP7" s="55"/>
-      <c r="AQ7" s="55"/>
-      <c r="AR7" s="55"/>
-      <c r="AS7" s="55"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="41"/>
+      <c r="AQ7" s="41"/>
+      <c r="AR7" s="41"/>
+      <c r="AS7" s="41"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="18"/>
       <c r="BE7" s="3"/>
@@ -2186,10 +2165,10 @@
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -2198,10 +2177,10 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H8" s="11">
         <v>0</v>
@@ -2250,33 +2229,69 @@
       <c r="AB8" s="14">
         <v>1</v>
       </c>
-      <c r="AC8" s="45" t="s">
+      <c r="AC8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM8" s="51"/>
+      <c r="AN8" s="51"/>
+      <c r="AO8" s="51"/>
+      <c r="AP8" s="51"/>
+      <c r="AQ8" s="51"/>
+      <c r="AR8" s="51"/>
+      <c r="AS8" s="51"/>
+      <c r="AT8" s="51"/>
+      <c r="AU8" s="51"/>
+      <c r="AV8" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46"/>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="47"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM8" s="55"/>
-      <c r="AN8" s="55"/>
-      <c r="AO8" s="55"/>
-      <c r="AP8" s="55"/>
-      <c r="AQ8" s="55"/>
-      <c r="AR8" s="55"/>
-      <c r="AS8" s="55"/>
-      <c r="AU8" s="3"/>
-      <c r="BA8" s="18"/>
-      <c r="BE8" s="3"/>
-      <c r="BI8" s="18"/>
-      <c r="BO8" s="3"/>
-      <c r="BQ8" s="18"/>
+      <c r="AW8" s="52"/>
+      <c r="AX8" s="52"/>
+      <c r="AY8" s="52"/>
+      <c r="AZ8" s="52"/>
+      <c r="BA8" s="52"/>
+      <c r="BB8" s="52"/>
+      <c r="BC8" s="52"/>
+      <c r="BD8" s="52"/>
+      <c r="BE8" s="52"/>
+      <c r="BF8" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG8" s="53"/>
+      <c r="BH8" s="53"/>
+      <c r="BI8" s="53"/>
+      <c r="BJ8" s="53"/>
+      <c r="BK8" s="53"/>
+      <c r="BL8" s="53"/>
+      <c r="BM8" s="53"/>
+      <c r="BN8" s="53"/>
+      <c r="BO8" s="53"/>
+      <c r="BP8" s="53"/>
+      <c r="BQ8" s="53"/>
       <c r="BY8" s="20"/>
       <c r="CG8" s="18"/>
       <c r="CI8" s="3"/>
@@ -2284,27 +2299,27 @@
       <c r="CS8" s="3"/>
       <c r="CW8" s="18"/>
       <c r="CX8">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="H9" s="11">
         <v>0</v>
@@ -2353,33 +2368,69 @@
       <c r="AB9" s="14">
         <v>1</v>
       </c>
-      <c r="AC9" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD9" s="46"/>
-      <c r="AE9" s="46"/>
-      <c r="AF9" s="46"/>
-      <c r="AG9" s="46"/>
-      <c r="AH9" s="46"/>
-      <c r="AI9" s="46"/>
-      <c r="AJ9" s="47"/>
+      <c r="AC9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="15">
+        <v>1</v>
+      </c>
       <c r="AK9" s="10"/>
-      <c r="AL9" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="55"/>
-      <c r="AR9" s="55"/>
-      <c r="AS9" s="55"/>
-      <c r="AU9" s="3"/>
-      <c r="BA9" s="18"/>
-      <c r="BE9" s="3"/>
-      <c r="BI9" s="18"/>
-      <c r="BO9" s="3"/>
-      <c r="BQ9" s="18"/>
+      <c r="AL9" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM9" s="51"/>
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="51"/>
+      <c r="AP9" s="51"/>
+      <c r="AQ9" s="51"/>
+      <c r="AR9" s="51"/>
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="51"/>
+      <c r="AU9" s="51"/>
+      <c r="AV9" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW9" s="52"/>
+      <c r="AX9" s="52"/>
+      <c r="AY9" s="52"/>
+      <c r="AZ9" s="52"/>
+      <c r="BA9" s="52"/>
+      <c r="BB9" s="52"/>
+      <c r="BC9" s="52"/>
+      <c r="BD9" s="52"/>
+      <c r="BE9" s="52"/>
+      <c r="BF9" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG9" s="53"/>
+      <c r="BH9" s="53"/>
+      <c r="BI9" s="53"/>
+      <c r="BJ9" s="53"/>
+      <c r="BK9" s="53"/>
+      <c r="BL9" s="53"/>
+      <c r="BM9" s="53"/>
+      <c r="BN9" s="53"/>
+      <c r="BO9" s="53"/>
+      <c r="BP9" s="53"/>
+      <c r="BQ9" s="53"/>
       <c r="BY9" s="20"/>
       <c r="CG9" s="18"/>
       <c r="CI9" s="3"/>
@@ -2387,27 +2438,27 @@
       <c r="CS9" s="3"/>
       <c r="CW9" s="18"/>
       <c r="CX9">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="H10" s="11">
         <v>0</v>
@@ -2424,16 +2475,14 @@
       <c r="L10" s="12">
         <v>1</v>
       </c>
-      <c r="M10" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
       <c r="U10" s="14">
         <v>0</v>
       </c>
@@ -2458,35 +2507,29 @@
       <c r="AB10" s="14">
         <v>1</v>
       </c>
-      <c r="AC10" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="46"/>
-      <c r="AH10" s="46"/>
-      <c r="AI10" s="46"/>
-      <c r="AJ10" s="47"/>
+      <c r="AC10" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD10" s="45"/>
+      <c r="AE10" s="45"/>
+      <c r="AF10" s="45"/>
+      <c r="AG10" s="45"/>
+      <c r="AH10" s="45"/>
+      <c r="AI10" s="45"/>
+      <c r="AJ10" s="46"/>
       <c r="AK10" s="10"/>
-      <c r="AL10" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM10" s="55"/>
-      <c r="AN10" s="55"/>
-      <c r="AO10" s="55"/>
-      <c r="AP10" s="55"/>
-      <c r="AQ10" s="55"/>
-      <c r="AR10" s="55"/>
-      <c r="AS10" s="55"/>
-      <c r="AT10" s="55"/>
-      <c r="AU10" s="55"/>
-      <c r="AV10" s="55"/>
-      <c r="AW10" s="55"/>
-      <c r="AX10" s="55"/>
-      <c r="AY10" s="55"/>
-      <c r="AZ10" s="55"/>
-      <c r="BA10" s="55"/>
+      <c r="AL10" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="41"/>
+      <c r="AQ10" s="41"/>
+      <c r="AR10" s="41"/>
+      <c r="AS10" s="41"/>
+      <c r="AU10" s="3"/>
+      <c r="BA10" s="18"/>
       <c r="BE10" s="3"/>
       <c r="BI10" s="18"/>
       <c r="BO10" s="3"/>
@@ -2498,27 +2541,27 @@
       <c r="CS10" s="3"/>
       <c r="CW10" s="18"/>
       <c r="CX10">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="H11" s="11">
         <v>0</v>
@@ -2567,32 +2610,27 @@
       <c r="AB11" s="14">
         <v>1</v>
       </c>
-      <c r="AC11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="15">
-        <v>1</v>
-      </c>
+      <c r="AC11" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD11" s="45"/>
+      <c r="AE11" s="45"/>
+      <c r="AF11" s="45"/>
+      <c r="AG11" s="45"/>
+      <c r="AH11" s="45"/>
+      <c r="AI11" s="45"/>
+      <c r="AJ11" s="46"/>
       <c r="AK11" s="10"/>
-      <c r="AS11" s="18"/>
+      <c r="AL11" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM11" s="41"/>
+      <c r="AN11" s="41"/>
+      <c r="AO11" s="41"/>
+      <c r="AP11" s="41"/>
+      <c r="AQ11" s="41"/>
+      <c r="AR11" s="41"/>
+      <c r="AS11" s="41"/>
       <c r="AU11" s="3"/>
       <c r="BA11" s="18"/>
       <c r="BE11" s="3"/>
@@ -2606,18 +2644,18 @@
       <c r="CS11" s="3"/>
       <c r="CW11" s="18"/>
       <c r="CX11">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -2626,7 +2664,7 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H12" s="11">
         <v>1</v>
@@ -2700,40 +2738,40 @@
         <v>1</v>
       </c>
       <c r="AK12" s="10"/>
-      <c r="AL12" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM12" s="55"/>
-      <c r="AN12" s="55"/>
-      <c r="AO12" s="55"/>
-      <c r="AP12" s="55"/>
-      <c r="AQ12" s="55"/>
-      <c r="AR12" s="55"/>
-      <c r="AS12" s="55"/>
-      <c r="AT12" s="55"/>
-      <c r="AU12" s="55"/>
-      <c r="AV12" s="55"/>
-      <c r="AW12" s="55"/>
-      <c r="AX12" s="55"/>
-      <c r="AY12" s="55"/>
-      <c r="AZ12" s="55"/>
-      <c r="BA12" s="55"/>
-      <c r="BB12" s="55"/>
-      <c r="BC12" s="55"/>
-      <c r="BD12" s="55"/>
-      <c r="BE12" s="55"/>
-      <c r="BF12" s="55"/>
-      <c r="BG12" s="55"/>
-      <c r="BH12" s="55"/>
-      <c r="BI12" s="55"/>
-      <c r="BJ12" s="55"/>
-      <c r="BK12" s="55"/>
-      <c r="BL12" s="55"/>
-      <c r="BM12" s="55"/>
-      <c r="BN12" s="55"/>
-      <c r="BO12" s="55"/>
-      <c r="BP12" s="55"/>
-      <c r="BQ12" s="55"/>
+      <c r="AL12" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM12" s="41"/>
+      <c r="AN12" s="41"/>
+      <c r="AO12" s="41"/>
+      <c r="AP12" s="41"/>
+      <c r="AQ12" s="41"/>
+      <c r="AR12" s="41"/>
+      <c r="AS12" s="41"/>
+      <c r="AT12" s="41"/>
+      <c r="AU12" s="41"/>
+      <c r="AV12" s="41"/>
+      <c r="AW12" s="41"/>
+      <c r="AX12" s="41"/>
+      <c r="AY12" s="41"/>
+      <c r="AZ12" s="41"/>
+      <c r="BA12" s="41"/>
+      <c r="BB12" s="41"/>
+      <c r="BC12" s="41"/>
+      <c r="BD12" s="41"/>
+      <c r="BE12" s="41"/>
+      <c r="BF12" s="41"/>
+      <c r="BG12" s="41"/>
+      <c r="BH12" s="41"/>
+      <c r="BI12" s="41"/>
+      <c r="BJ12" s="41"/>
+      <c r="BK12" s="41"/>
+      <c r="BL12" s="41"/>
+      <c r="BM12" s="41"/>
+      <c r="BN12" s="41"/>
+      <c r="BO12" s="41"/>
+      <c r="BP12" s="41"/>
+      <c r="BQ12" s="41"/>
       <c r="BY12" s="20"/>
       <c r="CG12" s="18"/>
       <c r="CI12" s="3"/>
@@ -2746,25 +2784,22 @@
     </row>
     <row r="13" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="H13" s="11">
         <v>1</v>
@@ -2781,26 +2816,26 @@
       <c r="L13" s="12">
         <v>1</v>
       </c>
-      <c r="M13" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="V13" s="49"/>
-      <c r="W13" s="49"/>
-      <c r="X13" s="49"/>
-      <c r="Y13" s="49"/>
-      <c r="Z13" s="49"/>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="50"/>
+      <c r="M13" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="64"/>
       <c r="AC13" s="15">
         <v>0</v>
       </c>
@@ -2826,653 +2861,656 @@
         <v>1</v>
       </c>
       <c r="AK13" s="10"/>
-      <c r="AL13" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM13" s="55"/>
-      <c r="AN13" s="55"/>
-      <c r="AO13" s="55"/>
-      <c r="AP13" s="55"/>
-      <c r="AQ13" s="55"/>
-      <c r="AR13" s="55"/>
-      <c r="AS13" s="55"/>
-      <c r="AT13" s="55"/>
-      <c r="AU13" s="55"/>
-      <c r="AV13" s="55"/>
-      <c r="AW13" s="55"/>
-      <c r="AX13" s="55"/>
-      <c r="AY13" s="55"/>
-      <c r="AZ13" s="55"/>
-      <c r="BA13" s="55"/>
-      <c r="BB13" s="55"/>
-      <c r="BC13" s="55"/>
-      <c r="BD13" s="55"/>
-      <c r="BE13" s="55"/>
-      <c r="BF13" s="55"/>
-      <c r="BG13" s="55"/>
-      <c r="BH13" s="55"/>
-      <c r="BI13" s="55"/>
-      <c r="BJ13" s="55"/>
-      <c r="BK13" s="55"/>
-      <c r="BL13" s="55"/>
-      <c r="BM13" s="55"/>
-      <c r="BN13" s="55"/>
-      <c r="BO13" s="55"/>
-      <c r="BP13" s="55"/>
-      <c r="BQ13" s="55"/>
-      <c r="BR13" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="BS13" s="37"/>
-      <c r="BT13" s="37"/>
-      <c r="BU13" s="37"/>
-      <c r="BV13" s="37"/>
-      <c r="BW13" s="37"/>
-      <c r="BX13" s="37"/>
-      <c r="BY13" s="37"/>
-      <c r="BZ13" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="CA13" s="37"/>
-      <c r="CB13" s="37"/>
-      <c r="CC13" s="37"/>
-      <c r="CD13" s="37"/>
-      <c r="CE13" s="37"/>
-      <c r="CF13" s="37"/>
-      <c r="CG13" s="37"/>
-      <c r="CH13" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="CI13" s="37"/>
-      <c r="CJ13" s="37"/>
-      <c r="CK13" s="37"/>
-      <c r="CL13" s="37"/>
-      <c r="CM13" s="37"/>
-      <c r="CN13" s="37"/>
-      <c r="CO13" s="37"/>
-      <c r="CP13" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="CQ13" s="37"/>
-      <c r="CR13" s="37"/>
-      <c r="CS13" s="37"/>
-      <c r="CT13" s="37"/>
-      <c r="CU13" s="37"/>
-      <c r="CV13" s="37"/>
-      <c r="CW13" s="37"/>
-      <c r="CX13" s="36" t="s">
-        <v>128</v>
+      <c r="AL13" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM13" s="41"/>
+      <c r="AN13" s="41"/>
+      <c r="AO13" s="41"/>
+      <c r="AP13" s="41"/>
+      <c r="AQ13" s="41"/>
+      <c r="AR13" s="41"/>
+      <c r="AS13" s="41"/>
+      <c r="AT13" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU13" s="53"/>
+      <c r="AV13" s="53"/>
+      <c r="AW13" s="53"/>
+      <c r="AX13" s="53"/>
+      <c r="AY13" s="53"/>
+      <c r="AZ13" s="53"/>
+      <c r="BA13" s="53"/>
+      <c r="BB13" s="53"/>
+      <c r="BC13" s="53"/>
+      <c r="BD13" s="53"/>
+      <c r="BE13" s="53"/>
+      <c r="BF13" s="53"/>
+      <c r="BG13" s="53"/>
+      <c r="BH13" s="53"/>
+      <c r="BI13" s="53"/>
+      <c r="BJ13" s="53"/>
+      <c r="BK13" s="53"/>
+      <c r="BL13" s="53"/>
+      <c r="BM13" s="53"/>
+      <c r="BN13" s="53"/>
+      <c r="BO13" s="53"/>
+      <c r="BP13" s="53"/>
+      <c r="BQ13" s="53"/>
+      <c r="BY13" s="20"/>
+      <c r="CG13" s="18"/>
+      <c r="CI13" s="3"/>
+      <c r="CO13" s="18"/>
+      <c r="CS13" s="3"/>
+      <c r="CW13" s="18"/>
+      <c r="CX13" s="21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
       </c>
       <c r="G14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="61"/>
+      <c r="U14" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="V14" s="63"/>
+      <c r="W14" s="63"/>
+      <c r="X14" s="63"/>
+      <c r="Y14" s="63"/>
+      <c r="Z14" s="63"/>
+      <c r="AA14" s="63"/>
+      <c r="AB14" s="64"/>
+      <c r="AC14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="15">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="10"/>
+      <c r="AL14" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM14" s="41"/>
+      <c r="AN14" s="41"/>
+      <c r="AO14" s="41"/>
+      <c r="AP14" s="41"/>
+      <c r="AQ14" s="41"/>
+      <c r="AR14" s="41"/>
+      <c r="AS14" s="41"/>
+      <c r="AT14" s="41"/>
+      <c r="AU14" s="41"/>
+      <c r="AV14" s="41"/>
+      <c r="AW14" s="41"/>
+      <c r="AX14" s="41"/>
+      <c r="AY14" s="41"/>
+      <c r="AZ14" s="41"/>
+      <c r="BA14" s="41"/>
+      <c r="BB14" s="41"/>
+      <c r="BC14" s="41"/>
+      <c r="BD14" s="41"/>
+      <c r="BE14" s="41"/>
+      <c r="BF14" s="41"/>
+      <c r="BG14" s="41"/>
+      <c r="BH14" s="41"/>
+      <c r="BI14" s="41"/>
+      <c r="BJ14" s="41"/>
+      <c r="BK14" s="41"/>
+      <c r="BL14" s="41"/>
+      <c r="BM14" s="41"/>
+      <c r="BN14" s="41"/>
+      <c r="BO14" s="41"/>
+      <c r="BP14" s="41"/>
+      <c r="BQ14" s="41"/>
+      <c r="BR14" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="BS14" s="68"/>
+      <c r="BT14" s="68"/>
+      <c r="BU14" s="68"/>
+      <c r="BV14" s="68"/>
+      <c r="BW14" s="68"/>
+      <c r="BX14" s="68"/>
+      <c r="BY14" s="68"/>
+      <c r="BZ14" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="H14" s="11">
-        <v>1</v>
-      </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>1</v>
-      </c>
-      <c r="L14" s="12">
-        <v>0</v>
-      </c>
-      <c r="M14" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="49"/>
-      <c r="Z14" s="49"/>
-      <c r="AA14" s="49"/>
-      <c r="AB14" s="50"/>
-      <c r="AC14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="15">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="15">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM14" s="37"/>
-      <c r="AN14" s="37"/>
-      <c r="AO14" s="37"/>
-      <c r="AP14" s="37"/>
-      <c r="AQ14" s="37"/>
-      <c r="AR14" s="37"/>
-      <c r="AS14" s="37"/>
-      <c r="AT14" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU14" s="37"/>
-      <c r="AV14" s="37"/>
-      <c r="AW14" s="37"/>
-      <c r="AX14" s="37"/>
-      <c r="AY14" s="37"/>
-      <c r="AZ14" s="37"/>
-      <c r="BA14" s="37"/>
-      <c r="BB14" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="BC14" s="37"/>
-      <c r="BD14" s="37"/>
-      <c r="BE14" s="37"/>
-      <c r="BF14" s="37"/>
-      <c r="BG14" s="37"/>
-      <c r="BH14" s="37"/>
-      <c r="BI14" s="37"/>
-      <c r="BJ14" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="BK14" s="37"/>
-      <c r="BL14" s="37"/>
-      <c r="BM14" s="37"/>
-      <c r="BN14" s="37"/>
-      <c r="BO14" s="37"/>
-      <c r="BP14" s="37"/>
-      <c r="BQ14" s="37"/>
-      <c r="BR14" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="BS14" s="37"/>
-      <c r="BT14" s="37"/>
-      <c r="BU14" s="37"/>
-      <c r="BV14" s="37"/>
-      <c r="BW14" s="37"/>
-      <c r="BX14" s="37"/>
-      <c r="BY14" s="37"/>
-      <c r="BZ14" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="CA14" s="37"/>
-      <c r="CB14" s="37"/>
-      <c r="CC14" s="37"/>
-      <c r="CD14" s="37"/>
-      <c r="CE14" s="37"/>
-      <c r="CF14" s="37"/>
-      <c r="CG14" s="37"/>
-      <c r="CH14" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="CI14" s="37"/>
-      <c r="CJ14" s="37"/>
-      <c r="CK14" s="37"/>
-      <c r="CL14" s="37"/>
-      <c r="CM14" s="37"/>
-      <c r="CN14" s="37"/>
-      <c r="CO14" s="37"/>
-      <c r="CP14" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="CQ14" s="37"/>
-      <c r="CR14" s="37"/>
-      <c r="CS14" s="37"/>
-      <c r="CT14" s="37"/>
-      <c r="CU14" s="37"/>
-      <c r="CV14" s="37"/>
-      <c r="CW14" s="37"/>
+      <c r="CA14" s="68"/>
+      <c r="CB14" s="68"/>
+      <c r="CC14" s="68"/>
+      <c r="CD14" s="68"/>
+      <c r="CE14" s="68"/>
+      <c r="CF14" s="68"/>
+      <c r="CG14" s="68"/>
+      <c r="CH14" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="CI14" s="68"/>
+      <c r="CJ14" s="68"/>
+      <c r="CK14" s="68"/>
+      <c r="CL14" s="68"/>
+      <c r="CM14" s="68"/>
+      <c r="CN14" s="68"/>
+      <c r="CO14" s="68"/>
+      <c r="CP14" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="CQ14" s="68"/>
+      <c r="CR14" s="68"/>
+      <c r="CS14" s="68"/>
+      <c r="CT14" s="68"/>
+      <c r="CU14" s="68"/>
+      <c r="CV14" s="68"/>
+      <c r="CW14" s="68"/>
       <c r="CX14" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:102" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
       <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12">
+        <v>1</v>
+      </c>
+      <c r="M15" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="V15" s="63"/>
+      <c r="W15" s="63"/>
+      <c r="X15" s="63"/>
+      <c r="Y15" s="63"/>
+      <c r="Z15" s="63"/>
+      <c r="AA15" s="63"/>
+      <c r="AB15" s="64"/>
+      <c r="AC15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="15">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="10"/>
+      <c r="AL15" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM15" s="68"/>
+      <c r="AN15" s="68"/>
+      <c r="AO15" s="68"/>
+      <c r="AP15" s="68"/>
+      <c r="AQ15" s="68"/>
+      <c r="AR15" s="68"/>
+      <c r="AS15" s="68"/>
+      <c r="AT15" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU15" s="68"/>
+      <c r="AV15" s="68"/>
+      <c r="AW15" s="68"/>
+      <c r="AX15" s="68"/>
+      <c r="AY15" s="68"/>
+      <c r="AZ15" s="68"/>
+      <c r="BA15" s="68"/>
+      <c r="BB15" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="BC15" s="68"/>
+      <c r="BD15" s="68"/>
+      <c r="BE15" s="68"/>
+      <c r="BF15" s="68"/>
+      <c r="BG15" s="68"/>
+      <c r="BH15" s="68"/>
+      <c r="BI15" s="68"/>
+      <c r="BJ15" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="BK15" s="68"/>
+      <c r="BL15" s="68"/>
+      <c r="BM15" s="68"/>
+      <c r="BN15" s="68"/>
+      <c r="BO15" s="68"/>
+      <c r="BP15" s="68"/>
+      <c r="BQ15" s="68"/>
+      <c r="BR15" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS15" s="68"/>
+      <c r="BT15" s="68"/>
+      <c r="BU15" s="68"/>
+      <c r="BV15" s="68"/>
+      <c r="BW15" s="68"/>
+      <c r="BX15" s="68"/>
+      <c r="BY15" s="68"/>
+      <c r="BZ15" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="CA15" s="68"/>
+      <c r="CB15" s="68"/>
+      <c r="CC15" s="68"/>
+      <c r="CD15" s="68"/>
+      <c r="CE15" s="68"/>
+      <c r="CF15" s="68"/>
+      <c r="CG15" s="68"/>
+      <c r="CH15" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="CI15" s="68"/>
+      <c r="CJ15" s="68"/>
+      <c r="CK15" s="68"/>
+      <c r="CL15" s="68"/>
+      <c r="CM15" s="68"/>
+      <c r="CN15" s="68"/>
+      <c r="CO15" s="68"/>
+      <c r="CP15" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="CQ15" s="68"/>
+      <c r="CR15" s="68"/>
+      <c r="CS15" s="68"/>
+      <c r="CT15" s="68"/>
+      <c r="CU15" s="68"/>
+      <c r="CV15" s="68"/>
+      <c r="CW15" s="68"/>
+      <c r="CX15" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="11">
-        <v>1</v>
-      </c>
-      <c r="I15" s="12">
-        <v>1</v>
-      </c>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <v>1</v>
-      </c>
-      <c r="L15" s="12">
-        <v>1</v>
-      </c>
-      <c r="M15" s="42" t="s">
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="63"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="15">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM16" s="41"/>
+      <c r="AN16" s="41"/>
+      <c r="AO16" s="41"/>
+      <c r="AP16" s="41"/>
+      <c r="AQ16" s="41"/>
+      <c r="AR16" s="41"/>
+      <c r="AS16" s="41"/>
+      <c r="AT16" s="41"/>
+      <c r="AU16" s="41"/>
+      <c r="AV16" s="41"/>
+      <c r="AW16" s="41"/>
+      <c r="AX16" s="41"/>
+      <c r="AY16" s="41"/>
+      <c r="AZ16" s="41"/>
+      <c r="BA16" s="41"/>
+      <c r="BB16" s="41"/>
+      <c r="BC16" s="41"/>
+      <c r="BD16" s="41"/>
+      <c r="BE16" s="41"/>
+      <c r="BF16" s="41"/>
+      <c r="BG16" s="41"/>
+      <c r="BH16" s="41"/>
+      <c r="BI16" s="41"/>
+      <c r="BJ16" s="41"/>
+      <c r="BK16" s="41"/>
+      <c r="BL16" s="41"/>
+      <c r="BM16" s="41"/>
+      <c r="BN16" s="41"/>
+      <c r="BO16" s="41"/>
+      <c r="BP16" s="41"/>
+      <c r="BQ16" s="41"/>
+      <c r="BR16" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
-      <c r="X15" s="49"/>
-      <c r="Y15" s="49"/>
-      <c r="Z15" s="49"/>
-      <c r="AA15" s="49"/>
-      <c r="AB15" s="50"/>
-      <c r="AC15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="15">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="15">
-        <v>1</v>
-      </c>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM15" s="55"/>
-      <c r="AN15" s="55"/>
-      <c r="AO15" s="55"/>
-      <c r="AP15" s="55"/>
-      <c r="AQ15" s="55"/>
-      <c r="AR15" s="55"/>
-      <c r="AS15" s="55"/>
-      <c r="AT15" s="55"/>
-      <c r="AU15" s="55"/>
-      <c r="AV15" s="55"/>
-      <c r="AW15" s="55"/>
-      <c r="AX15" s="55"/>
-      <c r="AY15" s="55"/>
-      <c r="AZ15" s="55"/>
-      <c r="BA15" s="55"/>
-      <c r="BB15" s="55"/>
-      <c r="BC15" s="55"/>
-      <c r="BD15" s="55"/>
-      <c r="BE15" s="55"/>
-      <c r="BF15" s="55"/>
-      <c r="BG15" s="55"/>
-      <c r="BH15" s="55"/>
-      <c r="BI15" s="55"/>
-      <c r="BJ15" s="55"/>
-      <c r="BK15" s="55"/>
-      <c r="BL15" s="55"/>
-      <c r="BM15" s="55"/>
-      <c r="BN15" s="55"/>
-      <c r="BO15" s="55"/>
-      <c r="BP15" s="55"/>
-      <c r="BQ15" s="55"/>
-      <c r="BR15" s="38" t="s">
+      <c r="BS16" s="69"/>
+      <c r="BT16" s="69"/>
+      <c r="BU16" s="69"/>
+      <c r="BV16" s="69"/>
+      <c r="BW16" s="69"/>
+      <c r="BX16" s="69"/>
+      <c r="BY16" s="69"/>
+      <c r="BZ16" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="CA16" s="70"/>
+      <c r="CB16" s="70"/>
+      <c r="CC16" s="70"/>
+      <c r="CD16" s="70"/>
+      <c r="CE16" s="70"/>
+      <c r="CF16" s="70"/>
+      <c r="CG16" s="70"/>
+      <c r="CH16" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="BS15" s="38"/>
-      <c r="BT15" s="38"/>
-      <c r="BU15" s="38"/>
-      <c r="BV15" s="38"/>
-      <c r="BW15" s="38"/>
-      <c r="BX15" s="38"/>
-      <c r="BY15" s="38"/>
-      <c r="BZ15" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="CA15" s="39"/>
-      <c r="CB15" s="39"/>
-      <c r="CC15" s="39"/>
-      <c r="CD15" s="39"/>
-      <c r="CE15" s="39"/>
-      <c r="CF15" s="39"/>
-      <c r="CG15" s="39"/>
-      <c r="CH15" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="CI15" s="40"/>
-      <c r="CJ15" s="40"/>
-      <c r="CK15" s="40"/>
-      <c r="CL15" s="40"/>
-      <c r="CM15" s="40"/>
-      <c r="CN15" s="40"/>
-      <c r="CO15" s="40"/>
-      <c r="CS15" s="3"/>
-      <c r="CW15" s="18"/>
-      <c r="CX15">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:102" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="23">
-        <v>1</v>
-      </c>
-      <c r="I16" s="24">
-        <v>1</v>
-      </c>
-      <c r="J16" s="24">
-        <v>1</v>
-      </c>
-      <c r="K16" s="24">
-        <v>0</v>
-      </c>
-      <c r="L16" s="24">
-        <v>0</v>
-      </c>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="V16" s="52"/>
-      <c r="W16" s="52"/>
-      <c r="X16" s="52"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="52"/>
-      <c r="AA16" s="52"/>
-      <c r="AB16" s="53"/>
-      <c r="AC16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="26">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="26">
-        <v>1</v>
-      </c>
-      <c r="AK16" s="10"/>
-      <c r="AS16" s="18"/>
-      <c r="AU16" s="3"/>
-      <c r="BA16" s="18"/>
-      <c r="BE16" s="3"/>
-      <c r="BI16" s="18"/>
-      <c r="BO16" s="3"/>
-      <c r="BQ16" s="18"/>
-      <c r="BY16" s="20"/>
-      <c r="CG16" s="18"/>
-      <c r="CI16" s="3"/>
-      <c r="CO16" s="18"/>
+      <c r="CI16" s="53"/>
+      <c r="CJ16" s="53"/>
+      <c r="CK16" s="53"/>
+      <c r="CL16" s="53"/>
+      <c r="CM16" s="53"/>
+      <c r="CN16" s="53"/>
+      <c r="CO16" s="53"/>
       <c r="CS16" s="3"/>
       <c r="CW16" s="18"/>
-    </row>
-    <row r="17" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="CX16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:101" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12">
-        <v>1</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <v>1</v>
-      </c>
-      <c r="M17" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
-      <c r="X17" s="49"/>
-      <c r="Y17" s="49"/>
-      <c r="Z17" s="49"/>
-      <c r="AA17" s="49"/>
-      <c r="AB17" s="50"/>
-      <c r="AC17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="15">
+      <c r="E17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="23">
+        <v>1</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
+      <c r="J17" s="24">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="V17" s="66"/>
+      <c r="W17" s="66"/>
+      <c r="X17" s="66"/>
+      <c r="Y17" s="66"/>
+      <c r="Z17" s="66"/>
+      <c r="AA17" s="66"/>
+      <c r="AB17" s="67"/>
+      <c r="AC17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="26">
         <v>1</v>
       </c>
       <c r="AK17" s="10"/>
-      <c r="AL17" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM17" s="55"/>
-      <c r="AN17" s="55"/>
-      <c r="AO17" s="55"/>
-      <c r="AP17" s="55"/>
-      <c r="AQ17" s="55"/>
-      <c r="AR17" s="55"/>
-      <c r="AS17" s="55"/>
-      <c r="AT17" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU17" s="40"/>
-      <c r="AV17" s="40"/>
-      <c r="AW17" s="40"/>
-      <c r="AX17" s="40"/>
-      <c r="AY17" s="40"/>
-      <c r="AZ17" s="40"/>
-      <c r="BA17" s="40"/>
-      <c r="BB17" s="40"/>
-      <c r="BC17" s="40"/>
-      <c r="BD17" s="40"/>
-      <c r="BE17" s="40"/>
-      <c r="BF17" s="40"/>
-      <c r="BG17" s="40"/>
-      <c r="BH17" s="40"/>
-      <c r="BI17" s="40"/>
-      <c r="BJ17" s="40"/>
-      <c r="BK17" s="40"/>
-      <c r="BL17" s="40"/>
-      <c r="BM17" s="40"/>
-      <c r="BN17" s="40"/>
-      <c r="BO17" s="40"/>
-      <c r="BP17" s="40"/>
-      <c r="BQ17" s="40"/>
+      <c r="AS17" s="18"/>
+      <c r="AU17" s="3"/>
+      <c r="BA17" s="18"/>
+      <c r="BE17" s="3"/>
+      <c r="BI17" s="18"/>
+      <c r="BO17" s="3"/>
+      <c r="BQ17" s="18"/>
       <c r="BY17" s="20"/>
       <c r="CG17" s="18"/>
       <c r="CI17" s="3"/>
       <c r="CO17" s="18"/>
       <c r="CS17" s="3"/>
       <c r="CW17" s="18"/>
-      <c r="CX17" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:102" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="H18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="N18" s="56"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="63" t="s">
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="54"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="V18" s="63"/>
-      <c r="W18" s="63"/>
-      <c r="X18" s="63"/>
-      <c r="Y18" s="63"/>
-      <c r="Z18" s="63"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD18" s="64"/>
-      <c r="AE18" s="64"/>
-      <c r="AF18" s="64"/>
-      <c r="AG18" s="64"/>
-      <c r="AH18" s="64"/>
-      <c r="AI18" s="64"/>
-      <c r="AJ18" s="65"/>
+      <c r="AD18" s="55"/>
+      <c r="AE18" s="55"/>
+      <c r="AF18" s="55"/>
+      <c r="AG18" s="55"/>
+      <c r="AH18" s="55"/>
+      <c r="AI18" s="55"/>
+      <c r="AJ18" s="56"/>
       <c r="AS18" s="18"/>
       <c r="AU18" s="3"/>
       <c r="BA18" s="18"/>
@@ -3487,14 +3525,14 @@
       <c r="CS18" s="3"/>
       <c r="CW18" s="18"/>
     </row>
-    <row r="20" spans="1:102" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:102" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H21" s="28">
         <v>1</v>
@@ -3585,180 +3623,180 @@
       </c>
       <c r="AK21" s="10"/>
     </row>
-    <row r="22" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H22" s="67">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="H22" s="38">
         <v>18</v>
       </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="N22" s="67"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="68"/>
-      <c r="U22" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="V22" s="67"/>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="67"/>
-      <c r="AB22" s="68"/>
-      <c r="AC22" s="69" t="s">
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="77"/>
+      <c r="U22" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="77"/>
+      <c r="AC22" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="38"/>
+      <c r="AG22" s="38"/>
+      <c r="AH22" s="38"/>
+      <c r="AI22" s="38"/>
+      <c r="AJ22" s="39"/>
+      <c r="AK22" s="10"/>
+    </row>
+    <row r="23" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="31">
+        <v>1</v>
+      </c>
+      <c r="I23" s="31">
+        <v>1</v>
+      </c>
+      <c r="J23" s="31">
+        <v>0</v>
+      </c>
+      <c r="K23" s="31">
+        <v>0</v>
+      </c>
+      <c r="L23" s="32">
+        <v>0</v>
+      </c>
+      <c r="M23" s="30">
+        <v>0</v>
+      </c>
+      <c r="N23" s="31">
+        <v>0</v>
+      </c>
+      <c r="O23" s="31">
+        <v>0</v>
+      </c>
+      <c r="P23" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="31">
+        <v>0</v>
+      </c>
+      <c r="R23" s="31">
+        <v>0</v>
+      </c>
+      <c r="S23" s="31">
+        <v>0</v>
+      </c>
+      <c r="T23" s="32">
+        <v>0</v>
+      </c>
+      <c r="U23" s="30">
+        <v>0</v>
+      </c>
+      <c r="V23" s="31">
+        <v>0</v>
+      </c>
+      <c r="W23" s="31">
+        <v>0</v>
+      </c>
+      <c r="X23" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="32">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="10"/>
+    </row>
+    <row r="24" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="H24" s="38">
+        <v>18</v>
+      </c>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="77"/>
+      <c r="U24" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="37"/>
+      <c r="AA24" s="37"/>
+      <c r="AB24" s="77"/>
+      <c r="AC24" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="AD22" s="67"/>
-      <c r="AE22" s="67"/>
-      <c r="AF22" s="67"/>
-      <c r="AG22" s="67"/>
-      <c r="AH22" s="67"/>
-      <c r="AI22" s="67"/>
-      <c r="AJ22" s="68"/>
-      <c r="AK22" s="10"/>
-    </row>
-    <row r="23" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" s="31">
-        <v>1</v>
-      </c>
-      <c r="I23" s="31">
-        <v>1</v>
-      </c>
-      <c r="J23" s="31">
-        <v>0</v>
-      </c>
-      <c r="K23" s="31">
-        <v>0</v>
-      </c>
-      <c r="L23" s="32">
-        <v>0</v>
-      </c>
-      <c r="M23" s="30">
-        <v>0</v>
-      </c>
-      <c r="N23" s="31">
-        <v>0</v>
-      </c>
-      <c r="O23" s="31">
-        <v>0</v>
-      </c>
-      <c r="P23" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="31">
-        <v>0</v>
-      </c>
-      <c r="R23" s="31">
-        <v>0</v>
-      </c>
-      <c r="S23" s="31">
-        <v>0</v>
-      </c>
-      <c r="T23" s="32">
-        <v>0</v>
-      </c>
-      <c r="U23" s="30">
-        <v>0</v>
-      </c>
-      <c r="V23" s="31">
-        <v>0</v>
-      </c>
-      <c r="W23" s="31">
-        <v>0</v>
-      </c>
-      <c r="X23" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="32">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="30">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AF23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="32">
-        <v>1</v>
-      </c>
-      <c r="AK23" s="10"/>
-    </row>
-    <row r="24" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H24" s="67">
-        <v>18</v>
-      </c>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="N24" s="67"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="68"/>
-      <c r="U24" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="V24" s="67"/>
-      <c r="W24" s="67"/>
-      <c r="X24" s="67"/>
-      <c r="Y24" s="67"/>
-      <c r="Z24" s="67"/>
-      <c r="AA24" s="67"/>
-      <c r="AB24" s="68"/>
-      <c r="AC24" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD24" s="67"/>
-      <c r="AE24" s="67"/>
-      <c r="AF24" s="67"/>
-      <c r="AG24" s="67"/>
-      <c r="AH24" s="67"/>
-      <c r="AI24" s="67"/>
-      <c r="AJ24" s="68"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="77"/>
       <c r="AK24" s="10"/>
     </row>
-    <row r="25" spans="1:102" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:101" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -3790,9 +3828,9 @@
       <c r="AJ25" s="32"/>
       <c r="AK25" s="10"/>
     </row>
-    <row r="26" spans="1:102" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H26" s="31">
         <v>1</v>
@@ -3883,296 +3921,296 @@
       </c>
       <c r="AK26" s="10"/>
     </row>
-    <row r="27" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H27" s="67">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="H27" s="38">
         <v>18</v>
       </c>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="N27" s="67"/>
-      <c r="O27" s="67"/>
-      <c r="P27" s="67"/>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="67"/>
-      <c r="S27" s="67"/>
-      <c r="T27" s="68"/>
-      <c r="U27" s="69" t="s">
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="77"/>
+      <c r="U27" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD27" s="79"/>
+      <c r="AE27" s="79"/>
+      <c r="AF27" s="79"/>
+      <c r="AG27" s="79"/>
+      <c r="AH27" s="79"/>
+      <c r="AI27" s="79"/>
+      <c r="AJ27" s="80"/>
+      <c r="AK27" s="10"/>
+    </row>
+    <row r="28" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="31">
+        <v>0</v>
+      </c>
+      <c r="I28" s="31">
+        <v>0</v>
+      </c>
+      <c r="J28" s="31">
+        <v>0</v>
+      </c>
+      <c r="K28" s="31">
+        <v>0</v>
+      </c>
+      <c r="L28" s="32">
+        <v>0</v>
+      </c>
+      <c r="M28" s="30">
+        <v>0</v>
+      </c>
+      <c r="N28" s="31">
+        <v>0</v>
+      </c>
+      <c r="O28" s="31">
+        <v>0</v>
+      </c>
+      <c r="P28" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="31">
+        <v>0</v>
+      </c>
+      <c r="R28" s="31">
+        <v>0</v>
+      </c>
+      <c r="S28" s="31">
+        <v>0</v>
+      </c>
+      <c r="T28" s="32">
+        <v>0</v>
+      </c>
+      <c r="U28" s="30">
+        <v>0</v>
+      </c>
+      <c r="V28" s="31">
+        <v>0</v>
+      </c>
+      <c r="W28" s="31">
+        <v>0</v>
+      </c>
+      <c r="X28" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="31">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="31">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="32">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD28" s="45"/>
+      <c r="AE28" s="45"/>
+      <c r="AF28" s="45"/>
+      <c r="AG28" s="45"/>
+      <c r="AH28" s="45"/>
+      <c r="AI28" s="45"/>
+      <c r="AJ28" s="46"/>
+      <c r="AK28" s="10"/>
+    </row>
+    <row r="29" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="H29" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="V27" s="67"/>
-      <c r="W27" s="67"/>
-      <c r="X27" s="67"/>
-      <c r="Y27" s="67"/>
-      <c r="Z27" s="67"/>
-      <c r="AA27" s="67"/>
-      <c r="AB27" s="68"/>
-      <c r="AC27" s="69" t="s">
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="37"/>
+      <c r="Z29" s="37"/>
+      <c r="AA29" s="37"/>
+      <c r="AB29" s="77"/>
+      <c r="AC29" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD29" s="38"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="38"/>
+      <c r="AG29" s="38"/>
+      <c r="AH29" s="38"/>
+      <c r="AI29" s="38"/>
+      <c r="AJ29" s="39"/>
+      <c r="AK29" s="10"/>
+    </row>
+    <row r="30" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="34">
+        <v>0</v>
+      </c>
+      <c r="I30" s="34">
+        <v>0</v>
+      </c>
+      <c r="J30" s="34">
+        <v>0</v>
+      </c>
+      <c r="K30" s="34">
+        <v>0</v>
+      </c>
+      <c r="L30" s="35">
+        <v>0</v>
+      </c>
+      <c r="M30" s="33">
+        <v>0</v>
+      </c>
+      <c r="N30" s="34">
+        <v>0</v>
+      </c>
+      <c r="O30" s="34">
+        <v>0</v>
+      </c>
+      <c r="P30" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="34">
+        <v>0</v>
+      </c>
+      <c r="R30" s="34">
+        <v>0</v>
+      </c>
+      <c r="S30" s="34">
+        <v>0</v>
+      </c>
+      <c r="T30" s="35">
+        <v>0</v>
+      </c>
+      <c r="U30" s="33">
+        <v>0</v>
+      </c>
+      <c r="V30" s="34">
+        <v>0</v>
+      </c>
+      <c r="W30" s="34">
+        <v>0</v>
+      </c>
+      <c r="X30" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="34">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="35">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AG30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AI30" s="34">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="35">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="10"/>
+    </row>
+    <row r="31" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="H31" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="76"/>
+      <c r="U31" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="AD27" s="67"/>
-      <c r="AE27" s="67"/>
-      <c r="AF27" s="67"/>
-      <c r="AG27" s="67"/>
-      <c r="AH27" s="67"/>
-      <c r="AI27" s="67"/>
-      <c r="AJ27" s="68"/>
-      <c r="AK27" s="10"/>
-    </row>
-    <row r="28" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" s="31">
-        <v>0</v>
-      </c>
-      <c r="I28" s="31">
-        <v>0</v>
-      </c>
-      <c r="J28" s="31">
-        <v>0</v>
-      </c>
-      <c r="K28" s="31">
-        <v>0</v>
-      </c>
-      <c r="L28" s="32">
-        <v>0</v>
-      </c>
-      <c r="M28" s="30">
-        <v>0</v>
-      </c>
-      <c r="N28" s="31">
-        <v>0</v>
-      </c>
-      <c r="O28" s="31">
-        <v>0</v>
-      </c>
-      <c r="P28" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="31">
-        <v>0</v>
-      </c>
-      <c r="R28" s="31">
-        <v>0</v>
-      </c>
-      <c r="S28" s="31">
-        <v>0</v>
-      </c>
-      <c r="T28" s="32">
-        <v>0</v>
-      </c>
-      <c r="U28" s="30">
-        <v>0</v>
-      </c>
-      <c r="V28" s="31">
-        <v>0</v>
-      </c>
-      <c r="W28" s="31">
-        <v>0</v>
-      </c>
-      <c r="X28" s="31">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="31">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="31">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="31">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="32">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD28" s="46"/>
-      <c r="AE28" s="46"/>
-      <c r="AF28" s="46"/>
-      <c r="AG28" s="46"/>
-      <c r="AH28" s="46"/>
-      <c r="AI28" s="46"/>
-      <c r="AJ28" s="47"/>
-      <c r="AK28" s="10"/>
-    </row>
-    <row r="29" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H29" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="N29" s="67"/>
-      <c r="O29" s="67"/>
-      <c r="P29" s="67"/>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="67"/>
-      <c r="T29" s="68"/>
-      <c r="U29" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="V29" s="67"/>
-      <c r="W29" s="67"/>
-      <c r="X29" s="67"/>
-      <c r="Y29" s="67"/>
-      <c r="Z29" s="67"/>
-      <c r="AA29" s="67"/>
-      <c r="AB29" s="68"/>
-      <c r="AC29" s="69" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD29" s="67"/>
-      <c r="AE29" s="67"/>
-      <c r="AF29" s="67"/>
-      <c r="AG29" s="67"/>
-      <c r="AH29" s="67"/>
-      <c r="AI29" s="67"/>
-      <c r="AJ29" s="68"/>
-      <c r="AK29" s="10"/>
-    </row>
-    <row r="30" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="G30" t="s">
+      <c r="V31" s="75"/>
+      <c r="W31" s="75"/>
+      <c r="X31" s="75"/>
+      <c r="Y31" s="75"/>
+      <c r="Z31" s="75"/>
+      <c r="AA31" s="75"/>
+      <c r="AB31" s="76"/>
+      <c r="AC31" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="H30" s="34">
-        <v>0</v>
-      </c>
-      <c r="I30" s="34">
-        <v>0</v>
-      </c>
-      <c r="J30" s="34">
-        <v>0</v>
-      </c>
-      <c r="K30" s="34">
-        <v>0</v>
-      </c>
-      <c r="L30" s="35">
-        <v>0</v>
-      </c>
-      <c r="M30" s="33">
-        <v>0</v>
-      </c>
-      <c r="N30" s="34">
-        <v>0</v>
-      </c>
-      <c r="O30" s="34">
-        <v>0</v>
-      </c>
-      <c r="P30" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="34">
-        <v>0</v>
-      </c>
-      <c r="R30" s="34">
-        <v>0</v>
-      </c>
-      <c r="S30" s="34">
-        <v>0</v>
-      </c>
-      <c r="T30" s="35">
-        <v>0</v>
-      </c>
-      <c r="U30" s="33">
-        <v>0</v>
-      </c>
-      <c r="V30" s="34">
-        <v>0</v>
-      </c>
-      <c r="W30" s="34">
-        <v>0</v>
-      </c>
-      <c r="X30" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z30" s="34">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="35">
-        <v>1</v>
-      </c>
-      <c r="AC30" s="33">
-        <v>1</v>
-      </c>
-      <c r="AD30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AE30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AF30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AG30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AH30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AI30" s="34">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="35">
-        <v>1</v>
-      </c>
-      <c r="AK30" s="10"/>
-    </row>
-    <row r="31" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H31" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67"/>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="68"/>
-      <c r="U31" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="V31" s="67"/>
-      <c r="W31" s="67"/>
-      <c r="X31" s="67"/>
-      <c r="Y31" s="67"/>
-      <c r="Z31" s="67"/>
-      <c r="AA31" s="67"/>
-      <c r="AB31" s="68"/>
-      <c r="AC31" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD31" s="67"/>
-      <c r="AE31" s="67"/>
-      <c r="AF31" s="67"/>
-      <c r="AG31" s="67"/>
-      <c r="AH31" s="67"/>
-      <c r="AI31" s="67"/>
-      <c r="AJ31" s="68"/>
+      <c r="AD31" s="72"/>
+      <c r="AE31" s="72"/>
+      <c r="AF31" s="72"/>
+      <c r="AG31" s="72"/>
+      <c r="AH31" s="72"/>
+      <c r="AI31" s="72"/>
+      <c r="AJ31" s="73"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -4183,6 +4221,64 @@
     <sortCondition ref="L3:L15"/>
   </sortState>
   <mergeCells count="74">
+    <mergeCell ref="BR14:BY14"/>
+    <mergeCell ref="BZ14:CG14"/>
+    <mergeCell ref="CH14:CO14"/>
+    <mergeCell ref="CP14:CW14"/>
+    <mergeCell ref="CP15:CW15"/>
+    <mergeCell ref="CH16:CO16"/>
+    <mergeCell ref="BR15:BY15"/>
+    <mergeCell ref="BZ15:CG15"/>
+    <mergeCell ref="CH15:CO15"/>
+    <mergeCell ref="AL15:AS15"/>
+    <mergeCell ref="AT15:BA15"/>
+    <mergeCell ref="BJ15:BQ15"/>
+    <mergeCell ref="BB15:BI15"/>
+    <mergeCell ref="BR16:BY16"/>
+    <mergeCell ref="BZ16:CG16"/>
+    <mergeCell ref="M14:T14"/>
+    <mergeCell ref="U15:AB15"/>
+    <mergeCell ref="U16:AB16"/>
+    <mergeCell ref="U17:AB17"/>
+    <mergeCell ref="U13:AB13"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="AL11:AS11"/>
+    <mergeCell ref="AL6:BA6"/>
+    <mergeCell ref="AL14:BQ14"/>
+    <mergeCell ref="M18:T18"/>
+    <mergeCell ref="AV8:BE8"/>
+    <mergeCell ref="BF8:BQ8"/>
+    <mergeCell ref="AC10:AJ10"/>
+    <mergeCell ref="AL10:AS10"/>
+    <mergeCell ref="M6:T6"/>
+    <mergeCell ref="M13:T13"/>
+    <mergeCell ref="AC7:AJ7"/>
+    <mergeCell ref="AC6:AJ6"/>
+    <mergeCell ref="U14:AB14"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="M15:T15"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="AL1:CW1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="S1:AJ1"/>
+    <mergeCell ref="AL7:AS7"/>
+    <mergeCell ref="AL13:AS13"/>
+    <mergeCell ref="AC11:AJ11"/>
+    <mergeCell ref="AL16:BQ16"/>
+    <mergeCell ref="AL9:AU9"/>
+    <mergeCell ref="AV9:BE9"/>
+    <mergeCell ref="BF9:BQ9"/>
+    <mergeCell ref="AT13:BQ13"/>
+    <mergeCell ref="U18:AB18"/>
+    <mergeCell ref="AC18:AJ18"/>
+    <mergeCell ref="AL8:AU8"/>
+    <mergeCell ref="M24:T24"/>
+    <mergeCell ref="M27:T27"/>
+    <mergeCell ref="U27:AB27"/>
+    <mergeCell ref="AC27:AJ27"/>
+    <mergeCell ref="AC24:AJ24"/>
+    <mergeCell ref="U24:AB24"/>
     <mergeCell ref="H31:L31"/>
     <mergeCell ref="AL12:BQ12"/>
     <mergeCell ref="H22:L22"/>
@@ -4199,64 +4295,6 @@
     <mergeCell ref="AC22:AJ22"/>
     <mergeCell ref="U22:AB22"/>
     <mergeCell ref="M22:T22"/>
-    <mergeCell ref="M24:T24"/>
-    <mergeCell ref="M27:T27"/>
-    <mergeCell ref="U27:AB27"/>
-    <mergeCell ref="AC27:AJ27"/>
-    <mergeCell ref="AC24:AJ24"/>
-    <mergeCell ref="U24:AB24"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="AL1:CW1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:R1"/>
-    <mergeCell ref="S1:AJ1"/>
-    <mergeCell ref="AL9:AS9"/>
-    <mergeCell ref="AL17:AS17"/>
-    <mergeCell ref="AC8:AJ8"/>
-    <mergeCell ref="AL15:BQ15"/>
-    <mergeCell ref="AL6:AU6"/>
-    <mergeCell ref="AV6:BE6"/>
-    <mergeCell ref="BF6:BQ6"/>
-    <mergeCell ref="AT17:BQ17"/>
-    <mergeCell ref="U18:AB18"/>
-    <mergeCell ref="AC18:AJ18"/>
-    <mergeCell ref="AL5:AU5"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="AL8:AS8"/>
-    <mergeCell ref="AL10:BA10"/>
-    <mergeCell ref="AL13:BQ13"/>
-    <mergeCell ref="M18:T18"/>
-    <mergeCell ref="AV5:BE5"/>
-    <mergeCell ref="BF5:BQ5"/>
-    <mergeCell ref="AC7:AJ7"/>
-    <mergeCell ref="AL7:AS7"/>
-    <mergeCell ref="M10:T10"/>
-    <mergeCell ref="M17:T17"/>
-    <mergeCell ref="AC9:AJ9"/>
-    <mergeCell ref="AC10:AJ10"/>
-    <mergeCell ref="U13:AB13"/>
-    <mergeCell ref="M15:T15"/>
-    <mergeCell ref="M14:T14"/>
-    <mergeCell ref="M13:T13"/>
-    <mergeCell ref="U14:AB14"/>
-    <mergeCell ref="U15:AB15"/>
-    <mergeCell ref="U16:AB16"/>
-    <mergeCell ref="U17:AB17"/>
-    <mergeCell ref="CH15:CO15"/>
-    <mergeCell ref="BR14:BY14"/>
-    <mergeCell ref="BZ14:CG14"/>
-    <mergeCell ref="CH14:CO14"/>
-    <mergeCell ref="AL14:AS14"/>
-    <mergeCell ref="AT14:BA14"/>
-    <mergeCell ref="BJ14:BQ14"/>
-    <mergeCell ref="BB14:BI14"/>
-    <mergeCell ref="BR15:BY15"/>
-    <mergeCell ref="BZ15:CG15"/>
-    <mergeCell ref="BR13:BY13"/>
-    <mergeCell ref="BZ13:CG13"/>
-    <mergeCell ref="CH13:CO13"/>
-    <mergeCell ref="CP13:CW13"/>
-    <mergeCell ref="CP14:CW14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4280,182 +4318,182 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5">
         <v>64</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="4">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4">
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20">
         <f>SUM(B3:B18)</f>
@@ -4464,38 +4502,38 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22">
         <f>1024*1024</f>
         <v>1048576</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23">
         <f>INT(B22/B20)</f>
         <v>8004</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <f>INT(B23*8/1024)</f>
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added console to main project
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="200">
   <si>
     <t>CAN-Messages</t>
   </si>
@@ -592,6 +592,30 @@
   </si>
   <si>
     <t>DATA_OVERFLOW_SINGLE= 0x1D,      //11101</t>
+  </si>
+  <si>
+    <t>0000 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 1001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 0100 1010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0001 1010</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>e7</t>
+  </si>
+  <si>
+    <t>000b8</t>
+  </si>
+  <si>
+    <t>Started (1Bit)</t>
   </si>
 </sst>
 </file>
@@ -1006,19 +1030,34 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1035,18 +1074,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1135,7 +1162,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1439,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AT23" sqref="AT23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="BH20" sqref="BH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,115 +1484,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68" t="s">
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="69"/>
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="69"/>
+      <c r="AJ1" s="69"/>
       <c r="AK1" s="9"/>
-      <c r="AL1" s="68" t="s">
+      <c r="AL1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="68"/>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="68"/>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="68"/>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="68"/>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="68"/>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="68"/>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="68"/>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="68"/>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="68"/>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
+      <c r="AM1" s="69"/>
+      <c r="AN1" s="69"/>
+      <c r="AO1" s="69"/>
+      <c r="AP1" s="69"/>
+      <c r="AQ1" s="69"/>
+      <c r="AR1" s="69"/>
+      <c r="AS1" s="69"/>
+      <c r="AT1" s="69"/>
+      <c r="AU1" s="69"/>
+      <c r="AV1" s="69"/>
+      <c r="AW1" s="69"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="69"/>
+      <c r="AZ1" s="69"/>
+      <c r="BA1" s="69"/>
+      <c r="BB1" s="69"/>
+      <c r="BC1" s="69"/>
+      <c r="BD1" s="69"/>
+      <c r="BE1" s="69"/>
+      <c r="BF1" s="69"/>
+      <c r="BG1" s="69"/>
+      <c r="BH1" s="69"/>
+      <c r="BI1" s="69"/>
+      <c r="BJ1" s="69"/>
+      <c r="BK1" s="69"/>
+      <c r="BL1" s="69"/>
+      <c r="BM1" s="69"/>
+      <c r="BN1" s="69"/>
+      <c r="BO1" s="69"/>
+      <c r="BP1" s="69"/>
+      <c r="BQ1" s="69"/>
+      <c r="BR1" s="69"/>
+      <c r="BS1" s="69"/>
+      <c r="BT1" s="69"/>
+      <c r="BU1" s="69"/>
+      <c r="BV1" s="69"/>
+      <c r="BW1" s="69"/>
+      <c r="BX1" s="69"/>
+      <c r="BY1" s="69"/>
+      <c r="BZ1" s="69"/>
+      <c r="CA1" s="69"/>
+      <c r="CB1" s="69"/>
+      <c r="CC1" s="69"/>
+      <c r="CD1" s="69"/>
+      <c r="CE1" s="69"/>
+      <c r="CF1" s="69"/>
+      <c r="CG1" s="69"/>
+      <c r="CH1" s="69"/>
+      <c r="CI1" s="69"/>
+      <c r="CJ1" s="69"/>
+      <c r="CK1" s="69"/>
+      <c r="CL1" s="69"/>
+      <c r="CM1" s="69"/>
+      <c r="CN1" s="69"/>
+      <c r="CO1" s="69"/>
+      <c r="CP1" s="69"/>
+      <c r="CQ1" s="69"/>
+      <c r="CR1" s="69"/>
+      <c r="CS1" s="69"/>
+      <c r="CT1" s="69"/>
+      <c r="CU1" s="69"/>
+      <c r="CV1" s="69"/>
+      <c r="CW1" s="69"/>
       <c r="CX1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2103,50 +2129,50 @@
       <c r="AJ4" s="41">
         <v>1</v>
       </c>
-      <c r="AL4" s="64" t="s">
+      <c r="AL4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="AM4" s="65"/>
-      <c r="AN4" s="65"/>
-      <c r="AO4" s="65"/>
-      <c r="AP4" s="65"/>
-      <c r="AQ4" s="65"/>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="65"/>
-      <c r="AT4" s="53" t="s">
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="60"/>
+      <c r="AO4" s="60"/>
+      <c r="AP4" s="60"/>
+      <c r="AQ4" s="60"/>
+      <c r="AR4" s="60"/>
+      <c r="AS4" s="60"/>
+      <c r="AT4" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="AU4" s="53"/>
-      <c r="AV4" s="53"/>
-      <c r="AW4" s="53"/>
-      <c r="AX4" s="53"/>
-      <c r="AY4" s="53"/>
-      <c r="AZ4" s="53"/>
-      <c r="BA4" s="53"/>
-      <c r="BB4" s="53"/>
-      <c r="BC4" s="53"/>
-      <c r="BD4" s="53"/>
-      <c r="BE4" s="53"/>
-      <c r="BF4" s="53"/>
-      <c r="BG4" s="53"/>
-      <c r="BH4" s="53"/>
-      <c r="BI4" s="53"/>
-      <c r="BJ4" s="53"/>
-      <c r="BK4" s="53"/>
-      <c r="BL4" s="53"/>
-      <c r="BM4" s="53"/>
-      <c r="BN4" s="53"/>
-      <c r="BO4" s="53"/>
-      <c r="BP4" s="53"/>
-      <c r="BQ4" s="53"/>
-      <c r="BR4" s="53"/>
-      <c r="BS4" s="53"/>
-      <c r="BT4" s="53"/>
-      <c r="BU4" s="53"/>
-      <c r="BV4" s="53"/>
-      <c r="BW4" s="53"/>
-      <c r="BX4" s="53"/>
-      <c r="BY4" s="53"/>
+      <c r="AU4" s="55"/>
+      <c r="AV4" s="55"/>
+      <c r="AW4" s="55"/>
+      <c r="AX4" s="55"/>
+      <c r="AY4" s="55"/>
+      <c r="AZ4" s="55"/>
+      <c r="BA4" s="55"/>
+      <c r="BB4" s="55"/>
+      <c r="BC4" s="55"/>
+      <c r="BD4" s="55"/>
+      <c r="BE4" s="55"/>
+      <c r="BF4" s="55"/>
+      <c r="BG4" s="55"/>
+      <c r="BH4" s="55"/>
+      <c r="BI4" s="55"/>
+      <c r="BJ4" s="55"/>
+      <c r="BK4" s="55"/>
+      <c r="BL4" s="55"/>
+      <c r="BM4" s="55"/>
+      <c r="BN4" s="55"/>
+      <c r="BO4" s="55"/>
+      <c r="BP4" s="55"/>
+      <c r="BQ4" s="55"/>
+      <c r="BR4" s="55"/>
+      <c r="BS4" s="55"/>
+      <c r="BT4" s="55"/>
+      <c r="BU4" s="55"/>
+      <c r="BV4" s="55"/>
+      <c r="BW4" s="55"/>
+      <c r="BX4" s="55"/>
+      <c r="BY4" s="55"/>
       <c r="CG4" s="18"/>
       <c r="CI4" s="3"/>
       <c r="CO4" s="18"/>
@@ -2476,16 +2502,16 @@
       <c r="L7" s="12">
         <v>0</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
       <c r="U7" s="14">
         <v>0</v>
       </c>
@@ -2534,16 +2560,16 @@
       <c r="AJ7" s="41">
         <v>1</v>
       </c>
-      <c r="AL7" s="64" t="s">
+      <c r="AL7" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="AM7" s="65"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="65"/>
-      <c r="AP7" s="65"/>
-      <c r="AQ7" s="65"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="65"/>
+      <c r="AM7" s="60"/>
+      <c r="AN7" s="60"/>
+      <c r="AO7" s="60"/>
+      <c r="AP7" s="60"/>
+      <c r="AQ7" s="60"/>
+      <c r="AR7" s="60"/>
+      <c r="AS7" s="60"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="18"/>
       <c r="BE7" s="3"/>
@@ -2594,16 +2620,16 @@
       <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="54" t="s">
+      <c r="M8" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
       <c r="U8" s="14">
         <v>0</v>
       </c>
@@ -2652,64 +2678,72 @@
       <c r="AJ8" s="41">
         <v>1</v>
       </c>
-      <c r="AL8" s="72" t="s">
+      <c r="AL8" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="AM8" s="73"/>
-      <c r="AN8" s="73"/>
-      <c r="AO8" s="73"/>
-      <c r="AP8" s="73"/>
-      <c r="AQ8" s="73"/>
-      <c r="AR8" s="73"/>
-      <c r="AS8" s="73"/>
-      <c r="AT8" s="73"/>
-      <c r="AU8" s="73"/>
-      <c r="AV8" s="63" t="s">
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="AW8" s="63"/>
-      <c r="AX8" s="63"/>
-      <c r="AY8" s="63"/>
-      <c r="AZ8" s="63"/>
-      <c r="BA8" s="63"/>
-      <c r="BB8" s="63"/>
-      <c r="BC8" s="63"/>
-      <c r="BD8" s="63"/>
-      <c r="BE8" s="63"/>
-      <c r="BF8" s="57" t="s">
+      <c r="AW8" s="57"/>
+      <c r="AX8" s="57"/>
+      <c r="AY8" s="57"/>
+      <c r="AZ8" s="57"/>
+      <c r="BA8" s="57"/>
+      <c r="BB8" s="57"/>
+      <c r="BC8" s="57"/>
+      <c r="BD8" s="57"/>
+      <c r="BE8" s="57"/>
+      <c r="BF8" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="BG8" s="57"/>
-      <c r="BH8" s="57"/>
-      <c r="BI8" s="57"/>
-      <c r="BJ8" s="57"/>
-      <c r="BK8" s="57"/>
-      <c r="BL8" s="57"/>
-      <c r="BM8" s="57"/>
-      <c r="BN8" s="57"/>
-      <c r="BO8" s="57"/>
-      <c r="BP8" s="57"/>
-      <c r="BQ8" s="57"/>
-      <c r="BR8" s="74" t="s">
+      <c r="BG8" s="58"/>
+      <c r="BH8" s="58"/>
+      <c r="BI8" s="58"/>
+      <c r="BJ8" s="58"/>
+      <c r="BK8" s="58"/>
+      <c r="BL8" s="58"/>
+      <c r="BM8" s="58"/>
+      <c r="BN8" s="58"/>
+      <c r="BO8" s="58"/>
+      <c r="BP8" s="58"/>
+      <c r="BQ8" s="58"/>
+      <c r="BR8" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="BS8" s="74"/>
-      <c r="BT8" s="74"/>
-      <c r="BU8" s="74"/>
-      <c r="BV8" s="74"/>
-      <c r="BW8" s="74"/>
-      <c r="BX8" s="74"/>
-      <c r="BY8" s="74"/>
-      <c r="BZ8" s="74"/>
-      <c r="CA8" s="74"/>
-      <c r="CB8" s="74"/>
-      <c r="CC8" s="74"/>
-      <c r="CD8" s="74"/>
-      <c r="CE8" s="74"/>
-      <c r="CF8" s="74"/>
-      <c r="CG8" s="74"/>
-      <c r="CI8" s="3"/>
-      <c r="CO8" s="18"/>
+      <c r="BS8" s="75"/>
+      <c r="BT8" s="75"/>
+      <c r="BU8" s="75"/>
+      <c r="BV8" s="75"/>
+      <c r="BW8" s="75"/>
+      <c r="BX8" s="75"/>
+      <c r="BY8" s="75"/>
+      <c r="BZ8" s="75"/>
+      <c r="CA8" s="75"/>
+      <c r="CB8" s="75"/>
+      <c r="CC8" s="75"/>
+      <c r="CD8" s="75"/>
+      <c r="CE8" s="75"/>
+      <c r="CF8" s="75"/>
+      <c r="CG8" s="75"/>
+      <c r="CH8" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="CI8" s="60"/>
+      <c r="CJ8" s="60"/>
+      <c r="CK8" s="60"/>
+      <c r="CL8" s="60"/>
+      <c r="CM8" s="60"/>
+      <c r="CN8" s="60"/>
+      <c r="CO8" s="60"/>
       <c r="CS8" s="3"/>
       <c r="CW8" s="18"/>
       <c r="CX8">
@@ -2751,16 +2785,16 @@
       <c r="L9" s="34">
         <v>0</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
       <c r="U9" s="35">
         <v>0</v>
       </c>
@@ -3062,16 +3096,16 @@
       <c r="L11" s="12">
         <v>0</v>
       </c>
-      <c r="M11" s="54" t="s">
+      <c r="M11" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
       <c r="U11" s="14">
         <v>0</v>
       </c>
@@ -3120,16 +3154,16 @@
       <c r="AJ11" s="41">
         <v>1</v>
       </c>
-      <c r="AL11" s="64" t="s">
+      <c r="AL11" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="AM11" s="65"/>
-      <c r="AN11" s="65"/>
-      <c r="AO11" s="65"/>
-      <c r="AP11" s="65"/>
-      <c r="AQ11" s="65"/>
-      <c r="AR11" s="65"/>
-      <c r="AS11" s="65"/>
+      <c r="AM11" s="60"/>
+      <c r="AN11" s="60"/>
+      <c r="AO11" s="60"/>
+      <c r="AP11" s="60"/>
+      <c r="AQ11" s="60"/>
+      <c r="AR11" s="60"/>
+      <c r="AS11" s="60"/>
       <c r="AU11" s="3"/>
       <c r="BA11" s="18"/>
       <c r="BE11" s="3"/>
@@ -3252,16 +3286,16 @@
       <c r="AJ12" s="48">
         <v>1</v>
       </c>
-      <c r="AL12" s="64" t="s">
+      <c r="AL12" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="AM12" s="65"/>
-      <c r="AN12" s="65"/>
-      <c r="AO12" s="65"/>
-      <c r="AP12" s="65"/>
-      <c r="AQ12" s="65"/>
-      <c r="AR12" s="65"/>
-      <c r="AS12" s="65"/>
+      <c r="AM12" s="60"/>
+      <c r="AN12" s="60"/>
+      <c r="AO12" s="60"/>
+      <c r="AP12" s="60"/>
+      <c r="AQ12" s="60"/>
+      <c r="AR12" s="60"/>
+      <c r="AS12" s="60"/>
       <c r="AU12" s="3"/>
       <c r="BA12" s="18"/>
       <c r="BE12" s="3"/>
@@ -3386,40 +3420,40 @@
         <v>1</v>
       </c>
       <c r="AK13" s="49"/>
-      <c r="AL13" s="85" t="s">
+      <c r="AL13" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="AM13" s="86"/>
-      <c r="AN13" s="86"/>
-      <c r="AO13" s="86"/>
-      <c r="AP13" s="86"/>
-      <c r="AQ13" s="86"/>
-      <c r="AR13" s="86"/>
-      <c r="AS13" s="86"/>
-      <c r="AT13" s="86"/>
-      <c r="AU13" s="86"/>
-      <c r="AV13" s="86"/>
-      <c r="AW13" s="86"/>
-      <c r="AX13" s="86"/>
-      <c r="AY13" s="86"/>
-      <c r="AZ13" s="86"/>
-      <c r="BA13" s="86"/>
-      <c r="BB13" s="86"/>
-      <c r="BC13" s="86"/>
-      <c r="BD13" s="86"/>
-      <c r="BE13" s="86"/>
-      <c r="BF13" s="86"/>
-      <c r="BG13" s="86"/>
-      <c r="BH13" s="86"/>
-      <c r="BI13" s="86"/>
-      <c r="BJ13" s="86"/>
-      <c r="BK13" s="86"/>
-      <c r="BL13" s="86"/>
-      <c r="BM13" s="86"/>
-      <c r="BN13" s="86"/>
-      <c r="BO13" s="86"/>
-      <c r="BP13" s="86"/>
-      <c r="BQ13" s="86"/>
+      <c r="AM13" s="87"/>
+      <c r="AN13" s="87"/>
+      <c r="AO13" s="87"/>
+      <c r="AP13" s="87"/>
+      <c r="AQ13" s="87"/>
+      <c r="AR13" s="87"/>
+      <c r="AS13" s="87"/>
+      <c r="AT13" s="87"/>
+      <c r="AU13" s="87"/>
+      <c r="AV13" s="87"/>
+      <c r="AW13" s="87"/>
+      <c r="AX13" s="87"/>
+      <c r="AY13" s="87"/>
+      <c r="AZ13" s="87"/>
+      <c r="BA13" s="87"/>
+      <c r="BB13" s="87"/>
+      <c r="BC13" s="87"/>
+      <c r="BD13" s="87"/>
+      <c r="BE13" s="87"/>
+      <c r="BF13" s="87"/>
+      <c r="BG13" s="87"/>
+      <c r="BH13" s="87"/>
+      <c r="BI13" s="87"/>
+      <c r="BJ13" s="87"/>
+      <c r="BK13" s="87"/>
+      <c r="BL13" s="87"/>
+      <c r="BM13" s="87"/>
+      <c r="BN13" s="87"/>
+      <c r="BO13" s="87"/>
+      <c r="BP13" s="87"/>
+      <c r="BQ13" s="87"/>
       <c r="BR13" s="23"/>
       <c r="BS13" s="23"/>
       <c r="BT13" s="23"/>
@@ -3514,16 +3548,16 @@
       <c r="T14" s="15">
         <v>1</v>
       </c>
-      <c r="U14" s="59" t="s">
+      <c r="U14" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="V14" s="59"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="59"/>
-      <c r="Y14" s="59"/>
-      <c r="Z14" s="59"/>
-      <c r="AA14" s="59"/>
-      <c r="AB14" s="59"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="64"/>
+      <c r="X14" s="64"/>
+      <c r="Y14" s="64"/>
+      <c r="Z14" s="64"/>
+      <c r="AA14" s="64"/>
+      <c r="AB14" s="64"/>
       <c r="AC14" s="13">
         <v>0</v>
       </c>
@@ -3548,50 +3582,50 @@
       <c r="AJ14" s="41">
         <v>1</v>
       </c>
-      <c r="AL14" s="64" t="s">
+      <c r="AL14" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AM14" s="66"/>
-      <c r="AN14" s="66"/>
-      <c r="AO14" s="66"/>
-      <c r="AP14" s="66"/>
-      <c r="AQ14" s="66"/>
-      <c r="AR14" s="66"/>
-      <c r="AS14" s="66"/>
-      <c r="AT14" s="66"/>
-      <c r="AU14" s="66"/>
-      <c r="AV14" s="66"/>
-      <c r="AW14" s="66"/>
-      <c r="AX14" s="66"/>
-      <c r="AY14" s="66"/>
-      <c r="AZ14" s="66"/>
-      <c r="BA14" s="66"/>
-      <c r="BB14" s="57" t="s">
+      <c r="AM14" s="61"/>
+      <c r="AN14" s="61"/>
+      <c r="AO14" s="61"/>
+      <c r="AP14" s="61"/>
+      <c r="AQ14" s="61"/>
+      <c r="AR14" s="61"/>
+      <c r="AS14" s="61"/>
+      <c r="AT14" s="61"/>
+      <c r="AU14" s="61"/>
+      <c r="AV14" s="61"/>
+      <c r="AW14" s="61"/>
+      <c r="AX14" s="61"/>
+      <c r="AY14" s="61"/>
+      <c r="AZ14" s="61"/>
+      <c r="BA14" s="61"/>
+      <c r="BB14" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="BC14" s="57"/>
-      <c r="BD14" s="57"/>
-      <c r="BE14" s="57"/>
-      <c r="BF14" s="57"/>
-      <c r="BG14" s="57"/>
-      <c r="BH14" s="57"/>
-      <c r="BI14" s="57"/>
-      <c r="BJ14" s="57"/>
-      <c r="BK14" s="57"/>
-      <c r="BL14" s="57"/>
-      <c r="BM14" s="57"/>
-      <c r="BN14" s="57"/>
-      <c r="BO14" s="57"/>
-      <c r="BP14" s="57"/>
-      <c r="BQ14" s="57"/>
-      <c r="BR14" s="57"/>
-      <c r="BS14" s="57"/>
-      <c r="BT14" s="57"/>
-      <c r="BU14" s="57"/>
-      <c r="BV14" s="57"/>
-      <c r="BW14" s="57"/>
-      <c r="BX14" s="57"/>
-      <c r="BY14" s="57"/>
+      <c r="BC14" s="58"/>
+      <c r="BD14" s="58"/>
+      <c r="BE14" s="58"/>
+      <c r="BF14" s="58"/>
+      <c r="BG14" s="58"/>
+      <c r="BH14" s="58"/>
+      <c r="BI14" s="58"/>
+      <c r="BJ14" s="58"/>
+      <c r="BK14" s="58"/>
+      <c r="BL14" s="58"/>
+      <c r="BM14" s="58"/>
+      <c r="BN14" s="58"/>
+      <c r="BO14" s="58"/>
+      <c r="BP14" s="58"/>
+      <c r="BQ14" s="58"/>
+      <c r="BR14" s="58"/>
+      <c r="BS14" s="58"/>
+      <c r="BT14" s="58"/>
+      <c r="BU14" s="58"/>
+      <c r="BV14" s="58"/>
+      <c r="BW14" s="58"/>
+      <c r="BX14" s="58"/>
+      <c r="BY14" s="58"/>
       <c r="CG14" s="18"/>
       <c r="CI14" s="3"/>
       <c r="CO14" s="18"/>
@@ -3662,100 +3696,100 @@
       <c r="T15" s="15">
         <v>1</v>
       </c>
-      <c r="U15" s="59" t="s">
+      <c r="U15" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="V15" s="59"/>
-      <c r="W15" s="59"/>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="60" t="s">
+      <c r="V15" s="64"/>
+      <c r="W15" s="64"/>
+      <c r="X15" s="64"/>
+      <c r="Y15" s="64"/>
+      <c r="Z15" s="64"/>
+      <c r="AA15" s="64"/>
+      <c r="AB15" s="64"/>
+      <c r="AC15" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="AD15" s="61"/>
-      <c r="AE15" s="61"/>
-      <c r="AF15" s="61"/>
-      <c r="AG15" s="61"/>
-      <c r="AH15" s="61"/>
-      <c r="AI15" s="61"/>
-      <c r="AJ15" s="61"/>
-      <c r="AL15" s="64" t="s">
+      <c r="AD15" s="66"/>
+      <c r="AE15" s="66"/>
+      <c r="AF15" s="66"/>
+      <c r="AG15" s="66"/>
+      <c r="AH15" s="66"/>
+      <c r="AI15" s="66"/>
+      <c r="AJ15" s="66"/>
+      <c r="AL15" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="AM15" s="65"/>
-      <c r="AN15" s="65"/>
-      <c r="AO15" s="65"/>
-      <c r="AP15" s="65"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="65"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="65"/>
-      <c r="AW15" s="65"/>
-      <c r="AX15" s="65"/>
-      <c r="AY15" s="65"/>
-      <c r="AZ15" s="65"/>
-      <c r="BA15" s="65"/>
-      <c r="BB15" s="65"/>
-      <c r="BC15" s="65"/>
-      <c r="BD15" s="65"/>
-      <c r="BE15" s="65"/>
-      <c r="BF15" s="65"/>
-      <c r="BG15" s="65"/>
-      <c r="BH15" s="65"/>
-      <c r="BI15" s="65"/>
-      <c r="BJ15" s="65"/>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="65"/>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-      <c r="BP15" s="65"/>
-      <c r="BQ15" s="65"/>
-      <c r="BR15" s="55" t="s">
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="60"/>
+      <c r="AO15" s="60"/>
+      <c r="AP15" s="60"/>
+      <c r="AQ15" s="60"/>
+      <c r="AR15" s="60"/>
+      <c r="AS15" s="60"/>
+      <c r="AT15" s="60"/>
+      <c r="AU15" s="60"/>
+      <c r="AV15" s="60"/>
+      <c r="AW15" s="60"/>
+      <c r="AX15" s="60"/>
+      <c r="AY15" s="60"/>
+      <c r="AZ15" s="60"/>
+      <c r="BA15" s="60"/>
+      <c r="BB15" s="60"/>
+      <c r="BC15" s="60"/>
+      <c r="BD15" s="60"/>
+      <c r="BE15" s="60"/>
+      <c r="BF15" s="60"/>
+      <c r="BG15" s="60"/>
+      <c r="BH15" s="60"/>
+      <c r="BI15" s="60"/>
+      <c r="BJ15" s="60"/>
+      <c r="BK15" s="60"/>
+      <c r="BL15" s="60"/>
+      <c r="BM15" s="60"/>
+      <c r="BN15" s="60"/>
+      <c r="BO15" s="60"/>
+      <c r="BP15" s="60"/>
+      <c r="BQ15" s="60"/>
+      <c r="BR15" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="BS15" s="55"/>
-      <c r="BT15" s="55"/>
-      <c r="BU15" s="55"/>
-      <c r="BV15" s="55"/>
-      <c r="BW15" s="55"/>
-      <c r="BX15" s="55"/>
-      <c r="BY15" s="55"/>
-      <c r="BZ15" s="55" t="s">
+      <c r="BS15" s="53"/>
+      <c r="BT15" s="53"/>
+      <c r="BU15" s="53"/>
+      <c r="BV15" s="53"/>
+      <c r="BW15" s="53"/>
+      <c r="BX15" s="53"/>
+      <c r="BY15" s="53"/>
+      <c r="BZ15" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="CA15" s="55"/>
-      <c r="CB15" s="55"/>
-      <c r="CC15" s="55"/>
-      <c r="CD15" s="55"/>
-      <c r="CE15" s="55"/>
-      <c r="CF15" s="55"/>
-      <c r="CG15" s="55"/>
-      <c r="CH15" s="55" t="s">
+      <c r="CA15" s="53"/>
+      <c r="CB15" s="53"/>
+      <c r="CC15" s="53"/>
+      <c r="CD15" s="53"/>
+      <c r="CE15" s="53"/>
+      <c r="CF15" s="53"/>
+      <c r="CG15" s="53"/>
+      <c r="CH15" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="CI15" s="55"/>
-      <c r="CJ15" s="55"/>
-      <c r="CK15" s="55"/>
-      <c r="CL15" s="55"/>
-      <c r="CM15" s="55"/>
-      <c r="CN15" s="55"/>
-      <c r="CO15" s="55"/>
-      <c r="CP15" s="55" t="s">
+      <c r="CI15" s="53"/>
+      <c r="CJ15" s="53"/>
+      <c r="CK15" s="53"/>
+      <c r="CL15" s="53"/>
+      <c r="CM15" s="53"/>
+      <c r="CN15" s="53"/>
+      <c r="CO15" s="53"/>
+      <c r="CP15" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="CQ15" s="55"/>
-      <c r="CR15" s="55"/>
-      <c r="CS15" s="55"/>
-      <c r="CT15" s="55"/>
-      <c r="CU15" s="55"/>
-      <c r="CV15" s="55"/>
-      <c r="CW15" s="55"/>
+      <c r="CQ15" s="53"/>
+      <c r="CR15" s="53"/>
+      <c r="CS15" s="53"/>
+      <c r="CT15" s="53"/>
+      <c r="CU15" s="53"/>
+      <c r="CV15" s="53"/>
+      <c r="CW15" s="53"/>
       <c r="CX15" s="31" t="s">
         <v>121</v>
       </c>
@@ -3818,106 +3852,106 @@
       <c r="T16" s="15">
         <v>1</v>
       </c>
-      <c r="U16" s="59" t="s">
+      <c r="U16" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="V16" s="59"/>
-      <c r="W16" s="59"/>
-      <c r="X16" s="59"/>
-      <c r="Y16" s="59"/>
-      <c r="Z16" s="59"/>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="60" t="s">
+      <c r="V16" s="64"/>
+      <c r="W16" s="64"/>
+      <c r="X16" s="64"/>
+      <c r="Y16" s="64"/>
+      <c r="Z16" s="64"/>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
-      <c r="AG16" s="61"/>
-      <c r="AH16" s="61"/>
-      <c r="AI16" s="61"/>
-      <c r="AJ16" s="61"/>
-      <c r="AL16" s="55" t="s">
+      <c r="AD16" s="66"/>
+      <c r="AE16" s="66"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="66"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="66"/>
+      <c r="AJ16" s="66"/>
+      <c r="AL16" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AM16" s="55"/>
-      <c r="AN16" s="55"/>
-      <c r="AO16" s="55"/>
-      <c r="AP16" s="55"/>
-      <c r="AQ16" s="55"/>
-      <c r="AR16" s="55"/>
-      <c r="AS16" s="55"/>
-      <c r="AT16" s="55" t="s">
+      <c r="AM16" s="53"/>
+      <c r="AN16" s="53"/>
+      <c r="AO16" s="53"/>
+      <c r="AP16" s="53"/>
+      <c r="AQ16" s="53"/>
+      <c r="AR16" s="53"/>
+      <c r="AS16" s="53"/>
+      <c r="AT16" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="AU16" s="55"/>
-      <c r="AV16" s="55"/>
-      <c r="AW16" s="55"/>
-      <c r="AX16" s="55"/>
-      <c r="AY16" s="55"/>
-      <c r="AZ16" s="55"/>
-      <c r="BA16" s="55"/>
-      <c r="BB16" s="55" t="s">
+      <c r="AU16" s="53"/>
+      <c r="AV16" s="53"/>
+      <c r="AW16" s="53"/>
+      <c r="AX16" s="53"/>
+      <c r="AY16" s="53"/>
+      <c r="AZ16" s="53"/>
+      <c r="BA16" s="53"/>
+      <c r="BB16" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="BC16" s="55"/>
-      <c r="BD16" s="55"/>
-      <c r="BE16" s="55"/>
-      <c r="BF16" s="55"/>
-      <c r="BG16" s="55"/>
-      <c r="BH16" s="55"/>
-      <c r="BI16" s="55"/>
-      <c r="BJ16" s="55" t="s">
+      <c r="BC16" s="53"/>
+      <c r="BD16" s="53"/>
+      <c r="BE16" s="53"/>
+      <c r="BF16" s="53"/>
+      <c r="BG16" s="53"/>
+      <c r="BH16" s="53"/>
+      <c r="BI16" s="53"/>
+      <c r="BJ16" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="BK16" s="55"/>
-      <c r="BL16" s="55"/>
-      <c r="BM16" s="55"/>
-      <c r="BN16" s="55"/>
-      <c r="BO16" s="55"/>
-      <c r="BP16" s="55"/>
-      <c r="BQ16" s="55"/>
-      <c r="BR16" s="55" t="s">
+      <c r="BK16" s="53"/>
+      <c r="BL16" s="53"/>
+      <c r="BM16" s="53"/>
+      <c r="BN16" s="53"/>
+      <c r="BO16" s="53"/>
+      <c r="BP16" s="53"/>
+      <c r="BQ16" s="53"/>
+      <c r="BR16" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="BS16" s="55"/>
-      <c r="BT16" s="55"/>
-      <c r="BU16" s="55"/>
-      <c r="BV16" s="55"/>
-      <c r="BW16" s="55"/>
-      <c r="BX16" s="55"/>
-      <c r="BY16" s="55"/>
-      <c r="BZ16" s="55" t="s">
+      <c r="BS16" s="53"/>
+      <c r="BT16" s="53"/>
+      <c r="BU16" s="53"/>
+      <c r="BV16" s="53"/>
+      <c r="BW16" s="53"/>
+      <c r="BX16" s="53"/>
+      <c r="BY16" s="53"/>
+      <c r="BZ16" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="CA16" s="55"/>
-      <c r="CB16" s="55"/>
-      <c r="CC16" s="55"/>
-      <c r="CD16" s="55"/>
-      <c r="CE16" s="55"/>
-      <c r="CF16" s="55"/>
-      <c r="CG16" s="55"/>
-      <c r="CH16" s="55" t="s">
+      <c r="CA16" s="53"/>
+      <c r="CB16" s="53"/>
+      <c r="CC16" s="53"/>
+      <c r="CD16" s="53"/>
+      <c r="CE16" s="53"/>
+      <c r="CF16" s="53"/>
+      <c r="CG16" s="53"/>
+      <c r="CH16" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="CI16" s="55"/>
-      <c r="CJ16" s="55"/>
-      <c r="CK16" s="55"/>
-      <c r="CL16" s="55"/>
-      <c r="CM16" s="55"/>
-      <c r="CN16" s="55"/>
-      <c r="CO16" s="55"/>
-      <c r="CP16" s="55" t="s">
+      <c r="CI16" s="53"/>
+      <c r="CJ16" s="53"/>
+      <c r="CK16" s="53"/>
+      <c r="CL16" s="53"/>
+      <c r="CM16" s="53"/>
+      <c r="CN16" s="53"/>
+      <c r="CO16" s="53"/>
+      <c r="CP16" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="CQ16" s="55"/>
-      <c r="CR16" s="55"/>
-      <c r="CS16" s="55"/>
-      <c r="CT16" s="55"/>
-      <c r="CU16" s="55"/>
-      <c r="CV16" s="55"/>
-      <c r="CW16" s="55"/>
+      <c r="CQ16" s="53"/>
+      <c r="CR16" s="53"/>
+      <c r="CS16" s="53"/>
+      <c r="CT16" s="53"/>
+      <c r="CU16" s="53"/>
+      <c r="CV16" s="53"/>
+      <c r="CW16" s="53"/>
       <c r="CX16" s="21" t="s">
         <v>122</v>
       </c>
@@ -3980,92 +4014,98 @@
       <c r="T17" s="15">
         <v>1</v>
       </c>
-      <c r="U17" s="59" t="s">
+      <c r="U17" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="V17" s="59"/>
-      <c r="W17" s="59"/>
-      <c r="X17" s="59"/>
-      <c r="Y17" s="59"/>
-      <c r="Z17" s="59"/>
-      <c r="AA17" s="59"/>
-      <c r="AB17" s="59"/>
-      <c r="AC17" s="60" t="s">
+      <c r="V17" s="64"/>
+      <c r="W17" s="64"/>
+      <c r="X17" s="64"/>
+      <c r="Y17" s="64"/>
+      <c r="Z17" s="64"/>
+      <c r="AA17" s="64"/>
+      <c r="AB17" s="64"/>
+      <c r="AC17" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AL17" s="64" t="s">
+      <c r="AD17" s="66"/>
+      <c r="AE17" s="66"/>
+      <c r="AF17" s="66"/>
+      <c r="AG17" s="66"/>
+      <c r="AH17" s="66"/>
+      <c r="AI17" s="66"/>
+      <c r="AJ17" s="66"/>
+      <c r="AL17" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="AM17" s="65"/>
-      <c r="AN17" s="65"/>
-      <c r="AO17" s="65"/>
-      <c r="AP17" s="65"/>
-      <c r="AQ17" s="65"/>
-      <c r="AR17" s="65"/>
-      <c r="AS17" s="65"/>
-      <c r="AT17" s="65"/>
-      <c r="AU17" s="65"/>
-      <c r="AV17" s="65"/>
-      <c r="AW17" s="65"/>
-      <c r="AX17" s="65"/>
-      <c r="AY17" s="65"/>
-      <c r="AZ17" s="65"/>
-      <c r="BA17" s="65"/>
-      <c r="BB17" s="65"/>
-      <c r="BC17" s="65"/>
-      <c r="BD17" s="65"/>
-      <c r="BE17" s="65"/>
-      <c r="BF17" s="65"/>
-      <c r="BG17" s="65"/>
-      <c r="BH17" s="65"/>
-      <c r="BI17" s="65"/>
-      <c r="BJ17" s="65"/>
-      <c r="BK17" s="65"/>
-      <c r="BL17" s="65"/>
-      <c r="BM17" s="65"/>
-      <c r="BN17" s="65"/>
-      <c r="BO17" s="65"/>
-      <c r="BP17" s="65"/>
-      <c r="BQ17" s="65"/>
-      <c r="BR17" s="56" t="s">
+      <c r="AM17" s="60"/>
+      <c r="AN17" s="60"/>
+      <c r="AO17" s="60"/>
+      <c r="AP17" s="60"/>
+      <c r="AQ17" s="60"/>
+      <c r="AR17" s="60"/>
+      <c r="AS17" s="60"/>
+      <c r="AT17" s="60"/>
+      <c r="AU17" s="60"/>
+      <c r="AV17" s="60"/>
+      <c r="AW17" s="60"/>
+      <c r="AX17" s="60"/>
+      <c r="AY17" s="60"/>
+      <c r="AZ17" s="60"/>
+      <c r="BA17" s="60"/>
+      <c r="BB17" s="60"/>
+      <c r="BC17" s="60"/>
+      <c r="BD17" s="60"/>
+      <c r="BE17" s="60"/>
+      <c r="BF17" s="60"/>
+      <c r="BG17" s="60"/>
+      <c r="BH17" s="60"/>
+      <c r="BI17" s="60"/>
+      <c r="BJ17" s="60"/>
+      <c r="BK17" s="60"/>
+      <c r="BL17" s="60"/>
+      <c r="BM17" s="60"/>
+      <c r="BN17" s="60"/>
+      <c r="BO17" s="60"/>
+      <c r="BP17" s="60"/>
+      <c r="BQ17" s="60"/>
+      <c r="BR17" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="BS17" s="56"/>
-      <c r="BT17" s="56"/>
-      <c r="BU17" s="56"/>
-      <c r="BV17" s="56"/>
-      <c r="BW17" s="56"/>
-      <c r="BX17" s="56"/>
-      <c r="BY17" s="56"/>
-      <c r="BZ17" s="58" t="s">
+      <c r="BS17" s="62"/>
+      <c r="BT17" s="62"/>
+      <c r="BU17" s="62"/>
+      <c r="BV17" s="62"/>
+      <c r="BW17" s="62"/>
+      <c r="BX17" s="62"/>
+      <c r="BY17" s="62"/>
+      <c r="BZ17" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="CA17" s="58"/>
-      <c r="CB17" s="58"/>
-      <c r="CC17" s="58"/>
-      <c r="CD17" s="58"/>
-      <c r="CE17" s="58"/>
-      <c r="CF17" s="58"/>
-      <c r="CG17" s="58"/>
-      <c r="CH17" s="57" t="s">
+      <c r="CA17" s="63"/>
+      <c r="CB17" s="63"/>
+      <c r="CC17" s="63"/>
+      <c r="CD17" s="63"/>
+      <c r="CE17" s="63"/>
+      <c r="CF17" s="63"/>
+      <c r="CG17" s="63"/>
+      <c r="CH17" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="CI17" s="57"/>
-      <c r="CJ17" s="57"/>
-      <c r="CK17" s="57"/>
-      <c r="CL17" s="57"/>
-      <c r="CM17" s="57"/>
-      <c r="CN17" s="57"/>
-      <c r="CO17" s="57"/>
-      <c r="CS17" s="3"/>
-      <c r="CW17" s="18"/>
+      <c r="CI17" s="58"/>
+      <c r="CJ17" s="58"/>
+      <c r="CK17" s="58"/>
+      <c r="CL17" s="58"/>
+      <c r="CM17" s="58"/>
+      <c r="CN17" s="58"/>
+      <c r="CO17" s="58"/>
+      <c r="CP17" s="58"/>
+      <c r="CQ17" s="58"/>
+      <c r="CR17" s="58"/>
+      <c r="CS17" s="58"/>
+      <c r="CT17" s="58"/>
+      <c r="CU17" s="58"/>
+      <c r="CV17" s="58"/>
+      <c r="CW17" s="58"/>
       <c r="CX17">
         <v>7</v>
       </c>
@@ -4128,16 +4168,16 @@
       <c r="T18" s="39">
         <v>1</v>
       </c>
-      <c r="U18" s="62" t="s">
+      <c r="U18" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="62"/>
-      <c r="AB18" s="62"/>
+      <c r="V18" s="67"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="67"/>
+      <c r="Y18" s="67"/>
+      <c r="Z18" s="67"/>
+      <c r="AA18" s="67"/>
+      <c r="AB18" s="67"/>
       <c r="AC18" s="13">
         <v>0</v>
       </c>
@@ -4181,42 +4221,42 @@
       <c r="H19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="67" t="s">
+      <c r="I19" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="71" t="s">
+      <c r="J19" s="68"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="71"/>
-      <c r="O19" s="71"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="71"/>
-      <c r="S19" s="71"/>
-      <c r="T19" s="71"/>
-      <c r="U19" s="70" t="s">
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="V19" s="70"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="70"/>
-      <c r="Y19" s="70"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="75" t="s">
+      <c r="V19" s="71"/>
+      <c r="W19" s="71"/>
+      <c r="X19" s="71"/>
+      <c r="Y19" s="71"/>
+      <c r="Z19" s="71"/>
+      <c r="AA19" s="71"/>
+      <c r="AB19" s="71"/>
+      <c r="AC19" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="AD19" s="75"/>
-      <c r="AE19" s="75"/>
-      <c r="AF19" s="75"/>
-      <c r="AG19" s="75"/>
-      <c r="AH19" s="75"/>
-      <c r="AI19" s="75"/>
-      <c r="AJ19" s="75"/>
+      <c r="AD19" s="76"/>
+      <c r="AE19" s="76"/>
+      <c r="AF19" s="76"/>
+      <c r="AG19" s="76"/>
+      <c r="AH19" s="76"/>
+      <c r="AI19" s="76"/>
+      <c r="AJ19" s="76"/>
       <c r="AK19" s="43"/>
       <c r="AS19" s="18"/>
       <c r="AU19" s="3"/>
@@ -4236,14 +4276,70 @@
       <c r="G21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BR21" s="96"/>
-      <c r="BS21" s="96"/>
-      <c r="BT21" s="96"/>
-      <c r="BU21" s="96"/>
-      <c r="BV21" s="96"/>
-      <c r="BW21" s="96"/>
-      <c r="BX21" s="96"/>
-      <c r="BY21" s="96"/>
+      <c r="AL21" s="54">
+        <v>1098</v>
+      </c>
+      <c r="AM21" s="53"/>
+      <c r="AN21" s="53"/>
+      <c r="AO21" s="53"/>
+      <c r="AP21" s="53"/>
+      <c r="AQ21" s="53"/>
+      <c r="AR21" s="53"/>
+      <c r="AS21" s="53"/>
+      <c r="AT21" s="53"/>
+      <c r="AU21" s="53"/>
+      <c r="AV21" s="53"/>
+      <c r="AW21" s="53"/>
+      <c r="AX21" s="53"/>
+      <c r="AY21" s="53"/>
+      <c r="AZ21" s="53"/>
+      <c r="BA21" s="53"/>
+      <c r="BB21" s="53"/>
+      <c r="BC21" s="53"/>
+      <c r="BD21" s="53"/>
+      <c r="BE21" s="53"/>
+      <c r="BF21" s="53"/>
+      <c r="BG21" s="53"/>
+      <c r="BH21" s="53"/>
+      <c r="BI21" s="53"/>
+      <c r="BJ21" s="53"/>
+      <c r="BK21" s="53"/>
+      <c r="BL21" s="53"/>
+      <c r="BM21" s="53"/>
+      <c r="BN21" s="53"/>
+      <c r="BO21" s="53"/>
+      <c r="BP21" s="53"/>
+      <c r="BQ21" s="53"/>
+      <c r="BR21" s="53">
+        <v>26</v>
+      </c>
+      <c r="BS21" s="53"/>
+      <c r="BT21" s="53"/>
+      <c r="BU21" s="53"/>
+      <c r="BV21" s="53"/>
+      <c r="BW21" s="53"/>
+      <c r="BX21" s="53"/>
+      <c r="BY21" s="53"/>
+      <c r="BZ21" s="53">
+        <v>137</v>
+      </c>
+      <c r="CA21" s="53"/>
+      <c r="CB21" s="53"/>
+      <c r="CC21" s="53"/>
+      <c r="CD21" s="53"/>
+      <c r="CE21" s="53"/>
+      <c r="CF21" s="53"/>
+      <c r="CG21" s="53"/>
+      <c r="CH21" s="53">
+        <v>8</v>
+      </c>
+      <c r="CI21" s="53"/>
+      <c r="CJ21" s="53"/>
+      <c r="CK21" s="53"/>
+      <c r="CL21" s="53"/>
+      <c r="CM21" s="53"/>
+      <c r="CN21" s="53"/>
+      <c r="CO21" s="53"/>
     </row>
     <row r="22" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
@@ -4337,46 +4433,91 @@
         <v>1</v>
       </c>
       <c r="AK22" s="10"/>
+      <c r="AM22" t="s">
+        <v>194</v>
+      </c>
+      <c r="BR22" t="s">
+        <v>195</v>
+      </c>
+      <c r="BZ22" t="s">
+        <v>193</v>
+      </c>
+      <c r="CI22" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="23" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H23" s="80">
+      <c r="H23" s="81">
         <v>18</v>
       </c>
-      <c r="I23" s="80"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="80"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="76" t="s">
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="81"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="78"/>
-      <c r="U23" s="76" t="s">
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="78"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="V23" s="77"/>
-      <c r="W23" s="77"/>
-      <c r="X23" s="77"/>
-      <c r="Y23" s="77"/>
-      <c r="Z23" s="77"/>
-      <c r="AA23" s="77"/>
-      <c r="AB23" s="78"/>
-      <c r="AC23" s="79" t="s">
+      <c r="V23" s="78"/>
+      <c r="W23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="78"/>
+      <c r="Z23" s="78"/>
+      <c r="AA23" s="78"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="AD23" s="80"/>
-      <c r="AE23" s="80"/>
-      <c r="AF23" s="80"/>
-      <c r="AG23" s="80"/>
-      <c r="AH23" s="80"/>
-      <c r="AI23" s="80"/>
-      <c r="AJ23" s="81"/>
+      <c r="AD23" s="81"/>
+      <c r="AE23" s="81"/>
+      <c r="AF23" s="81"/>
+      <c r="AG23" s="81"/>
+      <c r="AH23" s="81"/>
+      <c r="AI23" s="81"/>
+      <c r="AJ23" s="82"/>
       <c r="AK23" s="10"/>
+      <c r="AM23" t="s">
+        <v>198</v>
+      </c>
+      <c r="BR23" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="BS23" s="53"/>
+      <c r="BT23" s="53"/>
+      <c r="BU23" s="53"/>
+      <c r="BV23" s="53"/>
+      <c r="BW23" s="53"/>
+      <c r="BX23" s="53"/>
+      <c r="BY23" s="53"/>
+      <c r="BZ23" s="53">
+        <v>16</v>
+      </c>
+      <c r="CA23" s="53"/>
+      <c r="CB23" s="53"/>
+      <c r="CC23" s="53"/>
+      <c r="CD23" s="53"/>
+      <c r="CE23" s="53"/>
+      <c r="CF23" s="53"/>
+      <c r="CG23" s="53"/>
+      <c r="CH23" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="CI23" s="53"/>
+      <c r="CJ23" s="53"/>
+      <c r="CK23" s="53"/>
+      <c r="CL23" s="53"/>
+      <c r="CM23" s="53"/>
+      <c r="CN23" s="53"/>
+      <c r="CO23" s="53"/>
     </row>
     <row r="24" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
@@ -4472,43 +4613,43 @@
       <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H25" s="80">
+      <c r="H25" s="81">
         <v>18</v>
       </c>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="76" t="s">
+      <c r="I25" s="81"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="77"/>
-      <c r="T25" s="78"/>
-      <c r="U25" s="76" t="s">
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="V25" s="77"/>
-      <c r="W25" s="77"/>
-      <c r="X25" s="77"/>
-      <c r="Y25" s="77"/>
-      <c r="Z25" s="77"/>
-      <c r="AA25" s="77"/>
-      <c r="AB25" s="78"/>
-      <c r="AC25" s="76" t="s">
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="79"/>
+      <c r="AC25" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="AD25" s="77"/>
-      <c r="AE25" s="77"/>
-      <c r="AF25" s="77"/>
-      <c r="AG25" s="77"/>
-      <c r="AH25" s="77"/>
-      <c r="AI25" s="77"/>
-      <c r="AJ25" s="78"/>
+      <c r="AD25" s="78"/>
+      <c r="AE25" s="78"/>
+      <c r="AF25" s="78"/>
+      <c r="AG25" s="78"/>
+      <c r="AH25" s="78"/>
+      <c r="AI25" s="78"/>
+      <c r="AJ25" s="79"/>
       <c r="AK25" s="10"/>
     </row>
     <row r="26" spans="1:102" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4637,43 +4778,43 @@
       <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H28" s="80">
+      <c r="H28" s="81">
         <v>18</v>
       </c>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="76" t="s">
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="N28" s="77"/>
-      <c r="O28" s="77"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="77"/>
-      <c r="R28" s="77"/>
-      <c r="S28" s="77"/>
-      <c r="T28" s="78"/>
-      <c r="U28" s="79" t="s">
+      <c r="N28" s="78"/>
+      <c r="O28" s="78"/>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="79"/>
+      <c r="U28" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="V28" s="80"/>
-      <c r="W28" s="80"/>
-      <c r="X28" s="80"/>
-      <c r="Y28" s="80"/>
-      <c r="Z28" s="80"/>
-      <c r="AA28" s="80"/>
-      <c r="AB28" s="81"/>
-      <c r="AC28" s="82" t="s">
+      <c r="V28" s="81"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="82"/>
+      <c r="AC28" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="AD28" s="83"/>
-      <c r="AE28" s="83"/>
-      <c r="AF28" s="83"/>
-      <c r="AG28" s="83"/>
-      <c r="AH28" s="83"/>
-      <c r="AI28" s="83"/>
-      <c r="AJ28" s="84"/>
+      <c r="AD28" s="84"/>
+      <c r="AE28" s="84"/>
+      <c r="AF28" s="84"/>
+      <c r="AG28" s="84"/>
+      <c r="AH28" s="84"/>
+      <c r="AI28" s="84"/>
+      <c r="AJ28" s="85"/>
       <c r="AK28" s="10"/>
     </row>
     <row r="29" spans="1:102" x14ac:dyDescent="0.25">
@@ -4743,56 +4884,56 @@
       <c r="AB29" s="27">
         <v>1</v>
       </c>
-      <c r="AC29" s="93" t="s">
+      <c r="AC29" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="AD29" s="94"/>
-      <c r="AE29" s="94"/>
-      <c r="AF29" s="94"/>
-      <c r="AG29" s="94"/>
-      <c r="AH29" s="94"/>
-      <c r="AI29" s="94"/>
-      <c r="AJ29" s="95"/>
+      <c r="AD29" s="95"/>
+      <c r="AE29" s="95"/>
+      <c r="AF29" s="95"/>
+      <c r="AG29" s="95"/>
+      <c r="AH29" s="95"/>
+      <c r="AI29" s="95"/>
+      <c r="AJ29" s="96"/>
       <c r="AK29" s="10"/>
     </row>
     <row r="30" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H30" s="77" t="s">
+      <c r="H30" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="76" t="s">
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="77"/>
-      <c r="T30" s="78"/>
-      <c r="U30" s="76" t="s">
+      <c r="N30" s="78"/>
+      <c r="O30" s="78"/>
+      <c r="P30" s="78"/>
+      <c r="Q30" s="78"/>
+      <c r="R30" s="78"/>
+      <c r="S30" s="78"/>
+      <c r="T30" s="79"/>
+      <c r="U30" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="V30" s="77"/>
-      <c r="W30" s="77"/>
-      <c r="X30" s="77"/>
-      <c r="Y30" s="77"/>
-      <c r="Z30" s="77"/>
-      <c r="AA30" s="77"/>
-      <c r="AB30" s="78"/>
-      <c r="AC30" s="79" t="s">
+      <c r="V30" s="78"/>
+      <c r="W30" s="78"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="78"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="78"/>
+      <c r="AB30" s="79"/>
+      <c r="AC30" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="AD30" s="80"/>
-      <c r="AE30" s="80"/>
-      <c r="AF30" s="80"/>
-      <c r="AG30" s="80"/>
-      <c r="AH30" s="80"/>
-      <c r="AI30" s="80"/>
-      <c r="AJ30" s="81"/>
+      <c r="AD30" s="81"/>
+      <c r="AE30" s="81"/>
+      <c r="AF30" s="81"/>
+      <c r="AG30" s="81"/>
+      <c r="AH30" s="81"/>
+      <c r="AI30" s="81"/>
+      <c r="AJ30" s="82"/>
       <c r="AK30" s="10"/>
     </row>
     <row r="31" spans="1:102" x14ac:dyDescent="0.25">
@@ -4889,43 +5030,43 @@
       <c r="AK31" s="10"/>
     </row>
     <row r="32" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H32" s="77" t="s">
+      <c r="H32" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="81"/>
-      <c r="M32" s="87" t="s">
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="N32" s="88"/>
-      <c r="O32" s="88"/>
-      <c r="P32" s="88"/>
-      <c r="Q32" s="88"/>
-      <c r="R32" s="88"/>
-      <c r="S32" s="88"/>
-      <c r="T32" s="89"/>
-      <c r="U32" s="87" t="s">
+      <c r="N32" s="89"/>
+      <c r="O32" s="89"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="90"/>
+      <c r="U32" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="V32" s="88"/>
-      <c r="W32" s="88"/>
-      <c r="X32" s="88"/>
-      <c r="Y32" s="88"/>
-      <c r="Z32" s="88"/>
-      <c r="AA32" s="88"/>
-      <c r="AB32" s="89"/>
-      <c r="AC32" s="90" t="s">
+      <c r="V32" s="89"/>
+      <c r="W32" s="89"/>
+      <c r="X32" s="89"/>
+      <c r="Y32" s="89"/>
+      <c r="Z32" s="89"/>
+      <c r="AA32" s="89"/>
+      <c r="AB32" s="90"/>
+      <c r="AC32" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="AD32" s="91"/>
-      <c r="AE32" s="91"/>
-      <c r="AF32" s="91"/>
-      <c r="AG32" s="91"/>
-      <c r="AH32" s="91"/>
-      <c r="AI32" s="91"/>
-      <c r="AJ32" s="92"/>
+      <c r="AD32" s="92"/>
+      <c r="AE32" s="92"/>
+      <c r="AF32" s="92"/>
+      <c r="AG32" s="92"/>
+      <c r="AH32" s="92"/>
+      <c r="AI32" s="92"/>
+      <c r="AJ32" s="93"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -4935,7 +5076,8 @@
     <sortCondition ref="K3:K15"/>
     <sortCondition ref="L3:L15"/>
   </sortState>
-  <mergeCells count="70">
+  <mergeCells count="78">
+    <mergeCell ref="CH17:CW17"/>
     <mergeCell ref="H32:L32"/>
     <mergeCell ref="AL13:BQ13"/>
     <mergeCell ref="H23:L23"/>
@@ -4974,16 +5116,10 @@
     <mergeCell ref="AL12:AS12"/>
     <mergeCell ref="AL15:BQ15"/>
     <mergeCell ref="AC19:AJ19"/>
-    <mergeCell ref="U18:AB18"/>
-    <mergeCell ref="AL16:AS16"/>
-    <mergeCell ref="AT16:BA16"/>
-    <mergeCell ref="BJ16:BQ16"/>
-    <mergeCell ref="BB16:BI16"/>
     <mergeCell ref="CP15:CW15"/>
     <mergeCell ref="M9:T9"/>
     <mergeCell ref="BR17:BY17"/>
     <mergeCell ref="CP16:CW16"/>
-    <mergeCell ref="CH17:CO17"/>
     <mergeCell ref="BR16:BY16"/>
     <mergeCell ref="BZ16:CG16"/>
     <mergeCell ref="CH16:CO16"/>
@@ -4995,10 +5131,6 @@
     <mergeCell ref="U16:AB16"/>
     <mergeCell ref="U17:AB17"/>
     <mergeCell ref="U14:AB14"/>
-    <mergeCell ref="AT4:BY4"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="BR15:BY15"/>
-    <mergeCell ref="BZ15:CG15"/>
     <mergeCell ref="CH15:CO15"/>
     <mergeCell ref="M7:T7"/>
     <mergeCell ref="AV8:BE8"/>
@@ -5006,6 +5138,23 @@
     <mergeCell ref="M11:T11"/>
     <mergeCell ref="AL11:AS11"/>
     <mergeCell ref="AL14:BA14"/>
+    <mergeCell ref="CH8:CO8"/>
+    <mergeCell ref="AL21:BQ21"/>
+    <mergeCell ref="AT4:BY4"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="BR15:BY15"/>
+    <mergeCell ref="BZ15:CG15"/>
+    <mergeCell ref="U18:AB18"/>
+    <mergeCell ref="AL16:AS16"/>
+    <mergeCell ref="AT16:BA16"/>
+    <mergeCell ref="BJ16:BQ16"/>
+    <mergeCell ref="BB16:BI16"/>
+    <mergeCell ref="BR23:BY23"/>
+    <mergeCell ref="BZ23:CG23"/>
+    <mergeCell ref="CH23:CO23"/>
+    <mergeCell ref="BR21:BY21"/>
+    <mergeCell ref="BZ21:CG21"/>
+    <mergeCell ref="CH21:CO21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Console working and all options choosable (HEX HEX)
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="201">
   <si>
     <t>CAN-Messages</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>Started (1Bit)</t>
+  </si>
+  <si>
+    <t>11 0010 0111 1111 1111 0000 0110 0100 0000 0001 1110 0000</t>
   </si>
 </sst>
 </file>
@@ -1030,88 +1033,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1120,19 +1045,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1160,6 +1085,84 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1466,7 +1469,7 @@
   <dimension ref="A1:CX32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="BH20" sqref="BH20"/>
+      <selection activeCell="AV8" sqref="AV8:BE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,115 +1487,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69" t="s">
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
       <c r="AK1" s="9"/>
-      <c r="AL1" s="69" t="s">
+      <c r="AL1" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69"/>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="69"/>
-      <c r="AR1" s="69"/>
-      <c r="AS1" s="69"/>
-      <c r="AT1" s="69"/>
-      <c r="AU1" s="69"/>
-      <c r="AV1" s="69"/>
-      <c r="AW1" s="69"/>
-      <c r="AX1" s="69"/>
-      <c r="AY1" s="69"/>
-      <c r="AZ1" s="69"/>
-      <c r="BA1" s="69"/>
-      <c r="BB1" s="69"/>
-      <c r="BC1" s="69"/>
-      <c r="BD1" s="69"/>
-      <c r="BE1" s="69"/>
-      <c r="BF1" s="69"/>
-      <c r="BG1" s="69"/>
-      <c r="BH1" s="69"/>
-      <c r="BI1" s="69"/>
-      <c r="BJ1" s="69"/>
-      <c r="BK1" s="69"/>
-      <c r="BL1" s="69"/>
-      <c r="BM1" s="69"/>
-      <c r="BN1" s="69"/>
-      <c r="BO1" s="69"/>
-      <c r="BP1" s="69"/>
-      <c r="BQ1" s="69"/>
-      <c r="BR1" s="69"/>
-      <c r="BS1" s="69"/>
-      <c r="BT1" s="69"/>
-      <c r="BU1" s="69"/>
-      <c r="BV1" s="69"/>
-      <c r="BW1" s="69"/>
-      <c r="BX1" s="69"/>
-      <c r="BY1" s="69"/>
-      <c r="BZ1" s="69"/>
-      <c r="CA1" s="69"/>
-      <c r="CB1" s="69"/>
-      <c r="CC1" s="69"/>
-      <c r="CD1" s="69"/>
-      <c r="CE1" s="69"/>
-      <c r="CF1" s="69"/>
-      <c r="CG1" s="69"/>
-      <c r="CH1" s="69"/>
-      <c r="CI1" s="69"/>
-      <c r="CJ1" s="69"/>
-      <c r="CK1" s="69"/>
-      <c r="CL1" s="69"/>
-      <c r="CM1" s="69"/>
-      <c r="CN1" s="69"/>
-      <c r="CO1" s="69"/>
-      <c r="CP1" s="69"/>
-      <c r="CQ1" s="69"/>
-      <c r="CR1" s="69"/>
-      <c r="CS1" s="69"/>
-      <c r="CT1" s="69"/>
-      <c r="CU1" s="69"/>
-      <c r="CV1" s="69"/>
-      <c r="CW1" s="69"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="75"/>
+      <c r="AP1" s="75"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="75"/>
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="75"/>
+      <c r="AX1" s="75"/>
+      <c r="AY1" s="75"/>
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="75"/>
+      <c r="BC1" s="75"/>
+      <c r="BD1" s="75"/>
+      <c r="BE1" s="75"/>
+      <c r="BF1" s="75"/>
+      <c r="BG1" s="75"/>
+      <c r="BH1" s="75"/>
+      <c r="BI1" s="75"/>
+      <c r="BJ1" s="75"/>
+      <c r="BK1" s="75"/>
+      <c r="BL1" s="75"/>
+      <c r="BM1" s="75"/>
+      <c r="BN1" s="75"/>
+      <c r="BO1" s="75"/>
+      <c r="BP1" s="75"/>
+      <c r="BQ1" s="75"/>
+      <c r="BR1" s="75"/>
+      <c r="BS1" s="75"/>
+      <c r="BT1" s="75"/>
+      <c r="BU1" s="75"/>
+      <c r="BV1" s="75"/>
+      <c r="BW1" s="75"/>
+      <c r="BX1" s="75"/>
+      <c r="BY1" s="75"/>
+      <c r="BZ1" s="75"/>
+      <c r="CA1" s="75"/>
+      <c r="CB1" s="75"/>
+      <c r="CC1" s="75"/>
+      <c r="CD1" s="75"/>
+      <c r="CE1" s="75"/>
+      <c r="CF1" s="75"/>
+      <c r="CG1" s="75"/>
+      <c r="CH1" s="75"/>
+      <c r="CI1" s="75"/>
+      <c r="CJ1" s="75"/>
+      <c r="CK1" s="75"/>
+      <c r="CL1" s="75"/>
+      <c r="CM1" s="75"/>
+      <c r="CN1" s="75"/>
+      <c r="CO1" s="75"/>
+      <c r="CP1" s="75"/>
+      <c r="CQ1" s="75"/>
+      <c r="CR1" s="75"/>
+      <c r="CS1" s="75"/>
+      <c r="CT1" s="75"/>
+      <c r="CU1" s="75"/>
+      <c r="CV1" s="75"/>
+      <c r="CW1" s="75"/>
       <c r="CX1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2129,50 +2132,50 @@
       <c r="AJ4" s="41">
         <v>1</v>
       </c>
-      <c r="AL4" s="59" t="s">
+      <c r="AL4" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="60"/>
-      <c r="AO4" s="60"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="60"/>
-      <c r="AS4" s="60"/>
-      <c r="AT4" s="55" t="s">
+      <c r="AM4" s="78"/>
+      <c r="AN4" s="78"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="95" t="s">
         <v>93</v>
       </c>
-      <c r="AU4" s="55"/>
-      <c r="AV4" s="55"/>
-      <c r="AW4" s="55"/>
-      <c r="AX4" s="55"/>
-      <c r="AY4" s="55"/>
-      <c r="AZ4" s="55"/>
-      <c r="BA4" s="55"/>
-      <c r="BB4" s="55"/>
-      <c r="BC4" s="55"/>
-      <c r="BD4" s="55"/>
-      <c r="BE4" s="55"/>
-      <c r="BF4" s="55"/>
-      <c r="BG4" s="55"/>
-      <c r="BH4" s="55"/>
-      <c r="BI4" s="55"/>
-      <c r="BJ4" s="55"/>
-      <c r="BK4" s="55"/>
-      <c r="BL4" s="55"/>
-      <c r="BM4" s="55"/>
-      <c r="BN4" s="55"/>
-      <c r="BO4" s="55"/>
-      <c r="BP4" s="55"/>
-      <c r="BQ4" s="55"/>
-      <c r="BR4" s="55"/>
-      <c r="BS4" s="55"/>
-      <c r="BT4" s="55"/>
-      <c r="BU4" s="55"/>
-      <c r="BV4" s="55"/>
-      <c r="BW4" s="55"/>
-      <c r="BX4" s="55"/>
-      <c r="BY4" s="55"/>
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="95"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="95"/>
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="95"/>
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="95"/>
+      <c r="BG4" s="95"/>
+      <c r="BH4" s="95"/>
+      <c r="BI4" s="95"/>
+      <c r="BJ4" s="95"/>
+      <c r="BK4" s="95"/>
+      <c r="BL4" s="95"/>
+      <c r="BM4" s="95"/>
+      <c r="BN4" s="95"/>
+      <c r="BO4" s="95"/>
+      <c r="BP4" s="95"/>
+      <c r="BQ4" s="95"/>
+      <c r="BR4" s="95"/>
+      <c r="BS4" s="95"/>
+      <c r="BT4" s="95"/>
+      <c r="BU4" s="95"/>
+      <c r="BV4" s="95"/>
+      <c r="BW4" s="95"/>
+      <c r="BX4" s="95"/>
+      <c r="BY4" s="95"/>
       <c r="CG4" s="18"/>
       <c r="CI4" s="3"/>
       <c r="CO4" s="18"/>
@@ -2502,16 +2505,16 @@
       <c r="L7" s="12">
         <v>0</v>
       </c>
-      <c r="M7" s="56" t="s">
+      <c r="M7" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="86"/>
+      <c r="T7" s="86"/>
       <c r="U7" s="14">
         <v>0</v>
       </c>
@@ -2560,16 +2563,16 @@
       <c r="AJ7" s="41">
         <v>1</v>
       </c>
-      <c r="AL7" s="59" t="s">
+      <c r="AL7" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="AM7" s="60"/>
-      <c r="AN7" s="60"/>
-      <c r="AO7" s="60"/>
-      <c r="AP7" s="60"/>
-      <c r="AQ7" s="60"/>
-      <c r="AR7" s="60"/>
-      <c r="AS7" s="60"/>
+      <c r="AM7" s="78"/>
+      <c r="AN7" s="78"/>
+      <c r="AO7" s="78"/>
+      <c r="AP7" s="78"/>
+      <c r="AQ7" s="78"/>
+      <c r="AR7" s="78"/>
+      <c r="AS7" s="78"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="18"/>
       <c r="BE7" s="3"/>
@@ -2620,16 +2623,16 @@
       <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86"/>
       <c r="U8" s="14">
         <v>0</v>
       </c>
@@ -2678,72 +2681,72 @@
       <c r="AJ8" s="41">
         <v>1</v>
       </c>
-      <c r="AL8" s="73" t="s">
+      <c r="AL8" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="AM8" s="74"/>
-      <c r="AN8" s="74"/>
-      <c r="AO8" s="74"/>
-      <c r="AP8" s="74"/>
-      <c r="AQ8" s="74"/>
-      <c r="AR8" s="74"/>
-      <c r="AS8" s="74"/>
-      <c r="AT8" s="74"/>
-      <c r="AU8" s="74"/>
-      <c r="AV8" s="57" t="s">
+      <c r="AM8" s="82"/>
+      <c r="AN8" s="82"/>
+      <c r="AO8" s="82"/>
+      <c r="AP8" s="82"/>
+      <c r="AQ8" s="82"/>
+      <c r="AR8" s="82"/>
+      <c r="AS8" s="82"/>
+      <c r="AT8" s="82"/>
+      <c r="AU8" s="82"/>
+      <c r="AV8" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="AW8" s="57"/>
-      <c r="AX8" s="57"/>
-      <c r="AY8" s="57"/>
-      <c r="AZ8" s="57"/>
-      <c r="BA8" s="57"/>
-      <c r="BB8" s="57"/>
-      <c r="BC8" s="57"/>
-      <c r="BD8" s="57"/>
-      <c r="BE8" s="57"/>
-      <c r="BF8" s="58" t="s">
+      <c r="AW8" s="92"/>
+      <c r="AX8" s="92"/>
+      <c r="AY8" s="92"/>
+      <c r="AZ8" s="92"/>
+      <c r="BA8" s="92"/>
+      <c r="BB8" s="92"/>
+      <c r="BC8" s="92"/>
+      <c r="BD8" s="92"/>
+      <c r="BE8" s="92"/>
+      <c r="BF8" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="BG8" s="58"/>
-      <c r="BH8" s="58"/>
-      <c r="BI8" s="58"/>
-      <c r="BJ8" s="58"/>
-      <c r="BK8" s="58"/>
-      <c r="BL8" s="58"/>
-      <c r="BM8" s="58"/>
-      <c r="BN8" s="58"/>
-      <c r="BO8" s="58"/>
-      <c r="BP8" s="58"/>
-      <c r="BQ8" s="58"/>
-      <c r="BR8" s="75" t="s">
+      <c r="BG8" s="53"/>
+      <c r="BH8" s="53"/>
+      <c r="BI8" s="53"/>
+      <c r="BJ8" s="53"/>
+      <c r="BK8" s="53"/>
+      <c r="BL8" s="53"/>
+      <c r="BM8" s="53"/>
+      <c r="BN8" s="53"/>
+      <c r="BO8" s="53"/>
+      <c r="BP8" s="53"/>
+      <c r="BQ8" s="53"/>
+      <c r="BR8" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="BS8" s="75"/>
-      <c r="BT8" s="75"/>
-      <c r="BU8" s="75"/>
-      <c r="BV8" s="75"/>
-      <c r="BW8" s="75"/>
-      <c r="BX8" s="75"/>
-      <c r="BY8" s="75"/>
-      <c r="BZ8" s="75"/>
-      <c r="CA8" s="75"/>
-      <c r="CB8" s="75"/>
-      <c r="CC8" s="75"/>
-      <c r="CD8" s="75"/>
-      <c r="CE8" s="75"/>
-      <c r="CF8" s="75"/>
-      <c r="CG8" s="75"/>
-      <c r="CH8" s="60" t="s">
+      <c r="BS8" s="83"/>
+      <c r="BT8" s="83"/>
+      <c r="BU8" s="83"/>
+      <c r="BV8" s="83"/>
+      <c r="BW8" s="83"/>
+      <c r="BX8" s="83"/>
+      <c r="BY8" s="83"/>
+      <c r="BZ8" s="83"/>
+      <c r="CA8" s="83"/>
+      <c r="CB8" s="83"/>
+      <c r="CC8" s="83"/>
+      <c r="CD8" s="83"/>
+      <c r="CE8" s="83"/>
+      <c r="CF8" s="83"/>
+      <c r="CG8" s="83"/>
+      <c r="CH8" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="CI8" s="60"/>
-      <c r="CJ8" s="60"/>
-      <c r="CK8" s="60"/>
-      <c r="CL8" s="60"/>
-      <c r="CM8" s="60"/>
-      <c r="CN8" s="60"/>
-      <c r="CO8" s="60"/>
+      <c r="CI8" s="78"/>
+      <c r="CJ8" s="78"/>
+      <c r="CK8" s="78"/>
+      <c r="CL8" s="78"/>
+      <c r="CM8" s="78"/>
+      <c r="CN8" s="78"/>
+      <c r="CO8" s="78"/>
       <c r="CS8" s="3"/>
       <c r="CW8" s="18"/>
       <c r="CX8">
@@ -2785,16 +2788,16 @@
       <c r="L9" s="34">
         <v>0</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="M9" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="56"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
       <c r="U9" s="35">
         <v>0</v>
       </c>
@@ -3096,16 +3099,16 @@
       <c r="L11" s="12">
         <v>0</v>
       </c>
-      <c r="M11" s="56" t="s">
+      <c r="M11" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="56"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
       <c r="U11" s="14">
         <v>0</v>
       </c>
@@ -3154,16 +3157,16 @@
       <c r="AJ11" s="41">
         <v>1</v>
       </c>
-      <c r="AL11" s="59" t="s">
+      <c r="AL11" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="AM11" s="60"/>
-      <c r="AN11" s="60"/>
-      <c r="AO11" s="60"/>
-      <c r="AP11" s="60"/>
-      <c r="AQ11" s="60"/>
-      <c r="AR11" s="60"/>
-      <c r="AS11" s="60"/>
+      <c r="AM11" s="78"/>
+      <c r="AN11" s="78"/>
+      <c r="AO11" s="78"/>
+      <c r="AP11" s="78"/>
+      <c r="AQ11" s="78"/>
+      <c r="AR11" s="78"/>
+      <c r="AS11" s="78"/>
       <c r="AU11" s="3"/>
       <c r="BA11" s="18"/>
       <c r="BE11" s="3"/>
@@ -3286,16 +3289,16 @@
       <c r="AJ12" s="48">
         <v>1</v>
       </c>
-      <c r="AL12" s="59" t="s">
+      <c r="AL12" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="AM12" s="60"/>
-      <c r="AN12" s="60"/>
-      <c r="AO12" s="60"/>
-      <c r="AP12" s="60"/>
-      <c r="AQ12" s="60"/>
-      <c r="AR12" s="60"/>
-      <c r="AS12" s="60"/>
+      <c r="AM12" s="78"/>
+      <c r="AN12" s="78"/>
+      <c r="AO12" s="78"/>
+      <c r="AP12" s="78"/>
+      <c r="AQ12" s="78"/>
+      <c r="AR12" s="78"/>
+      <c r="AS12" s="78"/>
       <c r="AU12" s="3"/>
       <c r="BA12" s="18"/>
       <c r="BE12" s="3"/>
@@ -3420,40 +3423,40 @@
         <v>1</v>
       </c>
       <c r="AK13" s="49"/>
-      <c r="AL13" s="86" t="s">
+      <c r="AL13" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="AM13" s="87"/>
-      <c r="AN13" s="87"/>
-      <c r="AO13" s="87"/>
-      <c r="AP13" s="87"/>
-      <c r="AQ13" s="87"/>
-      <c r="AR13" s="87"/>
-      <c r="AS13" s="87"/>
-      <c r="AT13" s="87"/>
-      <c r="AU13" s="87"/>
-      <c r="AV13" s="87"/>
-      <c r="AW13" s="87"/>
-      <c r="AX13" s="87"/>
-      <c r="AY13" s="87"/>
-      <c r="AZ13" s="87"/>
-      <c r="BA13" s="87"/>
-      <c r="BB13" s="87"/>
-      <c r="BC13" s="87"/>
-      <c r="BD13" s="87"/>
-      <c r="BE13" s="87"/>
-      <c r="BF13" s="87"/>
-      <c r="BG13" s="87"/>
-      <c r="BH13" s="87"/>
-      <c r="BI13" s="87"/>
-      <c r="BJ13" s="87"/>
-      <c r="BK13" s="87"/>
-      <c r="BL13" s="87"/>
-      <c r="BM13" s="87"/>
-      <c r="BN13" s="87"/>
-      <c r="BO13" s="87"/>
-      <c r="BP13" s="87"/>
-      <c r="BQ13" s="87"/>
+      <c r="AM13" s="58"/>
+      <c r="AN13" s="58"/>
+      <c r="AO13" s="58"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="58"/>
+      <c r="AR13" s="58"/>
+      <c r="AS13" s="58"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="58"/>
+      <c r="AV13" s="58"/>
+      <c r="AW13" s="58"/>
+      <c r="AX13" s="58"/>
+      <c r="AY13" s="58"/>
+      <c r="AZ13" s="58"/>
+      <c r="BA13" s="58"/>
+      <c r="BB13" s="58"/>
+      <c r="BC13" s="58"/>
+      <c r="BD13" s="58"/>
+      <c r="BE13" s="58"/>
+      <c r="BF13" s="58"/>
+      <c r="BG13" s="58"/>
+      <c r="BH13" s="58"/>
+      <c r="BI13" s="58"/>
+      <c r="BJ13" s="58"/>
+      <c r="BK13" s="58"/>
+      <c r="BL13" s="58"/>
+      <c r="BM13" s="58"/>
+      <c r="BN13" s="58"/>
+      <c r="BO13" s="58"/>
+      <c r="BP13" s="58"/>
+      <c r="BQ13" s="58"/>
       <c r="BR13" s="23"/>
       <c r="BS13" s="23"/>
       <c r="BT13" s="23"/>
@@ -3548,16 +3551,16 @@
       <c r="T14" s="15">
         <v>1</v>
       </c>
-      <c r="U14" s="64" t="s">
+      <c r="U14" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="64"/>
-      <c r="Y14" s="64"/>
-      <c r="Z14" s="64"/>
-      <c r="AA14" s="64"/>
-      <c r="AB14" s="64"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="89"/>
       <c r="AC14" s="13">
         <v>0</v>
       </c>
@@ -3582,50 +3585,50 @@
       <c r="AJ14" s="41">
         <v>1</v>
       </c>
-      <c r="AL14" s="59" t="s">
+      <c r="AL14" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="AM14" s="61"/>
-      <c r="AN14" s="61"/>
-      <c r="AO14" s="61"/>
-      <c r="AP14" s="61"/>
-      <c r="AQ14" s="61"/>
-      <c r="AR14" s="61"/>
-      <c r="AS14" s="61"/>
-      <c r="AT14" s="61"/>
-      <c r="AU14" s="61"/>
-      <c r="AV14" s="61"/>
-      <c r="AW14" s="61"/>
-      <c r="AX14" s="61"/>
-      <c r="AY14" s="61"/>
-      <c r="AZ14" s="61"/>
-      <c r="BA14" s="61"/>
-      <c r="BB14" s="58" t="s">
+      <c r="AM14" s="93"/>
+      <c r="AN14" s="93"/>
+      <c r="AO14" s="93"/>
+      <c r="AP14" s="93"/>
+      <c r="AQ14" s="93"/>
+      <c r="AR14" s="93"/>
+      <c r="AS14" s="93"/>
+      <c r="AT14" s="93"/>
+      <c r="AU14" s="93"/>
+      <c r="AV14" s="93"/>
+      <c r="AW14" s="93"/>
+      <c r="AX14" s="93"/>
+      <c r="AY14" s="93"/>
+      <c r="AZ14" s="93"/>
+      <c r="BA14" s="93"/>
+      <c r="BB14" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="BC14" s="58"/>
-      <c r="BD14" s="58"/>
-      <c r="BE14" s="58"/>
-      <c r="BF14" s="58"/>
-      <c r="BG14" s="58"/>
-      <c r="BH14" s="58"/>
-      <c r="BI14" s="58"/>
-      <c r="BJ14" s="58"/>
-      <c r="BK14" s="58"/>
-      <c r="BL14" s="58"/>
-      <c r="BM14" s="58"/>
-      <c r="BN14" s="58"/>
-      <c r="BO14" s="58"/>
-      <c r="BP14" s="58"/>
-      <c r="BQ14" s="58"/>
-      <c r="BR14" s="58"/>
-      <c r="BS14" s="58"/>
-      <c r="BT14" s="58"/>
-      <c r="BU14" s="58"/>
-      <c r="BV14" s="58"/>
-      <c r="BW14" s="58"/>
-      <c r="BX14" s="58"/>
-      <c r="BY14" s="58"/>
+      <c r="BC14" s="53"/>
+      <c r="BD14" s="53"/>
+      <c r="BE14" s="53"/>
+      <c r="BF14" s="53"/>
+      <c r="BG14" s="53"/>
+      <c r="BH14" s="53"/>
+      <c r="BI14" s="53"/>
+      <c r="BJ14" s="53"/>
+      <c r="BK14" s="53"/>
+      <c r="BL14" s="53"/>
+      <c r="BM14" s="53"/>
+      <c r="BN14" s="53"/>
+      <c r="BO14" s="53"/>
+      <c r="BP14" s="53"/>
+      <c r="BQ14" s="53"/>
+      <c r="BR14" s="53"/>
+      <c r="BS14" s="53"/>
+      <c r="BT14" s="53"/>
+      <c r="BU14" s="53"/>
+      <c r="BV14" s="53"/>
+      <c r="BW14" s="53"/>
+      <c r="BX14" s="53"/>
+      <c r="BY14" s="53"/>
       <c r="CG14" s="18"/>
       <c r="CI14" s="3"/>
       <c r="CO14" s="18"/>
@@ -3696,100 +3699,100 @@
       <c r="T15" s="15">
         <v>1</v>
       </c>
-      <c r="U15" s="64" t="s">
+      <c r="U15" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="V15" s="64"/>
-      <c r="W15" s="64"/>
-      <c r="X15" s="64"/>
-      <c r="Y15" s="64"/>
-      <c r="Z15" s="64"/>
-      <c r="AA15" s="64"/>
-      <c r="AB15" s="64"/>
-      <c r="AC15" s="65" t="s">
+      <c r="V15" s="89"/>
+      <c r="W15" s="89"/>
+      <c r="X15" s="89"/>
+      <c r="Y15" s="89"/>
+      <c r="Z15" s="89"/>
+      <c r="AA15" s="89"/>
+      <c r="AB15" s="89"/>
+      <c r="AC15" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="AD15" s="66"/>
-      <c r="AE15" s="66"/>
-      <c r="AF15" s="66"/>
-      <c r="AG15" s="66"/>
-      <c r="AH15" s="66"/>
-      <c r="AI15" s="66"/>
-      <c r="AJ15" s="66"/>
-      <c r="AL15" s="59" t="s">
+      <c r="AD15" s="91"/>
+      <c r="AE15" s="91"/>
+      <c r="AF15" s="91"/>
+      <c r="AG15" s="91"/>
+      <c r="AH15" s="91"/>
+      <c r="AI15" s="91"/>
+      <c r="AJ15" s="91"/>
+      <c r="AL15" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="AM15" s="60"/>
-      <c r="AN15" s="60"/>
-      <c r="AO15" s="60"/>
-      <c r="AP15" s="60"/>
-      <c r="AQ15" s="60"/>
-      <c r="AR15" s="60"/>
-      <c r="AS15" s="60"/>
-      <c r="AT15" s="60"/>
-      <c r="AU15" s="60"/>
-      <c r="AV15" s="60"/>
-      <c r="AW15" s="60"/>
-      <c r="AX15" s="60"/>
-      <c r="AY15" s="60"/>
-      <c r="AZ15" s="60"/>
-      <c r="BA15" s="60"/>
-      <c r="BB15" s="60"/>
-      <c r="BC15" s="60"/>
-      <c r="BD15" s="60"/>
-      <c r="BE15" s="60"/>
-      <c r="BF15" s="60"/>
-      <c r="BG15" s="60"/>
-      <c r="BH15" s="60"/>
-      <c r="BI15" s="60"/>
-      <c r="BJ15" s="60"/>
-      <c r="BK15" s="60"/>
-      <c r="BL15" s="60"/>
-      <c r="BM15" s="60"/>
-      <c r="BN15" s="60"/>
-      <c r="BO15" s="60"/>
-      <c r="BP15" s="60"/>
-      <c r="BQ15" s="60"/>
-      <c r="BR15" s="53" t="s">
+      <c r="AM15" s="78"/>
+      <c r="AN15" s="78"/>
+      <c r="AO15" s="78"/>
+      <c r="AP15" s="78"/>
+      <c r="AQ15" s="78"/>
+      <c r="AR15" s="78"/>
+      <c r="AS15" s="78"/>
+      <c r="AT15" s="78"/>
+      <c r="AU15" s="78"/>
+      <c r="AV15" s="78"/>
+      <c r="AW15" s="78"/>
+      <c r="AX15" s="78"/>
+      <c r="AY15" s="78"/>
+      <c r="AZ15" s="78"/>
+      <c r="BA15" s="78"/>
+      <c r="BB15" s="78"/>
+      <c r="BC15" s="78"/>
+      <c r="BD15" s="78"/>
+      <c r="BE15" s="78"/>
+      <c r="BF15" s="78"/>
+      <c r="BG15" s="78"/>
+      <c r="BH15" s="78"/>
+      <c r="BI15" s="78"/>
+      <c r="BJ15" s="78"/>
+      <c r="BK15" s="78"/>
+      <c r="BL15" s="78"/>
+      <c r="BM15" s="78"/>
+      <c r="BN15" s="78"/>
+      <c r="BO15" s="78"/>
+      <c r="BP15" s="78"/>
+      <c r="BQ15" s="78"/>
+      <c r="BR15" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="BS15" s="53"/>
-      <c r="BT15" s="53"/>
-      <c r="BU15" s="53"/>
-      <c r="BV15" s="53"/>
-      <c r="BW15" s="53"/>
-      <c r="BX15" s="53"/>
-      <c r="BY15" s="53"/>
-      <c r="BZ15" s="53" t="s">
+      <c r="BS15" s="85"/>
+      <c r="BT15" s="85"/>
+      <c r="BU15" s="85"/>
+      <c r="BV15" s="85"/>
+      <c r="BW15" s="85"/>
+      <c r="BX15" s="85"/>
+      <c r="BY15" s="85"/>
+      <c r="BZ15" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="CA15" s="53"/>
-      <c r="CB15" s="53"/>
-      <c r="CC15" s="53"/>
-      <c r="CD15" s="53"/>
-      <c r="CE15" s="53"/>
-      <c r="CF15" s="53"/>
-      <c r="CG15" s="53"/>
-      <c r="CH15" s="53" t="s">
+      <c r="CA15" s="85"/>
+      <c r="CB15" s="85"/>
+      <c r="CC15" s="85"/>
+      <c r="CD15" s="85"/>
+      <c r="CE15" s="85"/>
+      <c r="CF15" s="85"/>
+      <c r="CG15" s="85"/>
+      <c r="CH15" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="CI15" s="53"/>
-      <c r="CJ15" s="53"/>
-      <c r="CK15" s="53"/>
-      <c r="CL15" s="53"/>
-      <c r="CM15" s="53"/>
-      <c r="CN15" s="53"/>
-      <c r="CO15" s="53"/>
-      <c r="CP15" s="53" t="s">
+      <c r="CI15" s="85"/>
+      <c r="CJ15" s="85"/>
+      <c r="CK15" s="85"/>
+      <c r="CL15" s="85"/>
+      <c r="CM15" s="85"/>
+      <c r="CN15" s="85"/>
+      <c r="CO15" s="85"/>
+      <c r="CP15" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="CQ15" s="53"/>
-      <c r="CR15" s="53"/>
-      <c r="CS15" s="53"/>
-      <c r="CT15" s="53"/>
-      <c r="CU15" s="53"/>
-      <c r="CV15" s="53"/>
-      <c r="CW15" s="53"/>
+      <c r="CQ15" s="85"/>
+      <c r="CR15" s="85"/>
+      <c r="CS15" s="85"/>
+      <c r="CT15" s="85"/>
+      <c r="CU15" s="85"/>
+      <c r="CV15" s="85"/>
+      <c r="CW15" s="85"/>
       <c r="CX15" s="31" t="s">
         <v>121</v>
       </c>
@@ -3852,106 +3855,106 @@
       <c r="T16" s="15">
         <v>1</v>
       </c>
-      <c r="U16" s="64" t="s">
+      <c r="U16" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
-      <c r="X16" s="64"/>
-      <c r="Y16" s="64"/>
-      <c r="Z16" s="64"/>
-      <c r="AA16" s="64"/>
-      <c r="AB16" s="64"/>
-      <c r="AC16" s="65" t="s">
+      <c r="V16" s="89"/>
+      <c r="W16" s="89"/>
+      <c r="X16" s="89"/>
+      <c r="Y16" s="89"/>
+      <c r="Z16" s="89"/>
+      <c r="AA16" s="89"/>
+      <c r="AB16" s="89"/>
+      <c r="AC16" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="66"/>
-      <c r="AG16" s="66"/>
-      <c r="AH16" s="66"/>
-      <c r="AI16" s="66"/>
-      <c r="AJ16" s="66"/>
-      <c r="AL16" s="53" t="s">
+      <c r="AD16" s="91"/>
+      <c r="AE16" s="91"/>
+      <c r="AF16" s="91"/>
+      <c r="AG16" s="91"/>
+      <c r="AH16" s="91"/>
+      <c r="AI16" s="91"/>
+      <c r="AJ16" s="91"/>
+      <c r="AL16" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="AM16" s="53"/>
-      <c r="AN16" s="53"/>
-      <c r="AO16" s="53"/>
-      <c r="AP16" s="53"/>
-      <c r="AQ16" s="53"/>
-      <c r="AR16" s="53"/>
-      <c r="AS16" s="53"/>
-      <c r="AT16" s="53" t="s">
+      <c r="AM16" s="85"/>
+      <c r="AN16" s="85"/>
+      <c r="AO16" s="85"/>
+      <c r="AP16" s="85"/>
+      <c r="AQ16" s="85"/>
+      <c r="AR16" s="85"/>
+      <c r="AS16" s="85"/>
+      <c r="AT16" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="AU16" s="53"/>
-      <c r="AV16" s="53"/>
-      <c r="AW16" s="53"/>
-      <c r="AX16" s="53"/>
-      <c r="AY16" s="53"/>
-      <c r="AZ16" s="53"/>
-      <c r="BA16" s="53"/>
-      <c r="BB16" s="53" t="s">
+      <c r="AU16" s="85"/>
+      <c r="AV16" s="85"/>
+      <c r="AW16" s="85"/>
+      <c r="AX16" s="85"/>
+      <c r="AY16" s="85"/>
+      <c r="AZ16" s="85"/>
+      <c r="BA16" s="85"/>
+      <c r="BB16" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="BC16" s="53"/>
-      <c r="BD16" s="53"/>
-      <c r="BE16" s="53"/>
-      <c r="BF16" s="53"/>
-      <c r="BG16" s="53"/>
-      <c r="BH16" s="53"/>
-      <c r="BI16" s="53"/>
-      <c r="BJ16" s="53" t="s">
+      <c r="BC16" s="85"/>
+      <c r="BD16" s="85"/>
+      <c r="BE16" s="85"/>
+      <c r="BF16" s="85"/>
+      <c r="BG16" s="85"/>
+      <c r="BH16" s="85"/>
+      <c r="BI16" s="85"/>
+      <c r="BJ16" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="BK16" s="53"/>
-      <c r="BL16" s="53"/>
-      <c r="BM16" s="53"/>
-      <c r="BN16" s="53"/>
-      <c r="BO16" s="53"/>
-      <c r="BP16" s="53"/>
-      <c r="BQ16" s="53"/>
-      <c r="BR16" s="53" t="s">
+      <c r="BK16" s="85"/>
+      <c r="BL16" s="85"/>
+      <c r="BM16" s="85"/>
+      <c r="BN16" s="85"/>
+      <c r="BO16" s="85"/>
+      <c r="BP16" s="85"/>
+      <c r="BQ16" s="85"/>
+      <c r="BR16" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="BS16" s="53"/>
-      <c r="BT16" s="53"/>
-      <c r="BU16" s="53"/>
-      <c r="BV16" s="53"/>
-      <c r="BW16" s="53"/>
-      <c r="BX16" s="53"/>
-      <c r="BY16" s="53"/>
-      <c r="BZ16" s="53" t="s">
+      <c r="BS16" s="85"/>
+      <c r="BT16" s="85"/>
+      <c r="BU16" s="85"/>
+      <c r="BV16" s="85"/>
+      <c r="BW16" s="85"/>
+      <c r="BX16" s="85"/>
+      <c r="BY16" s="85"/>
+      <c r="BZ16" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="CA16" s="53"/>
-      <c r="CB16" s="53"/>
-      <c r="CC16" s="53"/>
-      <c r="CD16" s="53"/>
-      <c r="CE16" s="53"/>
-      <c r="CF16" s="53"/>
-      <c r="CG16" s="53"/>
-      <c r="CH16" s="53" t="s">
+      <c r="CA16" s="85"/>
+      <c r="CB16" s="85"/>
+      <c r="CC16" s="85"/>
+      <c r="CD16" s="85"/>
+      <c r="CE16" s="85"/>
+      <c r="CF16" s="85"/>
+      <c r="CG16" s="85"/>
+      <c r="CH16" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="CI16" s="53"/>
-      <c r="CJ16" s="53"/>
-      <c r="CK16" s="53"/>
-      <c r="CL16" s="53"/>
-      <c r="CM16" s="53"/>
-      <c r="CN16" s="53"/>
-      <c r="CO16" s="53"/>
-      <c r="CP16" s="53" t="s">
+      <c r="CI16" s="85"/>
+      <c r="CJ16" s="85"/>
+      <c r="CK16" s="85"/>
+      <c r="CL16" s="85"/>
+      <c r="CM16" s="85"/>
+      <c r="CN16" s="85"/>
+      <c r="CO16" s="85"/>
+      <c r="CP16" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="CQ16" s="53"/>
-      <c r="CR16" s="53"/>
-      <c r="CS16" s="53"/>
-      <c r="CT16" s="53"/>
-      <c r="CU16" s="53"/>
-      <c r="CV16" s="53"/>
-      <c r="CW16" s="53"/>
+      <c r="CQ16" s="85"/>
+      <c r="CR16" s="85"/>
+      <c r="CS16" s="85"/>
+      <c r="CT16" s="85"/>
+      <c r="CU16" s="85"/>
+      <c r="CV16" s="85"/>
+      <c r="CW16" s="85"/>
       <c r="CX16" s="21" t="s">
         <v>122</v>
       </c>
@@ -4014,98 +4017,98 @@
       <c r="T17" s="15">
         <v>1</v>
       </c>
-      <c r="U17" s="64" t="s">
+      <c r="U17" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="64"/>
-      <c r="Y17" s="64"/>
-      <c r="Z17" s="64"/>
-      <c r="AA17" s="64"/>
-      <c r="AB17" s="64"/>
-      <c r="AC17" s="65" t="s">
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="89"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="89"/>
+      <c r="AB17" s="89"/>
+      <c r="AC17" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="AD17" s="66"/>
-      <c r="AE17" s="66"/>
-      <c r="AF17" s="66"/>
-      <c r="AG17" s="66"/>
-      <c r="AH17" s="66"/>
-      <c r="AI17" s="66"/>
-      <c r="AJ17" s="66"/>
-      <c r="AL17" s="59" t="s">
+      <c r="AD17" s="91"/>
+      <c r="AE17" s="91"/>
+      <c r="AF17" s="91"/>
+      <c r="AG17" s="91"/>
+      <c r="AH17" s="91"/>
+      <c r="AI17" s="91"/>
+      <c r="AJ17" s="91"/>
+      <c r="AL17" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="AM17" s="60"/>
-      <c r="AN17" s="60"/>
-      <c r="AO17" s="60"/>
-      <c r="AP17" s="60"/>
-      <c r="AQ17" s="60"/>
-      <c r="AR17" s="60"/>
-      <c r="AS17" s="60"/>
-      <c r="AT17" s="60"/>
-      <c r="AU17" s="60"/>
-      <c r="AV17" s="60"/>
-      <c r="AW17" s="60"/>
-      <c r="AX17" s="60"/>
-      <c r="AY17" s="60"/>
-      <c r="AZ17" s="60"/>
-      <c r="BA17" s="60"/>
-      <c r="BB17" s="60"/>
-      <c r="BC17" s="60"/>
-      <c r="BD17" s="60"/>
-      <c r="BE17" s="60"/>
-      <c r="BF17" s="60"/>
-      <c r="BG17" s="60"/>
-      <c r="BH17" s="60"/>
-      <c r="BI17" s="60"/>
-      <c r="BJ17" s="60"/>
-      <c r="BK17" s="60"/>
-      <c r="BL17" s="60"/>
-      <c r="BM17" s="60"/>
-      <c r="BN17" s="60"/>
-      <c r="BO17" s="60"/>
-      <c r="BP17" s="60"/>
-      <c r="BQ17" s="60"/>
-      <c r="BR17" s="62" t="s">
+      <c r="AM17" s="78"/>
+      <c r="AN17" s="78"/>
+      <c r="AO17" s="78"/>
+      <c r="AP17" s="78"/>
+      <c r="AQ17" s="78"/>
+      <c r="AR17" s="78"/>
+      <c r="AS17" s="78"/>
+      <c r="AT17" s="78"/>
+      <c r="AU17" s="78"/>
+      <c r="AV17" s="78"/>
+      <c r="AW17" s="78"/>
+      <c r="AX17" s="78"/>
+      <c r="AY17" s="78"/>
+      <c r="AZ17" s="78"/>
+      <c r="BA17" s="78"/>
+      <c r="BB17" s="78"/>
+      <c r="BC17" s="78"/>
+      <c r="BD17" s="78"/>
+      <c r="BE17" s="78"/>
+      <c r="BF17" s="78"/>
+      <c r="BG17" s="78"/>
+      <c r="BH17" s="78"/>
+      <c r="BI17" s="78"/>
+      <c r="BJ17" s="78"/>
+      <c r="BK17" s="78"/>
+      <c r="BL17" s="78"/>
+      <c r="BM17" s="78"/>
+      <c r="BN17" s="78"/>
+      <c r="BO17" s="78"/>
+      <c r="BP17" s="78"/>
+      <c r="BQ17" s="78"/>
+      <c r="BR17" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="BS17" s="62"/>
-      <c r="BT17" s="62"/>
-      <c r="BU17" s="62"/>
-      <c r="BV17" s="62"/>
-      <c r="BW17" s="62"/>
-      <c r="BX17" s="62"/>
-      <c r="BY17" s="62"/>
-      <c r="BZ17" s="63" t="s">
+      <c r="BS17" s="87"/>
+      <c r="BT17" s="87"/>
+      <c r="BU17" s="87"/>
+      <c r="BV17" s="87"/>
+      <c r="BW17" s="87"/>
+      <c r="BX17" s="87"/>
+      <c r="BY17" s="87"/>
+      <c r="BZ17" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="CA17" s="63"/>
-      <c r="CB17" s="63"/>
-      <c r="CC17" s="63"/>
-      <c r="CD17" s="63"/>
-      <c r="CE17" s="63"/>
-      <c r="CF17" s="63"/>
-      <c r="CG17" s="63"/>
-      <c r="CH17" s="58" t="s">
+      <c r="CA17" s="88"/>
+      <c r="CB17" s="88"/>
+      <c r="CC17" s="88"/>
+      <c r="CD17" s="88"/>
+      <c r="CE17" s="88"/>
+      <c r="CF17" s="88"/>
+      <c r="CG17" s="88"/>
+      <c r="CH17" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="CI17" s="58"/>
-      <c r="CJ17" s="58"/>
-      <c r="CK17" s="58"/>
-      <c r="CL17" s="58"/>
-      <c r="CM17" s="58"/>
-      <c r="CN17" s="58"/>
-      <c r="CO17" s="58"/>
-      <c r="CP17" s="58"/>
-      <c r="CQ17" s="58"/>
-      <c r="CR17" s="58"/>
-      <c r="CS17" s="58"/>
-      <c r="CT17" s="58"/>
-      <c r="CU17" s="58"/>
-      <c r="CV17" s="58"/>
-      <c r="CW17" s="58"/>
+      <c r="CI17" s="53"/>
+      <c r="CJ17" s="53"/>
+      <c r="CK17" s="53"/>
+      <c r="CL17" s="53"/>
+      <c r="CM17" s="53"/>
+      <c r="CN17" s="53"/>
+      <c r="CO17" s="53"/>
+      <c r="CP17" s="53"/>
+      <c r="CQ17" s="53"/>
+      <c r="CR17" s="53"/>
+      <c r="CS17" s="53"/>
+      <c r="CT17" s="53"/>
+      <c r="CU17" s="53"/>
+      <c r="CV17" s="53"/>
+      <c r="CW17" s="53"/>
       <c r="CX17">
         <v>7</v>
       </c>
@@ -4168,16 +4171,16 @@
       <c r="T18" s="39">
         <v>1</v>
       </c>
-      <c r="U18" s="67" t="s">
+      <c r="U18" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="V18" s="67"/>
-      <c r="W18" s="67"/>
-      <c r="X18" s="67"/>
-      <c r="Y18" s="67"/>
-      <c r="Z18" s="67"/>
-      <c r="AA18" s="67"/>
-      <c r="AB18" s="67"/>
+      <c r="V18" s="96"/>
+      <c r="W18" s="96"/>
+      <c r="X18" s="96"/>
+      <c r="Y18" s="96"/>
+      <c r="Z18" s="96"/>
+      <c r="AA18" s="96"/>
+      <c r="AB18" s="96"/>
       <c r="AC18" s="13">
         <v>0</v>
       </c>
@@ -4221,42 +4224,42 @@
       <c r="H19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="72" t="s">
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="72"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="72"/>
-      <c r="U19" s="71" t="s">
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="80"/>
+      <c r="T19" s="80"/>
+      <c r="U19" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="V19" s="71"/>
-      <c r="W19" s="71"/>
-      <c r="X19" s="71"/>
-      <c r="Y19" s="71"/>
-      <c r="Z19" s="71"/>
-      <c r="AA19" s="71"/>
-      <c r="AB19" s="71"/>
-      <c r="AC19" s="76" t="s">
+      <c r="V19" s="79"/>
+      <c r="W19" s="79"/>
+      <c r="X19" s="79"/>
+      <c r="Y19" s="79"/>
+      <c r="Z19" s="79"/>
+      <c r="AA19" s="79"/>
+      <c r="AB19" s="79"/>
+      <c r="AC19" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="AD19" s="76"/>
-      <c r="AE19" s="76"/>
-      <c r="AF19" s="76"/>
-      <c r="AG19" s="76"/>
-      <c r="AH19" s="76"/>
-      <c r="AI19" s="76"/>
-      <c r="AJ19" s="76"/>
+      <c r="AD19" s="84"/>
+      <c r="AE19" s="84"/>
+      <c r="AF19" s="84"/>
+      <c r="AG19" s="84"/>
+      <c r="AH19" s="84"/>
+      <c r="AI19" s="84"/>
+      <c r="AJ19" s="84"/>
       <c r="AK19" s="43"/>
       <c r="AS19" s="18"/>
       <c r="AU19" s="3"/>
@@ -4276,70 +4279,70 @@
       <c r="G21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AL21" s="54">
+      <c r="AL21" s="94">
         <v>1098</v>
       </c>
-      <c r="AM21" s="53"/>
-      <c r="AN21" s="53"/>
-      <c r="AO21" s="53"/>
-      <c r="AP21" s="53"/>
-      <c r="AQ21" s="53"/>
-      <c r="AR21" s="53"/>
-      <c r="AS21" s="53"/>
-      <c r="AT21" s="53"/>
-      <c r="AU21" s="53"/>
-      <c r="AV21" s="53"/>
-      <c r="AW21" s="53"/>
-      <c r="AX21" s="53"/>
-      <c r="AY21" s="53"/>
-      <c r="AZ21" s="53"/>
-      <c r="BA21" s="53"/>
-      <c r="BB21" s="53"/>
-      <c r="BC21" s="53"/>
-      <c r="BD21" s="53"/>
-      <c r="BE21" s="53"/>
-      <c r="BF21" s="53"/>
-      <c r="BG21" s="53"/>
-      <c r="BH21" s="53"/>
-      <c r="BI21" s="53"/>
-      <c r="BJ21" s="53"/>
-      <c r="BK21" s="53"/>
-      <c r="BL21" s="53"/>
-      <c r="BM21" s="53"/>
-      <c r="BN21" s="53"/>
-      <c r="BO21" s="53"/>
-      <c r="BP21" s="53"/>
-      <c r="BQ21" s="53"/>
-      <c r="BR21" s="53">
+      <c r="AM21" s="85"/>
+      <c r="AN21" s="85"/>
+      <c r="AO21" s="85"/>
+      <c r="AP21" s="85"/>
+      <c r="AQ21" s="85"/>
+      <c r="AR21" s="85"/>
+      <c r="AS21" s="85"/>
+      <c r="AT21" s="85"/>
+      <c r="AU21" s="85"/>
+      <c r="AV21" s="85"/>
+      <c r="AW21" s="85"/>
+      <c r="AX21" s="85"/>
+      <c r="AY21" s="85"/>
+      <c r="AZ21" s="85"/>
+      <c r="BA21" s="85"/>
+      <c r="BB21" s="85"/>
+      <c r="BC21" s="85"/>
+      <c r="BD21" s="85"/>
+      <c r="BE21" s="85"/>
+      <c r="BF21" s="85"/>
+      <c r="BG21" s="85"/>
+      <c r="BH21" s="85"/>
+      <c r="BI21" s="85"/>
+      <c r="BJ21" s="85"/>
+      <c r="BK21" s="85"/>
+      <c r="BL21" s="85"/>
+      <c r="BM21" s="85"/>
+      <c r="BN21" s="85"/>
+      <c r="BO21" s="85"/>
+      <c r="BP21" s="85"/>
+      <c r="BQ21" s="85"/>
+      <c r="BR21" s="85">
         <v>26</v>
       </c>
-      <c r="BS21" s="53"/>
-      <c r="BT21" s="53"/>
-      <c r="BU21" s="53"/>
-      <c r="BV21" s="53"/>
-      <c r="BW21" s="53"/>
-      <c r="BX21" s="53"/>
-      <c r="BY21" s="53"/>
-      <c r="BZ21" s="53">
+      <c r="BS21" s="85"/>
+      <c r="BT21" s="85"/>
+      <c r="BU21" s="85"/>
+      <c r="BV21" s="85"/>
+      <c r="BW21" s="85"/>
+      <c r="BX21" s="85"/>
+      <c r="BY21" s="85"/>
+      <c r="BZ21" s="85">
         <v>137</v>
       </c>
-      <c r="CA21" s="53"/>
-      <c r="CB21" s="53"/>
-      <c r="CC21" s="53"/>
-      <c r="CD21" s="53"/>
-      <c r="CE21" s="53"/>
-      <c r="CF21" s="53"/>
-      <c r="CG21" s="53"/>
-      <c r="CH21" s="53">
+      <c r="CA21" s="85"/>
+      <c r="CB21" s="85"/>
+      <c r="CC21" s="85"/>
+      <c r="CD21" s="85"/>
+      <c r="CE21" s="85"/>
+      <c r="CF21" s="85"/>
+      <c r="CG21" s="85"/>
+      <c r="CH21" s="85">
         <v>8</v>
       </c>
-      <c r="CI21" s="53"/>
-      <c r="CJ21" s="53"/>
-      <c r="CK21" s="53"/>
-      <c r="CL21" s="53"/>
-      <c r="CM21" s="53"/>
-      <c r="CN21" s="53"/>
-      <c r="CO21" s="53"/>
+      <c r="CI21" s="85"/>
+      <c r="CJ21" s="85"/>
+      <c r="CK21" s="85"/>
+      <c r="CL21" s="85"/>
+      <c r="CM21" s="85"/>
+      <c r="CN21" s="85"/>
+      <c r="CO21" s="85"/>
     </row>
     <row r="22" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
@@ -4447,77 +4450,77 @@
       </c>
     </row>
     <row r="23" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H23" s="81">
+      <c r="H23" s="55">
         <v>18</v>
       </c>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="77" t="s">
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="78"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="78"/>
-      <c r="T23" s="79"/>
-      <c r="U23" s="77" t="s">
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="V23" s="78"/>
-      <c r="W23" s="78"/>
-      <c r="X23" s="78"/>
-      <c r="Y23" s="78"/>
-      <c r="Z23" s="78"/>
-      <c r="AA23" s="78"/>
-      <c r="AB23" s="79"/>
-      <c r="AC23" s="80" t="s">
+      <c r="V23" s="54"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="54"/>
+      <c r="Y23" s="54"/>
+      <c r="Z23" s="54"/>
+      <c r="AA23" s="54"/>
+      <c r="AB23" s="61"/>
+      <c r="AC23" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="AD23" s="81"/>
-      <c r="AE23" s="81"/>
-      <c r="AF23" s="81"/>
-      <c r="AG23" s="81"/>
-      <c r="AH23" s="81"/>
-      <c r="AI23" s="81"/>
-      <c r="AJ23" s="82"/>
+      <c r="AD23" s="55"/>
+      <c r="AE23" s="55"/>
+      <c r="AF23" s="55"/>
+      <c r="AG23" s="55"/>
+      <c r="AH23" s="55"/>
+      <c r="AI23" s="55"/>
+      <c r="AJ23" s="56"/>
       <c r="AK23" s="10"/>
       <c r="AM23" t="s">
         <v>198</v>
       </c>
-      <c r="BR23" s="53" t="s">
+      <c r="BR23" s="85" t="s">
         <v>197</v>
       </c>
-      <c r="BS23" s="53"/>
-      <c r="BT23" s="53"/>
-      <c r="BU23" s="53"/>
-      <c r="BV23" s="53"/>
-      <c r="BW23" s="53"/>
-      <c r="BX23" s="53"/>
-      <c r="BY23" s="53"/>
-      <c r="BZ23" s="53">
+      <c r="BS23" s="85"/>
+      <c r="BT23" s="85"/>
+      <c r="BU23" s="85"/>
+      <c r="BV23" s="85"/>
+      <c r="BW23" s="85"/>
+      <c r="BX23" s="85"/>
+      <c r="BY23" s="85"/>
+      <c r="BZ23" s="85">
         <v>16</v>
       </c>
-      <c r="CA23" s="53"/>
-      <c r="CB23" s="53"/>
-      <c r="CC23" s="53"/>
-      <c r="CD23" s="53"/>
-      <c r="CE23" s="53"/>
-      <c r="CF23" s="53"/>
-      <c r="CG23" s="53"/>
-      <c r="CH23" s="53" t="s">
+      <c r="CA23" s="85"/>
+      <c r="CB23" s="85"/>
+      <c r="CC23" s="85"/>
+      <c r="CD23" s="85"/>
+      <c r="CE23" s="85"/>
+      <c r="CF23" s="85"/>
+      <c r="CG23" s="85"/>
+      <c r="CH23" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="CI23" s="53"/>
-      <c r="CJ23" s="53"/>
-      <c r="CK23" s="53"/>
-      <c r="CL23" s="53"/>
-      <c r="CM23" s="53"/>
-      <c r="CN23" s="53"/>
-      <c r="CO23" s="53"/>
+      <c r="CI23" s="85"/>
+      <c r="CJ23" s="85"/>
+      <c r="CK23" s="85"/>
+      <c r="CL23" s="85"/>
+      <c r="CM23" s="85"/>
+      <c r="CN23" s="85"/>
+      <c r="CO23" s="85"/>
     </row>
     <row r="24" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
@@ -4613,44 +4616,47 @@
       <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H25" s="81">
+      <c r="H25" s="55">
         <v>18</v>
       </c>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="77" t="s">
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N25" s="78"/>
-      <c r="O25" s="78"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="79"/>
-      <c r="U25" s="77" t="s">
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
+      <c r="T25" s="61"/>
+      <c r="U25" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="V25" s="78"/>
-      <c r="W25" s="78"/>
-      <c r="X25" s="78"/>
-      <c r="Y25" s="78"/>
-      <c r="Z25" s="78"/>
-      <c r="AA25" s="78"/>
-      <c r="AB25" s="79"/>
-      <c r="AC25" s="77" t="s">
+      <c r="V25" s="54"/>
+      <c r="W25" s="54"/>
+      <c r="X25" s="54"/>
+      <c r="Y25" s="54"/>
+      <c r="Z25" s="54"/>
+      <c r="AA25" s="54"/>
+      <c r="AB25" s="61"/>
+      <c r="AC25" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="AD25" s="78"/>
-      <c r="AE25" s="78"/>
-      <c r="AF25" s="78"/>
-      <c r="AG25" s="78"/>
-      <c r="AH25" s="78"/>
-      <c r="AI25" s="78"/>
-      <c r="AJ25" s="79"/>
+      <c r="AD25" s="54"/>
+      <c r="AE25" s="54"/>
+      <c r="AF25" s="54"/>
+      <c r="AG25" s="54"/>
+      <c r="AH25" s="54"/>
+      <c r="AI25" s="54"/>
+      <c r="AJ25" s="61"/>
       <c r="AK25" s="10"/>
+      <c r="AM25" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="26" spans="1:102" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H26" s="26"/>
@@ -4778,43 +4784,43 @@
       <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H28" s="81">
+      <c r="H28" s="55">
         <v>18</v>
       </c>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="82"/>
-      <c r="M28" s="77" t="s">
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N28" s="78"/>
-      <c r="O28" s="78"/>
-      <c r="P28" s="78"/>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="78"/>
-      <c r="S28" s="78"/>
-      <c r="T28" s="79"/>
-      <c r="U28" s="80" t="s">
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="61"/>
+      <c r="U28" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="V28" s="81"/>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="81"/>
-      <c r="Z28" s="81"/>
-      <c r="AA28" s="81"/>
-      <c r="AB28" s="82"/>
-      <c r="AC28" s="83" t="s">
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="55"/>
+      <c r="AA28" s="55"/>
+      <c r="AB28" s="56"/>
+      <c r="AC28" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="AD28" s="84"/>
-      <c r="AE28" s="84"/>
-      <c r="AF28" s="84"/>
-      <c r="AG28" s="84"/>
-      <c r="AH28" s="84"/>
-      <c r="AI28" s="84"/>
-      <c r="AJ28" s="85"/>
+      <c r="AD28" s="72"/>
+      <c r="AE28" s="72"/>
+      <c r="AF28" s="72"/>
+      <c r="AG28" s="72"/>
+      <c r="AH28" s="72"/>
+      <c r="AI28" s="72"/>
+      <c r="AJ28" s="73"/>
       <c r="AK28" s="10"/>
     </row>
     <row r="29" spans="1:102" x14ac:dyDescent="0.25">
@@ -4884,56 +4890,56 @@
       <c r="AB29" s="27">
         <v>1</v>
       </c>
-      <c r="AC29" s="94" t="s">
+      <c r="AC29" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="AD29" s="95"/>
-      <c r="AE29" s="95"/>
-      <c r="AF29" s="95"/>
-      <c r="AG29" s="95"/>
-      <c r="AH29" s="95"/>
-      <c r="AI29" s="95"/>
-      <c r="AJ29" s="96"/>
+      <c r="AD29" s="69"/>
+      <c r="AE29" s="69"/>
+      <c r="AF29" s="69"/>
+      <c r="AG29" s="69"/>
+      <c r="AH29" s="69"/>
+      <c r="AI29" s="69"/>
+      <c r="AJ29" s="70"/>
       <c r="AK29" s="10"/>
     </row>
     <row r="30" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H30" s="78" t="s">
+      <c r="H30" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="82"/>
-      <c r="M30" s="77" t="s">
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="N30" s="78"/>
-      <c r="O30" s="78"/>
-      <c r="P30" s="78"/>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="78"/>
-      <c r="S30" s="78"/>
-      <c r="T30" s="79"/>
-      <c r="U30" s="77" t="s">
+      <c r="N30" s="54"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="V30" s="78"/>
-      <c r="W30" s="78"/>
-      <c r="X30" s="78"/>
-      <c r="Y30" s="78"/>
-      <c r="Z30" s="78"/>
-      <c r="AA30" s="78"/>
-      <c r="AB30" s="79"/>
-      <c r="AC30" s="80" t="s">
+      <c r="V30" s="54"/>
+      <c r="W30" s="54"/>
+      <c r="X30" s="54"/>
+      <c r="Y30" s="54"/>
+      <c r="Z30" s="54"/>
+      <c r="AA30" s="54"/>
+      <c r="AB30" s="61"/>
+      <c r="AC30" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="AD30" s="81"/>
-      <c r="AE30" s="81"/>
-      <c r="AF30" s="81"/>
-      <c r="AG30" s="81"/>
-      <c r="AH30" s="81"/>
-      <c r="AI30" s="81"/>
-      <c r="AJ30" s="82"/>
+      <c r="AD30" s="55"/>
+      <c r="AE30" s="55"/>
+      <c r="AF30" s="55"/>
+      <c r="AG30" s="55"/>
+      <c r="AH30" s="55"/>
+      <c r="AI30" s="55"/>
+      <c r="AJ30" s="56"/>
       <c r="AK30" s="10"/>
     </row>
     <row r="31" spans="1:102" x14ac:dyDescent="0.25">
@@ -5030,43 +5036,43 @@
       <c r="AK31" s="10"/>
     </row>
     <row r="32" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H32" s="78" t="s">
+      <c r="H32" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="81"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="81"/>
-      <c r="L32" s="82"/>
-      <c r="M32" s="88" t="s">
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="N32" s="89"/>
-      <c r="O32" s="89"/>
-      <c r="P32" s="89"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="89"/>
-      <c r="T32" s="90"/>
-      <c r="U32" s="88" t="s">
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="64"/>
+      <c r="U32" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="V32" s="89"/>
-      <c r="W32" s="89"/>
-      <c r="X32" s="89"/>
-      <c r="Y32" s="89"/>
-      <c r="Z32" s="89"/>
-      <c r="AA32" s="89"/>
-      <c r="AB32" s="90"/>
-      <c r="AC32" s="91" t="s">
+      <c r="V32" s="63"/>
+      <c r="W32" s="63"/>
+      <c r="X32" s="63"/>
+      <c r="Y32" s="63"/>
+      <c r="Z32" s="63"/>
+      <c r="AA32" s="63"/>
+      <c r="AB32" s="64"/>
+      <c r="AC32" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="AD32" s="92"/>
-      <c r="AE32" s="92"/>
-      <c r="AF32" s="92"/>
-      <c r="AG32" s="92"/>
-      <c r="AH32" s="92"/>
-      <c r="AI32" s="92"/>
-      <c r="AJ32" s="93"/>
+      <c r="AD32" s="66"/>
+      <c r="AE32" s="66"/>
+      <c r="AF32" s="66"/>
+      <c r="AG32" s="66"/>
+      <c r="AH32" s="66"/>
+      <c r="AI32" s="66"/>
+      <c r="AJ32" s="67"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -5077,6 +5083,68 @@
     <sortCondition ref="L3:L15"/>
   </sortState>
   <mergeCells count="78">
+    <mergeCell ref="BR23:BY23"/>
+    <mergeCell ref="BZ23:CG23"/>
+    <mergeCell ref="CH23:CO23"/>
+    <mergeCell ref="BR21:BY21"/>
+    <mergeCell ref="BZ21:CG21"/>
+    <mergeCell ref="CH21:CO21"/>
+    <mergeCell ref="AL14:BA14"/>
+    <mergeCell ref="CH8:CO8"/>
+    <mergeCell ref="AL21:BQ21"/>
+    <mergeCell ref="AT4:BY4"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="BR15:BY15"/>
+    <mergeCell ref="BZ15:CG15"/>
+    <mergeCell ref="U18:AB18"/>
+    <mergeCell ref="AL16:AS16"/>
+    <mergeCell ref="AT16:BA16"/>
+    <mergeCell ref="BJ16:BQ16"/>
+    <mergeCell ref="BB16:BI16"/>
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="AV8:BE8"/>
+    <mergeCell ref="BF8:BQ8"/>
+    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="AL11:AS11"/>
+    <mergeCell ref="CP15:CW15"/>
+    <mergeCell ref="M9:T9"/>
+    <mergeCell ref="BR17:BY17"/>
+    <mergeCell ref="CP16:CW16"/>
+    <mergeCell ref="BR16:BY16"/>
+    <mergeCell ref="BZ16:CG16"/>
+    <mergeCell ref="CH16:CO16"/>
+    <mergeCell ref="BZ17:CG17"/>
+    <mergeCell ref="U15:AB15"/>
+    <mergeCell ref="AC17:AJ17"/>
+    <mergeCell ref="AC16:AJ16"/>
+    <mergeCell ref="AC15:AJ15"/>
+    <mergeCell ref="U16:AB16"/>
+    <mergeCell ref="U17:AB17"/>
+    <mergeCell ref="U14:AB14"/>
+    <mergeCell ref="CH15:CO15"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="AL1:CW1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="S1:AJ1"/>
+    <mergeCell ref="AL7:AS7"/>
+    <mergeCell ref="AL17:BQ17"/>
+    <mergeCell ref="BB14:BY14"/>
+    <mergeCell ref="U19:AB19"/>
+    <mergeCell ref="M19:T19"/>
+    <mergeCell ref="AL8:AU8"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="BR8:CG8"/>
+    <mergeCell ref="AL12:AS12"/>
+    <mergeCell ref="AL15:BQ15"/>
+    <mergeCell ref="AC19:AJ19"/>
+    <mergeCell ref="M23:T23"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="M28:T28"/>
+    <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="AC28:AJ28"/>
+    <mergeCell ref="AC25:AJ25"/>
+    <mergeCell ref="U25:AB25"/>
     <mergeCell ref="CH17:CW17"/>
     <mergeCell ref="H32:L32"/>
     <mergeCell ref="AL13:BQ13"/>
@@ -5093,68 +5161,6 @@
     <mergeCell ref="AC29:AJ29"/>
     <mergeCell ref="AC23:AJ23"/>
     <mergeCell ref="U23:AB23"/>
-    <mergeCell ref="M23:T23"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="M28:T28"/>
-    <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="AC28:AJ28"/>
-    <mergeCell ref="AC25:AJ25"/>
-    <mergeCell ref="U25:AB25"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="AL1:CW1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:R1"/>
-    <mergeCell ref="S1:AJ1"/>
-    <mergeCell ref="AL7:AS7"/>
-    <mergeCell ref="AL17:BQ17"/>
-    <mergeCell ref="BB14:BY14"/>
-    <mergeCell ref="U19:AB19"/>
-    <mergeCell ref="M19:T19"/>
-    <mergeCell ref="AL8:AU8"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="BR8:CG8"/>
-    <mergeCell ref="AL12:AS12"/>
-    <mergeCell ref="AL15:BQ15"/>
-    <mergeCell ref="AC19:AJ19"/>
-    <mergeCell ref="CP15:CW15"/>
-    <mergeCell ref="M9:T9"/>
-    <mergeCell ref="BR17:BY17"/>
-    <mergeCell ref="CP16:CW16"/>
-    <mergeCell ref="BR16:BY16"/>
-    <mergeCell ref="BZ16:CG16"/>
-    <mergeCell ref="CH16:CO16"/>
-    <mergeCell ref="BZ17:CG17"/>
-    <mergeCell ref="U15:AB15"/>
-    <mergeCell ref="AC17:AJ17"/>
-    <mergeCell ref="AC16:AJ16"/>
-    <mergeCell ref="AC15:AJ15"/>
-    <mergeCell ref="U16:AB16"/>
-    <mergeCell ref="U17:AB17"/>
-    <mergeCell ref="U14:AB14"/>
-    <mergeCell ref="CH15:CO15"/>
-    <mergeCell ref="M7:T7"/>
-    <mergeCell ref="AV8:BE8"/>
-    <mergeCell ref="BF8:BQ8"/>
-    <mergeCell ref="M11:T11"/>
-    <mergeCell ref="AL11:AS11"/>
-    <mergeCell ref="AL14:BA14"/>
-    <mergeCell ref="CH8:CO8"/>
-    <mergeCell ref="AL21:BQ21"/>
-    <mergeCell ref="AT4:BY4"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="BR15:BY15"/>
-    <mergeCell ref="BZ15:CG15"/>
-    <mergeCell ref="U18:AB18"/>
-    <mergeCell ref="AL16:AS16"/>
-    <mergeCell ref="AT16:BA16"/>
-    <mergeCell ref="BJ16:BQ16"/>
-    <mergeCell ref="BB16:BI16"/>
-    <mergeCell ref="BR23:BY23"/>
-    <mergeCell ref="BZ23:CG23"/>
-    <mergeCell ref="CH23:CO23"/>
-    <mergeCell ref="BR21:BY21"/>
-    <mergeCell ref="BZ21:CG21"/>
-    <mergeCell ref="CH21:CO21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Console for settings working, protocol updated
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -261,9 +261,6 @@
     <t>Threshold 10 Bit</t>
   </si>
   <si>
-    <t>0-Level 10 Bit</t>
-  </si>
-  <si>
     <t>Sampling Rate in 100Hz</t>
   </si>
   <si>
@@ -615,10 +612,13 @@
     <t>000b8</t>
   </si>
   <si>
-    <t>Started (1Bit)</t>
-  </si>
-  <si>
     <t>11 0010 0111 1111 1111 0000 0110 0100 0000 0001 1110 0000</t>
+  </si>
+  <si>
+    <t>Started and Ctrl-Flags</t>
+  </si>
+  <si>
+    <t>0-Level 16 Bit</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1033,88 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1045,19 +1123,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1085,84 +1163,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:CX32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AV8" sqref="AV8:BE8"/>
+      <selection activeCell="CX9" sqref="CX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,115 +1487,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75" t="s">
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="69"/>
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="69"/>
+      <c r="AJ1" s="69"/>
       <c r="AK1" s="9"/>
-      <c r="AL1" s="75" t="s">
+      <c r="AL1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="75"/>
-      <c r="AU1" s="75"/>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="75"/>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="75"/>
-      <c r="BB1" s="75"/>
-      <c r="BC1" s="75"/>
-      <c r="BD1" s="75"/>
-      <c r="BE1" s="75"/>
-      <c r="BF1" s="75"/>
-      <c r="BG1" s="75"/>
-      <c r="BH1" s="75"/>
-      <c r="BI1" s="75"/>
-      <c r="BJ1" s="75"/>
-      <c r="BK1" s="75"/>
-      <c r="BL1" s="75"/>
-      <c r="BM1" s="75"/>
-      <c r="BN1" s="75"/>
-      <c r="BO1" s="75"/>
-      <c r="BP1" s="75"/>
-      <c r="BQ1" s="75"/>
-      <c r="BR1" s="75"/>
-      <c r="BS1" s="75"/>
-      <c r="BT1" s="75"/>
-      <c r="BU1" s="75"/>
-      <c r="BV1" s="75"/>
-      <c r="BW1" s="75"/>
-      <c r="BX1" s="75"/>
-      <c r="BY1" s="75"/>
-      <c r="BZ1" s="75"/>
-      <c r="CA1" s="75"/>
-      <c r="CB1" s="75"/>
-      <c r="CC1" s="75"/>
-      <c r="CD1" s="75"/>
-      <c r="CE1" s="75"/>
-      <c r="CF1" s="75"/>
-      <c r="CG1" s="75"/>
-      <c r="CH1" s="75"/>
-      <c r="CI1" s="75"/>
-      <c r="CJ1" s="75"/>
-      <c r="CK1" s="75"/>
-      <c r="CL1" s="75"/>
-      <c r="CM1" s="75"/>
-      <c r="CN1" s="75"/>
-      <c r="CO1" s="75"/>
-      <c r="CP1" s="75"/>
-      <c r="CQ1" s="75"/>
-      <c r="CR1" s="75"/>
-      <c r="CS1" s="75"/>
-      <c r="CT1" s="75"/>
-      <c r="CU1" s="75"/>
-      <c r="CV1" s="75"/>
-      <c r="CW1" s="75"/>
+      <c r="AM1" s="69"/>
+      <c r="AN1" s="69"/>
+      <c r="AO1" s="69"/>
+      <c r="AP1" s="69"/>
+      <c r="AQ1" s="69"/>
+      <c r="AR1" s="69"/>
+      <c r="AS1" s="69"/>
+      <c r="AT1" s="69"/>
+      <c r="AU1" s="69"/>
+      <c r="AV1" s="69"/>
+      <c r="AW1" s="69"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="69"/>
+      <c r="AZ1" s="69"/>
+      <c r="BA1" s="69"/>
+      <c r="BB1" s="69"/>
+      <c r="BC1" s="69"/>
+      <c r="BD1" s="69"/>
+      <c r="BE1" s="69"/>
+      <c r="BF1" s="69"/>
+      <c r="BG1" s="69"/>
+      <c r="BH1" s="69"/>
+      <c r="BI1" s="69"/>
+      <c r="BJ1" s="69"/>
+      <c r="BK1" s="69"/>
+      <c r="BL1" s="69"/>
+      <c r="BM1" s="69"/>
+      <c r="BN1" s="69"/>
+      <c r="BO1" s="69"/>
+      <c r="BP1" s="69"/>
+      <c r="BQ1" s="69"/>
+      <c r="BR1" s="69"/>
+      <c r="BS1" s="69"/>
+      <c r="BT1" s="69"/>
+      <c r="BU1" s="69"/>
+      <c r="BV1" s="69"/>
+      <c r="BW1" s="69"/>
+      <c r="BX1" s="69"/>
+      <c r="BY1" s="69"/>
+      <c r="BZ1" s="69"/>
+      <c r="CA1" s="69"/>
+      <c r="CB1" s="69"/>
+      <c r="CC1" s="69"/>
+      <c r="CD1" s="69"/>
+      <c r="CE1" s="69"/>
+      <c r="CF1" s="69"/>
+      <c r="CG1" s="69"/>
+      <c r="CH1" s="69"/>
+      <c r="CI1" s="69"/>
+      <c r="CJ1" s="69"/>
+      <c r="CK1" s="69"/>
+      <c r="CL1" s="69"/>
+      <c r="CM1" s="69"/>
+      <c r="CN1" s="69"/>
+      <c r="CO1" s="69"/>
+      <c r="CP1" s="69"/>
+      <c r="CQ1" s="69"/>
+      <c r="CR1" s="69"/>
+      <c r="CS1" s="69"/>
+      <c r="CT1" s="69"/>
+      <c r="CU1" s="69"/>
+      <c r="CV1" s="69"/>
+      <c r="CW1" s="69"/>
       <c r="CX1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="CX2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -2037,7 +2037,7 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -2132,50 +2132,50 @@
       <c r="AJ4" s="41">
         <v>1</v>
       </c>
-      <c r="AL4" s="77" t="s">
+      <c r="AL4" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="AM4" s="78"/>
-      <c r="AN4" s="78"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="95" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="95"/>
-      <c r="AX4" s="95"/>
-      <c r="AY4" s="95"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="95"/>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="95"/>
-      <c r="BF4" s="95"/>
-      <c r="BG4" s="95"/>
-      <c r="BH4" s="95"/>
-      <c r="BI4" s="95"/>
-      <c r="BJ4" s="95"/>
-      <c r="BK4" s="95"/>
-      <c r="BL4" s="95"/>
-      <c r="BM4" s="95"/>
-      <c r="BN4" s="95"/>
-      <c r="BO4" s="95"/>
-      <c r="BP4" s="95"/>
-      <c r="BQ4" s="95"/>
-      <c r="BR4" s="95"/>
-      <c r="BS4" s="95"/>
-      <c r="BT4" s="95"/>
-      <c r="BU4" s="95"/>
-      <c r="BV4" s="95"/>
-      <c r="BW4" s="95"/>
-      <c r="BX4" s="95"/>
-      <c r="BY4" s="95"/>
+      <c r="AM4" s="56"/>
+      <c r="AN4" s="56"/>
+      <c r="AO4" s="56"/>
+      <c r="AP4" s="56"/>
+      <c r="AQ4" s="56"/>
+      <c r="AR4" s="56"/>
+      <c r="AS4" s="56"/>
+      <c r="AT4" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="58"/>
+      <c r="AY4" s="58"/>
+      <c r="AZ4" s="58"/>
+      <c r="BA4" s="58"/>
+      <c r="BB4" s="58"/>
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="58"/>
+      <c r="BF4" s="58"/>
+      <c r="BG4" s="58"/>
+      <c r="BH4" s="58"/>
+      <c r="BI4" s="58"/>
+      <c r="BJ4" s="58"/>
+      <c r="BK4" s="58"/>
+      <c r="BL4" s="58"/>
+      <c r="BM4" s="58"/>
+      <c r="BN4" s="58"/>
+      <c r="BO4" s="58"/>
+      <c r="BP4" s="58"/>
+      <c r="BQ4" s="58"/>
+      <c r="BR4" s="58"/>
+      <c r="BS4" s="58"/>
+      <c r="BT4" s="58"/>
+      <c r="BU4" s="58"/>
+      <c r="BV4" s="58"/>
+      <c r="BW4" s="58"/>
+      <c r="BX4" s="58"/>
+      <c r="BY4" s="58"/>
       <c r="CG4" s="18"/>
       <c r="CI4" s="3"/>
       <c r="CO4" s="18"/>
@@ -2199,10 +2199,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="11">
         <v>0</v>
@@ -2319,10 +2319,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
@@ -2482,7 +2482,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -2505,16 +2505,16 @@
       <c r="L7" s="12">
         <v>0</v>
       </c>
-      <c r="M7" s="86" t="s">
+      <c r="M7" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="86"/>
-      <c r="T7" s="86"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
       <c r="U7" s="14">
         <v>0</v>
       </c>
@@ -2563,16 +2563,16 @@
       <c r="AJ7" s="41">
         <v>1</v>
       </c>
-      <c r="AL7" s="77" t="s">
+      <c r="AL7" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="AM7" s="78"/>
-      <c r="AN7" s="78"/>
-      <c r="AO7" s="78"/>
-      <c r="AP7" s="78"/>
-      <c r="AQ7" s="78"/>
-      <c r="AR7" s="78"/>
-      <c r="AS7" s="78"/>
+      <c r="AM7" s="56"/>
+      <c r="AN7" s="56"/>
+      <c r="AO7" s="56"/>
+      <c r="AP7" s="56"/>
+      <c r="AQ7" s="56"/>
+      <c r="AR7" s="56"/>
+      <c r="AS7" s="56"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="18"/>
       <c r="BE7" s="3"/>
@@ -2623,16 +2623,16 @@
       <c r="L8" s="12">
         <v>1</v>
       </c>
-      <c r="M8" s="86" t="s">
+      <c r="M8" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="86"/>
-      <c r="Q8" s="86"/>
-      <c r="R8" s="86"/>
-      <c r="S8" s="86"/>
-      <c r="T8" s="86"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="14">
         <v>0</v>
       </c>
@@ -2681,76 +2681,82 @@
       <c r="AJ8" s="41">
         <v>1</v>
       </c>
-      <c r="AL8" s="81" t="s">
+      <c r="AL8" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="AM8" s="82"/>
-      <c r="AN8" s="82"/>
-      <c r="AO8" s="82"/>
-      <c r="AP8" s="82"/>
-      <c r="AQ8" s="82"/>
-      <c r="AR8" s="82"/>
-      <c r="AS8" s="82"/>
-      <c r="AT8" s="82"/>
-      <c r="AU8" s="82"/>
-      <c r="AV8" s="92" t="s">
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW8" s="61"/>
+      <c r="AX8" s="61"/>
+      <c r="AY8" s="61"/>
+      <c r="AZ8" s="61"/>
+      <c r="BA8" s="61"/>
+      <c r="BB8" s="61"/>
+      <c r="BC8" s="61"/>
+      <c r="BD8" s="61"/>
+      <c r="BE8" s="61"/>
+      <c r="BF8" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="AW8" s="92"/>
-      <c r="AX8" s="92"/>
-      <c r="AY8" s="92"/>
-      <c r="AZ8" s="92"/>
-      <c r="BA8" s="92"/>
-      <c r="BB8" s="92"/>
-      <c r="BC8" s="92"/>
-      <c r="BD8" s="92"/>
-      <c r="BE8" s="92"/>
-      <c r="BF8" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="BG8" s="53"/>
-      <c r="BH8" s="53"/>
-      <c r="BI8" s="53"/>
-      <c r="BJ8" s="53"/>
-      <c r="BK8" s="53"/>
-      <c r="BL8" s="53"/>
-      <c r="BM8" s="53"/>
-      <c r="BN8" s="53"/>
-      <c r="BO8" s="53"/>
-      <c r="BP8" s="53"/>
-      <c r="BQ8" s="53"/>
-      <c r="BR8" s="83" t="s">
-        <v>128</v>
-      </c>
-      <c r="BS8" s="83"/>
-      <c r="BT8" s="83"/>
-      <c r="BU8" s="83"/>
-      <c r="BV8" s="83"/>
-      <c r="BW8" s="83"/>
-      <c r="BX8" s="83"/>
-      <c r="BY8" s="83"/>
-      <c r="BZ8" s="83"/>
-      <c r="CA8" s="83"/>
-      <c r="CB8" s="83"/>
-      <c r="CC8" s="83"/>
-      <c r="CD8" s="83"/>
-      <c r="CE8" s="83"/>
-      <c r="CF8" s="83"/>
-      <c r="CG8" s="83"/>
-      <c r="CH8" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="CI8" s="78"/>
-      <c r="CJ8" s="78"/>
-      <c r="CK8" s="78"/>
-      <c r="CL8" s="78"/>
-      <c r="CM8" s="78"/>
-      <c r="CN8" s="78"/>
-      <c r="CO8" s="78"/>
-      <c r="CS8" s="3"/>
-      <c r="CW8" s="18"/>
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62"/>
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62"/>
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+      <c r="BM8" s="62"/>
+      <c r="BN8" s="62"/>
+      <c r="BO8" s="62"/>
+      <c r="BP8" s="62"/>
+      <c r="BQ8" s="62"/>
+      <c r="BR8" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="BS8" s="75"/>
+      <c r="BT8" s="75"/>
+      <c r="BU8" s="75"/>
+      <c r="BV8" s="75"/>
+      <c r="BW8" s="75"/>
+      <c r="BX8" s="75"/>
+      <c r="BY8" s="75"/>
+      <c r="BZ8" s="75"/>
+      <c r="CA8" s="75"/>
+      <c r="CB8" s="75"/>
+      <c r="CC8" s="75"/>
+      <c r="CD8" s="75"/>
+      <c r="CE8" s="75"/>
+      <c r="CF8" s="75"/>
+      <c r="CG8" s="75"/>
+      <c r="CH8" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="CI8" s="56"/>
+      <c r="CJ8" s="56"/>
+      <c r="CK8" s="56"/>
+      <c r="CL8" s="56"/>
+      <c r="CM8" s="56"/>
+      <c r="CN8" s="56"/>
+      <c r="CO8" s="56"/>
+      <c r="CP8" s="56"/>
+      <c r="CQ8" s="56"/>
+      <c r="CR8" s="56"/>
+      <c r="CS8" s="56"/>
+      <c r="CT8" s="56"/>
+      <c r="CU8" s="56"/>
+      <c r="CV8" s="56"/>
+      <c r="CW8" s="56"/>
       <c r="CX8">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:102" x14ac:dyDescent="0.25">
@@ -2764,10 +2770,10 @@
         <v>20</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32" t="s">
@@ -2788,16 +2794,16 @@
       <c r="L9" s="34">
         <v>0</v>
       </c>
-      <c r="M9" s="86" t="s">
+      <c r="M9" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="86"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="86"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
       <c r="U9" s="35">
         <v>0</v>
       </c>
@@ -2913,10 +2919,10 @@
         <v>19</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32" t="s">
@@ -3099,16 +3105,16 @@
       <c r="L11" s="12">
         <v>0</v>
       </c>
-      <c r="M11" s="86" t="s">
+      <c r="M11" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
       <c r="U11" s="14">
         <v>0</v>
       </c>
@@ -3157,16 +3163,16 @@
       <c r="AJ11" s="41">
         <v>1</v>
       </c>
-      <c r="AL11" s="77" t="s">
-        <v>123</v>
-      </c>
-      <c r="AM11" s="78"/>
-      <c r="AN11" s="78"/>
-      <c r="AO11" s="78"/>
-      <c r="AP11" s="78"/>
-      <c r="AQ11" s="78"/>
-      <c r="AR11" s="78"/>
-      <c r="AS11" s="78"/>
+      <c r="AL11" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM11" s="56"/>
+      <c r="AN11" s="56"/>
+      <c r="AO11" s="56"/>
+      <c r="AP11" s="56"/>
+      <c r="AQ11" s="56"/>
+      <c r="AR11" s="56"/>
+      <c r="AS11" s="56"/>
       <c r="AU11" s="3"/>
       <c r="BA11" s="18"/>
       <c r="BE11" s="3"/>
@@ -3289,16 +3295,16 @@
       <c r="AJ12" s="48">
         <v>1</v>
       </c>
-      <c r="AL12" s="77" t="s">
-        <v>123</v>
-      </c>
-      <c r="AM12" s="78"/>
-      <c r="AN12" s="78"/>
-      <c r="AO12" s="78"/>
-      <c r="AP12" s="78"/>
-      <c r="AQ12" s="78"/>
-      <c r="AR12" s="78"/>
-      <c r="AS12" s="78"/>
+      <c r="AL12" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM12" s="56"/>
+      <c r="AN12" s="56"/>
+      <c r="AO12" s="56"/>
+      <c r="AP12" s="56"/>
+      <c r="AQ12" s="56"/>
+      <c r="AR12" s="56"/>
+      <c r="AS12" s="56"/>
       <c r="AU12" s="3"/>
       <c r="BA12" s="18"/>
       <c r="BE12" s="3"/>
@@ -3333,7 +3339,7 @@
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H13" s="11">
         <v>1</v>
@@ -3423,40 +3429,40 @@
         <v>1</v>
       </c>
       <c r="AK13" s="49"/>
-      <c r="AL13" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM13" s="58"/>
-      <c r="AN13" s="58"/>
-      <c r="AO13" s="58"/>
-      <c r="AP13" s="58"/>
-      <c r="AQ13" s="58"/>
-      <c r="AR13" s="58"/>
-      <c r="AS13" s="58"/>
-      <c r="AT13" s="58"/>
-      <c r="AU13" s="58"/>
-      <c r="AV13" s="58"/>
-      <c r="AW13" s="58"/>
-      <c r="AX13" s="58"/>
-      <c r="AY13" s="58"/>
-      <c r="AZ13" s="58"/>
-      <c r="BA13" s="58"/>
-      <c r="BB13" s="58"/>
-      <c r="BC13" s="58"/>
-      <c r="BD13" s="58"/>
-      <c r="BE13" s="58"/>
-      <c r="BF13" s="58"/>
-      <c r="BG13" s="58"/>
-      <c r="BH13" s="58"/>
-      <c r="BI13" s="58"/>
-      <c r="BJ13" s="58"/>
-      <c r="BK13" s="58"/>
-      <c r="BL13" s="58"/>
-      <c r="BM13" s="58"/>
-      <c r="BN13" s="58"/>
-      <c r="BO13" s="58"/>
-      <c r="BP13" s="58"/>
-      <c r="BQ13" s="58"/>
+      <c r="AL13" s="86" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM13" s="87"/>
+      <c r="AN13" s="87"/>
+      <c r="AO13" s="87"/>
+      <c r="AP13" s="87"/>
+      <c r="AQ13" s="87"/>
+      <c r="AR13" s="87"/>
+      <c r="AS13" s="87"/>
+      <c r="AT13" s="87"/>
+      <c r="AU13" s="87"/>
+      <c r="AV13" s="87"/>
+      <c r="AW13" s="87"/>
+      <c r="AX13" s="87"/>
+      <c r="AY13" s="87"/>
+      <c r="AZ13" s="87"/>
+      <c r="BA13" s="87"/>
+      <c r="BB13" s="87"/>
+      <c r="BC13" s="87"/>
+      <c r="BD13" s="87"/>
+      <c r="BE13" s="87"/>
+      <c r="BF13" s="87"/>
+      <c r="BG13" s="87"/>
+      <c r="BH13" s="87"/>
+      <c r="BI13" s="87"/>
+      <c r="BJ13" s="87"/>
+      <c r="BK13" s="87"/>
+      <c r="BL13" s="87"/>
+      <c r="BM13" s="87"/>
+      <c r="BN13" s="87"/>
+      <c r="BO13" s="87"/>
+      <c r="BP13" s="87"/>
+      <c r="BQ13" s="87"/>
       <c r="BR13" s="23"/>
       <c r="BS13" s="23"/>
       <c r="BT13" s="23"/>
@@ -3504,131 +3510,131 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>1</v>
+      </c>
+      <c r="M14" s="15">
+        <v>0</v>
+      </c>
+      <c r="N14" s="15">
+        <v>0</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
+      <c r="P14" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>0</v>
+      </c>
+      <c r="R14" s="15">
+        <v>0</v>
+      </c>
+      <c r="S14" s="15">
+        <v>0</v>
+      </c>
+      <c r="T14" s="15">
+        <v>1</v>
+      </c>
+      <c r="U14" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="V14" s="65"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="65"/>
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="65"/>
+      <c r="AA14" s="65"/>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="13">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="41">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM14" s="55"/>
+      <c r="AN14" s="55"/>
+      <c r="AO14" s="55"/>
+      <c r="AP14" s="55"/>
+      <c r="AQ14" s="55"/>
+      <c r="AR14" s="55"/>
+      <c r="AS14" s="55"/>
+      <c r="AT14" s="55"/>
+      <c r="AU14" s="55"/>
+      <c r="AV14" s="55"/>
+      <c r="AW14" s="55"/>
+      <c r="AX14" s="55"/>
+      <c r="AY14" s="55"/>
+      <c r="AZ14" s="55"/>
+      <c r="BA14" s="55"/>
+      <c r="BB14" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="11">
-        <v>1</v>
-      </c>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
-        <v>1</v>
-      </c>
-      <c r="M14" s="15">
-        <v>0</v>
-      </c>
-      <c r="N14" s="15">
-        <v>0</v>
-      </c>
-      <c r="O14" s="15">
-        <v>0</v>
-      </c>
-      <c r="P14" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="15">
-        <v>0</v>
-      </c>
-      <c r="R14" s="15">
-        <v>0</v>
-      </c>
-      <c r="S14" s="15">
-        <v>0</v>
-      </c>
-      <c r="T14" s="15">
-        <v>1</v>
-      </c>
-      <c r="U14" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="V14" s="89"/>
-      <c r="W14" s="89"/>
-      <c r="X14" s="89"/>
-      <c r="Y14" s="89"/>
-      <c r="Z14" s="89"/>
-      <c r="AA14" s="89"/>
-      <c r="AB14" s="89"/>
-      <c r="AC14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="41">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="77" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM14" s="93"/>
-      <c r="AN14" s="93"/>
-      <c r="AO14" s="93"/>
-      <c r="AP14" s="93"/>
-      <c r="AQ14" s="93"/>
-      <c r="AR14" s="93"/>
-      <c r="AS14" s="93"/>
-      <c r="AT14" s="93"/>
-      <c r="AU14" s="93"/>
-      <c r="AV14" s="93"/>
-      <c r="AW14" s="93"/>
-      <c r="AX14" s="93"/>
-      <c r="AY14" s="93"/>
-      <c r="AZ14" s="93"/>
-      <c r="BA14" s="93"/>
-      <c r="BB14" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="BC14" s="53"/>
-      <c r="BD14" s="53"/>
-      <c r="BE14" s="53"/>
-      <c r="BF14" s="53"/>
-      <c r="BG14" s="53"/>
-      <c r="BH14" s="53"/>
-      <c r="BI14" s="53"/>
-      <c r="BJ14" s="53"/>
-      <c r="BK14" s="53"/>
-      <c r="BL14" s="53"/>
-      <c r="BM14" s="53"/>
-      <c r="BN14" s="53"/>
-      <c r="BO14" s="53"/>
-      <c r="BP14" s="53"/>
-      <c r="BQ14" s="53"/>
-      <c r="BR14" s="53"/>
-      <c r="BS14" s="53"/>
-      <c r="BT14" s="53"/>
-      <c r="BU14" s="53"/>
-      <c r="BV14" s="53"/>
-      <c r="BW14" s="53"/>
-      <c r="BX14" s="53"/>
-      <c r="BY14" s="53"/>
+      <c r="BC14" s="62"/>
+      <c r="BD14" s="62"/>
+      <c r="BE14" s="62"/>
+      <c r="BF14" s="62"/>
+      <c r="BG14" s="62"/>
+      <c r="BH14" s="62"/>
+      <c r="BI14" s="62"/>
+      <c r="BJ14" s="62"/>
+      <c r="BK14" s="62"/>
+      <c r="BL14" s="62"/>
+      <c r="BM14" s="62"/>
+      <c r="BN14" s="62"/>
+      <c r="BO14" s="62"/>
+      <c r="BP14" s="62"/>
+      <c r="BQ14" s="62"/>
+      <c r="BR14" s="62"/>
+      <c r="BS14" s="62"/>
+      <c r="BT14" s="62"/>
+      <c r="BU14" s="62"/>
+      <c r="BV14" s="62"/>
+      <c r="BW14" s="62"/>
+      <c r="BX14" s="62"/>
+      <c r="BY14" s="62"/>
       <c r="CG14" s="18"/>
       <c r="CI14" s="3"/>
       <c r="CO14" s="18"/>
@@ -3658,7 +3664,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="11">
         <v>1</v>
@@ -3699,102 +3705,102 @@
       <c r="T15" s="15">
         <v>1</v>
       </c>
-      <c r="U15" s="89" t="s">
+      <c r="U15" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="V15" s="89"/>
-      <c r="W15" s="89"/>
-      <c r="X15" s="89"/>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="89"/>
-      <c r="AA15" s="89"/>
-      <c r="AB15" s="89"/>
-      <c r="AC15" s="90" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD15" s="91"/>
-      <c r="AE15" s="91"/>
-      <c r="AF15" s="91"/>
-      <c r="AG15" s="91"/>
-      <c r="AH15" s="91"/>
-      <c r="AI15" s="91"/>
-      <c r="AJ15" s="91"/>
-      <c r="AL15" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="AM15" s="78"/>
-      <c r="AN15" s="78"/>
-      <c r="AO15" s="78"/>
-      <c r="AP15" s="78"/>
-      <c r="AQ15" s="78"/>
-      <c r="AR15" s="78"/>
-      <c r="AS15" s="78"/>
-      <c r="AT15" s="78"/>
-      <c r="AU15" s="78"/>
-      <c r="AV15" s="78"/>
-      <c r="AW15" s="78"/>
-      <c r="AX15" s="78"/>
-      <c r="AY15" s="78"/>
-      <c r="AZ15" s="78"/>
-      <c r="BA15" s="78"/>
-      <c r="BB15" s="78"/>
-      <c r="BC15" s="78"/>
-      <c r="BD15" s="78"/>
-      <c r="BE15" s="78"/>
-      <c r="BF15" s="78"/>
-      <c r="BG15" s="78"/>
-      <c r="BH15" s="78"/>
-      <c r="BI15" s="78"/>
-      <c r="BJ15" s="78"/>
-      <c r="BK15" s="78"/>
-      <c r="BL15" s="78"/>
-      <c r="BM15" s="78"/>
-      <c r="BN15" s="78"/>
-      <c r="BO15" s="78"/>
-      <c r="BP15" s="78"/>
-      <c r="BQ15" s="78"/>
-      <c r="BR15" s="85" t="s">
+      <c r="V15" s="65"/>
+      <c r="W15" s="65"/>
+      <c r="X15" s="65"/>
+      <c r="Y15" s="65"/>
+      <c r="Z15" s="65"/>
+      <c r="AA15" s="65"/>
+      <c r="AB15" s="65"/>
+      <c r="AC15" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD15" s="67"/>
+      <c r="AE15" s="67"/>
+      <c r="AF15" s="67"/>
+      <c r="AG15" s="67"/>
+      <c r="AH15" s="67"/>
+      <c r="AI15" s="67"/>
+      <c r="AJ15" s="67"/>
+      <c r="AL15" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM15" s="56"/>
+      <c r="AN15" s="56"/>
+      <c r="AO15" s="56"/>
+      <c r="AP15" s="56"/>
+      <c r="AQ15" s="56"/>
+      <c r="AR15" s="56"/>
+      <c r="AS15" s="56"/>
+      <c r="AT15" s="56"/>
+      <c r="AU15" s="56"/>
+      <c r="AV15" s="56"/>
+      <c r="AW15" s="56"/>
+      <c r="AX15" s="56"/>
+      <c r="AY15" s="56"/>
+      <c r="AZ15" s="56"/>
+      <c r="BA15" s="56"/>
+      <c r="BB15" s="56"/>
+      <c r="BC15" s="56"/>
+      <c r="BD15" s="56"/>
+      <c r="BE15" s="56"/>
+      <c r="BF15" s="56"/>
+      <c r="BG15" s="56"/>
+      <c r="BH15" s="56"/>
+      <c r="BI15" s="56"/>
+      <c r="BJ15" s="56"/>
+      <c r="BK15" s="56"/>
+      <c r="BL15" s="56"/>
+      <c r="BM15" s="56"/>
+      <c r="BN15" s="56"/>
+      <c r="BO15" s="56"/>
+      <c r="BP15" s="56"/>
+      <c r="BQ15" s="56"/>
+      <c r="BR15" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="BS15" s="53"/>
+      <c r="BT15" s="53"/>
+      <c r="BU15" s="53"/>
+      <c r="BV15" s="53"/>
+      <c r="BW15" s="53"/>
+      <c r="BX15" s="53"/>
+      <c r="BY15" s="53"/>
+      <c r="BZ15" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="BS15" s="85"/>
-      <c r="BT15" s="85"/>
-      <c r="BU15" s="85"/>
-      <c r="BV15" s="85"/>
-      <c r="BW15" s="85"/>
-      <c r="BX15" s="85"/>
-      <c r="BY15" s="85"/>
-      <c r="BZ15" s="85" t="s">
+      <c r="CA15" s="53"/>
+      <c r="CB15" s="53"/>
+      <c r="CC15" s="53"/>
+      <c r="CD15" s="53"/>
+      <c r="CE15" s="53"/>
+      <c r="CF15" s="53"/>
+      <c r="CG15" s="53"/>
+      <c r="CH15" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="CI15" s="53"/>
+      <c r="CJ15" s="53"/>
+      <c r="CK15" s="53"/>
+      <c r="CL15" s="53"/>
+      <c r="CM15" s="53"/>
+      <c r="CN15" s="53"/>
+      <c r="CO15" s="53"/>
+      <c r="CP15" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="CA15" s="85"/>
-      <c r="CB15" s="85"/>
-      <c r="CC15" s="85"/>
-      <c r="CD15" s="85"/>
-      <c r="CE15" s="85"/>
-      <c r="CF15" s="85"/>
-      <c r="CG15" s="85"/>
-      <c r="CH15" s="85" t="s">
-        <v>115</v>
-      </c>
-      <c r="CI15" s="85"/>
-      <c r="CJ15" s="85"/>
-      <c r="CK15" s="85"/>
-      <c r="CL15" s="85"/>
-      <c r="CM15" s="85"/>
-      <c r="CN15" s="85"/>
-      <c r="CO15" s="85"/>
-      <c r="CP15" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="CQ15" s="85"/>
-      <c r="CR15" s="85"/>
-      <c r="CS15" s="85"/>
-      <c r="CT15" s="85"/>
-      <c r="CU15" s="85"/>
-      <c r="CV15" s="85"/>
-      <c r="CW15" s="85"/>
+      <c r="CQ15" s="53"/>
+      <c r="CR15" s="53"/>
+      <c r="CS15" s="53"/>
+      <c r="CT15" s="53"/>
+      <c r="CU15" s="53"/>
+      <c r="CV15" s="53"/>
+      <c r="CW15" s="53"/>
       <c r="CX15" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:102" x14ac:dyDescent="0.25">
@@ -3814,7 +3820,7 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" s="11">
         <v>1</v>
@@ -3855,108 +3861,108 @@
       <c r="T16" s="15">
         <v>1</v>
       </c>
-      <c r="U16" s="89" t="s">
+      <c r="U16" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="V16" s="89"/>
-      <c r="W16" s="89"/>
-      <c r="X16" s="89"/>
-      <c r="Y16" s="89"/>
-      <c r="Z16" s="89"/>
-      <c r="AA16" s="89"/>
-      <c r="AB16" s="89"/>
-      <c r="AC16" s="90" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD16" s="91"/>
-      <c r="AE16" s="91"/>
-      <c r="AF16" s="91"/>
-      <c r="AG16" s="91"/>
-      <c r="AH16" s="91"/>
-      <c r="AI16" s="91"/>
-      <c r="AJ16" s="91"/>
-      <c r="AL16" s="85" t="s">
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="65"/>
+      <c r="AA16" s="65"/>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD16" s="67"/>
+      <c r="AE16" s="67"/>
+      <c r="AF16" s="67"/>
+      <c r="AG16" s="67"/>
+      <c r="AH16" s="67"/>
+      <c r="AI16" s="67"/>
+      <c r="AJ16" s="67"/>
+      <c r="AL16" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM16" s="53"/>
+      <c r="AN16" s="53"/>
+      <c r="AO16" s="53"/>
+      <c r="AP16" s="53"/>
+      <c r="AQ16" s="53"/>
+      <c r="AR16" s="53"/>
+      <c r="AS16" s="53"/>
+      <c r="AT16" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU16" s="53"/>
+      <c r="AV16" s="53"/>
+      <c r="AW16" s="53"/>
+      <c r="AX16" s="53"/>
+      <c r="AY16" s="53"/>
+      <c r="AZ16" s="53"/>
+      <c r="BA16" s="53"/>
+      <c r="BB16" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AM16" s="85"/>
-      <c r="AN16" s="85"/>
-      <c r="AO16" s="85"/>
-      <c r="AP16" s="85"/>
-      <c r="AQ16" s="85"/>
-      <c r="AR16" s="85"/>
-      <c r="AS16" s="85"/>
-      <c r="AT16" s="85" t="s">
+      <c r="BC16" s="53"/>
+      <c r="BD16" s="53"/>
+      <c r="BE16" s="53"/>
+      <c r="BF16" s="53"/>
+      <c r="BG16" s="53"/>
+      <c r="BH16" s="53"/>
+      <c r="BI16" s="53"/>
+      <c r="BJ16" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="AU16" s="85"/>
-      <c r="AV16" s="85"/>
-      <c r="AW16" s="85"/>
-      <c r="AX16" s="85"/>
-      <c r="AY16" s="85"/>
-      <c r="AZ16" s="85"/>
-      <c r="BA16" s="85"/>
-      <c r="BB16" s="85" t="s">
+      <c r="BK16" s="53"/>
+      <c r="BL16" s="53"/>
+      <c r="BM16" s="53"/>
+      <c r="BN16" s="53"/>
+      <c r="BO16" s="53"/>
+      <c r="BP16" s="53"/>
+      <c r="BQ16" s="53"/>
+      <c r="BR16" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="BC16" s="85"/>
-      <c r="BD16" s="85"/>
-      <c r="BE16" s="85"/>
-      <c r="BF16" s="85"/>
-      <c r="BG16" s="85"/>
-      <c r="BH16" s="85"/>
-      <c r="BI16" s="85"/>
-      <c r="BJ16" s="85" t="s">
+      <c r="BS16" s="53"/>
+      <c r="BT16" s="53"/>
+      <c r="BU16" s="53"/>
+      <c r="BV16" s="53"/>
+      <c r="BW16" s="53"/>
+      <c r="BX16" s="53"/>
+      <c r="BY16" s="53"/>
+      <c r="BZ16" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="BK16" s="85"/>
-      <c r="BL16" s="85"/>
-      <c r="BM16" s="85"/>
-      <c r="BN16" s="85"/>
-      <c r="BO16" s="85"/>
-      <c r="BP16" s="85"/>
-      <c r="BQ16" s="85"/>
-      <c r="BR16" s="85" t="s">
+      <c r="CA16" s="53"/>
+      <c r="CB16" s="53"/>
+      <c r="CC16" s="53"/>
+      <c r="CD16" s="53"/>
+      <c r="CE16" s="53"/>
+      <c r="CF16" s="53"/>
+      <c r="CG16" s="53"/>
+      <c r="CH16" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="BS16" s="85"/>
-      <c r="BT16" s="85"/>
-      <c r="BU16" s="85"/>
-      <c r="BV16" s="85"/>
-      <c r="BW16" s="85"/>
-      <c r="BX16" s="85"/>
-      <c r="BY16" s="85"/>
-      <c r="BZ16" s="85" t="s">
+      <c r="CI16" s="53"/>
+      <c r="CJ16" s="53"/>
+      <c r="CK16" s="53"/>
+      <c r="CL16" s="53"/>
+      <c r="CM16" s="53"/>
+      <c r="CN16" s="53"/>
+      <c r="CO16" s="53"/>
+      <c r="CP16" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="CA16" s="85"/>
-      <c r="CB16" s="85"/>
-      <c r="CC16" s="85"/>
-      <c r="CD16" s="85"/>
-      <c r="CE16" s="85"/>
-      <c r="CF16" s="85"/>
-      <c r="CG16" s="85"/>
-      <c r="CH16" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="CI16" s="85"/>
-      <c r="CJ16" s="85"/>
-      <c r="CK16" s="85"/>
-      <c r="CL16" s="85"/>
-      <c r="CM16" s="85"/>
-      <c r="CN16" s="85"/>
-      <c r="CO16" s="85"/>
-      <c r="CP16" s="85" t="s">
-        <v>106</v>
-      </c>
-      <c r="CQ16" s="85"/>
-      <c r="CR16" s="85"/>
-      <c r="CS16" s="85"/>
-      <c r="CT16" s="85"/>
-      <c r="CU16" s="85"/>
-      <c r="CV16" s="85"/>
-      <c r="CW16" s="85"/>
+      <c r="CQ16" s="53"/>
+      <c r="CR16" s="53"/>
+      <c r="CS16" s="53"/>
+      <c r="CT16" s="53"/>
+      <c r="CU16" s="53"/>
+      <c r="CV16" s="53"/>
+      <c r="CW16" s="53"/>
       <c r="CX16" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:102" x14ac:dyDescent="0.25">
@@ -3976,139 +3982,139 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1</v>
+      </c>
+      <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="15">
+        <v>0</v>
+      </c>
+      <c r="N17" s="15">
+        <v>0</v>
+      </c>
+      <c r="O17" s="15">
+        <v>0</v>
+      </c>
+      <c r="P17" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="15">
+        <v>0</v>
+      </c>
+      <c r="R17" s="15">
+        <v>0</v>
+      </c>
+      <c r="S17" s="15">
+        <v>0</v>
+      </c>
+      <c r="T17" s="15">
+        <v>1</v>
+      </c>
+      <c r="U17" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="V17" s="65"/>
+      <c r="W17" s="65"/>
+      <c r="X17" s="65"/>
+      <c r="Y17" s="65"/>
+      <c r="Z17" s="65"/>
+      <c r="AA17" s="65"/>
+      <c r="AB17" s="65"/>
+      <c r="AC17" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD17" s="67"/>
+      <c r="AE17" s="67"/>
+      <c r="AF17" s="67"/>
+      <c r="AG17" s="67"/>
+      <c r="AH17" s="67"/>
+      <c r="AI17" s="67"/>
+      <c r="AJ17" s="67"/>
+      <c r="AL17" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12">
-        <v>1</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <v>0</v>
-      </c>
-      <c r="M17" s="15">
-        <v>0</v>
-      </c>
-      <c r="N17" s="15">
-        <v>0</v>
-      </c>
-      <c r="O17" s="15">
-        <v>0</v>
-      </c>
-      <c r="P17" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="15">
-        <v>0</v>
-      </c>
-      <c r="R17" s="15">
-        <v>0</v>
-      </c>
-      <c r="S17" s="15">
-        <v>0</v>
-      </c>
-      <c r="T17" s="15">
-        <v>1</v>
-      </c>
-      <c r="U17" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="V17" s="89"/>
-      <c r="W17" s="89"/>
-      <c r="X17" s="89"/>
-      <c r="Y17" s="89"/>
-      <c r="Z17" s="89"/>
-      <c r="AA17" s="89"/>
-      <c r="AB17" s="89"/>
-      <c r="AC17" s="90" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD17" s="91"/>
-      <c r="AE17" s="91"/>
-      <c r="AF17" s="91"/>
-      <c r="AG17" s="91"/>
-      <c r="AH17" s="91"/>
-      <c r="AI17" s="91"/>
-      <c r="AJ17" s="91"/>
-      <c r="AL17" s="77" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM17" s="78"/>
-      <c r="AN17" s="78"/>
-      <c r="AO17" s="78"/>
-      <c r="AP17" s="78"/>
-      <c r="AQ17" s="78"/>
-      <c r="AR17" s="78"/>
-      <c r="AS17" s="78"/>
-      <c r="AT17" s="78"/>
-      <c r="AU17" s="78"/>
-      <c r="AV17" s="78"/>
-      <c r="AW17" s="78"/>
-      <c r="AX17" s="78"/>
-      <c r="AY17" s="78"/>
-      <c r="AZ17" s="78"/>
-      <c r="BA17" s="78"/>
-      <c r="BB17" s="78"/>
-      <c r="BC17" s="78"/>
-      <c r="BD17" s="78"/>
-      <c r="BE17" s="78"/>
-      <c r="BF17" s="78"/>
-      <c r="BG17" s="78"/>
-      <c r="BH17" s="78"/>
-      <c r="BI17" s="78"/>
-      <c r="BJ17" s="78"/>
-      <c r="BK17" s="78"/>
-      <c r="BL17" s="78"/>
-      <c r="BM17" s="78"/>
-      <c r="BN17" s="78"/>
-      <c r="BO17" s="78"/>
-      <c r="BP17" s="78"/>
-      <c r="BQ17" s="78"/>
-      <c r="BR17" s="87" t="s">
+      <c r="AM17" s="56"/>
+      <c r="AN17" s="56"/>
+      <c r="AO17" s="56"/>
+      <c r="AP17" s="56"/>
+      <c r="AQ17" s="56"/>
+      <c r="AR17" s="56"/>
+      <c r="AS17" s="56"/>
+      <c r="AT17" s="56"/>
+      <c r="AU17" s="56"/>
+      <c r="AV17" s="56"/>
+      <c r="AW17" s="56"/>
+      <c r="AX17" s="56"/>
+      <c r="AY17" s="56"/>
+      <c r="AZ17" s="56"/>
+      <c r="BA17" s="56"/>
+      <c r="BB17" s="56"/>
+      <c r="BC17" s="56"/>
+      <c r="BD17" s="56"/>
+      <c r="BE17" s="56"/>
+      <c r="BF17" s="56"/>
+      <c r="BG17" s="56"/>
+      <c r="BH17" s="56"/>
+      <c r="BI17" s="56"/>
+      <c r="BJ17" s="56"/>
+      <c r="BK17" s="56"/>
+      <c r="BL17" s="56"/>
+      <c r="BM17" s="56"/>
+      <c r="BN17" s="56"/>
+      <c r="BO17" s="56"/>
+      <c r="BP17" s="56"/>
+      <c r="BQ17" s="56"/>
+      <c r="BR17" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS17" s="63"/>
+      <c r="BT17" s="63"/>
+      <c r="BU17" s="63"/>
+      <c r="BV17" s="63"/>
+      <c r="BW17" s="63"/>
+      <c r="BX17" s="63"/>
+      <c r="BY17" s="63"/>
+      <c r="BZ17" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="BS17" s="87"/>
-      <c r="BT17" s="87"/>
-      <c r="BU17" s="87"/>
-      <c r="BV17" s="87"/>
-      <c r="BW17" s="87"/>
-      <c r="BX17" s="87"/>
-      <c r="BY17" s="87"/>
-      <c r="BZ17" s="88" t="s">
+      <c r="CA17" s="64"/>
+      <c r="CB17" s="64"/>
+      <c r="CC17" s="64"/>
+      <c r="CD17" s="64"/>
+      <c r="CE17" s="64"/>
+      <c r="CF17" s="64"/>
+      <c r="CG17" s="64"/>
+      <c r="CH17" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="CA17" s="88"/>
-      <c r="CB17" s="88"/>
-      <c r="CC17" s="88"/>
-      <c r="CD17" s="88"/>
-      <c r="CE17" s="88"/>
-      <c r="CF17" s="88"/>
-      <c r="CG17" s="88"/>
-      <c r="CH17" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="CI17" s="53"/>
-      <c r="CJ17" s="53"/>
-      <c r="CK17" s="53"/>
-      <c r="CL17" s="53"/>
-      <c r="CM17" s="53"/>
-      <c r="CN17" s="53"/>
-      <c r="CO17" s="53"/>
-      <c r="CP17" s="53"/>
-      <c r="CQ17" s="53"/>
-      <c r="CR17" s="53"/>
-      <c r="CS17" s="53"/>
-      <c r="CT17" s="53"/>
-      <c r="CU17" s="53"/>
-      <c r="CV17" s="53"/>
-      <c r="CW17" s="53"/>
+      <c r="CI17" s="62"/>
+      <c r="CJ17" s="62"/>
+      <c r="CK17" s="62"/>
+      <c r="CL17" s="62"/>
+      <c r="CM17" s="62"/>
+      <c r="CN17" s="62"/>
+      <c r="CO17" s="62"/>
+      <c r="CP17" s="62"/>
+      <c r="CQ17" s="62"/>
+      <c r="CR17" s="62"/>
+      <c r="CS17" s="62"/>
+      <c r="CT17" s="62"/>
+      <c r="CU17" s="62"/>
+      <c r="CV17" s="62"/>
+      <c r="CW17" s="62"/>
       <c r="CX17">
         <v>7</v>
       </c>
@@ -4124,13 +4130,13 @@
         <v>20</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" s="33">
         <v>1</v>
@@ -4171,16 +4177,16 @@
       <c r="T18" s="39">
         <v>1</v>
       </c>
-      <c r="U18" s="96" t="s">
+      <c r="U18" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="V18" s="96"/>
-      <c r="W18" s="96"/>
-      <c r="X18" s="96"/>
-      <c r="Y18" s="96"/>
-      <c r="Z18" s="96"/>
-      <c r="AA18" s="96"/>
-      <c r="AB18" s="96"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
       <c r="AC18" s="13">
         <v>0</v>
       </c>
@@ -4224,42 +4230,42 @@
       <c r="H19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="74" t="s">
+      <c r="I19" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="80" t="s">
+      <c r="J19" s="68"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="80"/>
-      <c r="R19" s="80"/>
-      <c r="S19" s="80"/>
-      <c r="T19" s="80"/>
-      <c r="U19" s="79" t="s">
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="V19" s="79"/>
-      <c r="W19" s="79"/>
-      <c r="X19" s="79"/>
-      <c r="Y19" s="79"/>
-      <c r="Z19" s="79"/>
-      <c r="AA19" s="79"/>
-      <c r="AB19" s="79"/>
-      <c r="AC19" s="84" t="s">
+      <c r="V19" s="71"/>
+      <c r="W19" s="71"/>
+      <c r="X19" s="71"/>
+      <c r="Y19" s="71"/>
+      <c r="Z19" s="71"/>
+      <c r="AA19" s="71"/>
+      <c r="AB19" s="71"/>
+      <c r="AC19" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="AD19" s="84"/>
-      <c r="AE19" s="84"/>
-      <c r="AF19" s="84"/>
-      <c r="AG19" s="84"/>
-      <c r="AH19" s="84"/>
-      <c r="AI19" s="84"/>
-      <c r="AJ19" s="84"/>
+      <c r="AD19" s="76"/>
+      <c r="AE19" s="76"/>
+      <c r="AF19" s="76"/>
+      <c r="AG19" s="76"/>
+      <c r="AH19" s="76"/>
+      <c r="AI19" s="76"/>
+      <c r="AJ19" s="76"/>
       <c r="AK19" s="43"/>
       <c r="AS19" s="18"/>
       <c r="AU19" s="3"/>
@@ -4277,72 +4283,72 @@
     </row>
     <row r="21" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL21" s="94">
+        <v>90</v>
+      </c>
+      <c r="AL21" s="57">
         <v>1098</v>
       </c>
-      <c r="AM21" s="85"/>
-      <c r="AN21" s="85"/>
-      <c r="AO21" s="85"/>
-      <c r="AP21" s="85"/>
-      <c r="AQ21" s="85"/>
-      <c r="AR21" s="85"/>
-      <c r="AS21" s="85"/>
-      <c r="AT21" s="85"/>
-      <c r="AU21" s="85"/>
-      <c r="AV21" s="85"/>
-      <c r="AW21" s="85"/>
-      <c r="AX21" s="85"/>
-      <c r="AY21" s="85"/>
-      <c r="AZ21" s="85"/>
-      <c r="BA21" s="85"/>
-      <c r="BB21" s="85"/>
-      <c r="BC21" s="85"/>
-      <c r="BD21" s="85"/>
-      <c r="BE21" s="85"/>
-      <c r="BF21" s="85"/>
-      <c r="BG21" s="85"/>
-      <c r="BH21" s="85"/>
-      <c r="BI21" s="85"/>
-      <c r="BJ21" s="85"/>
-      <c r="BK21" s="85"/>
-      <c r="BL21" s="85"/>
-      <c r="BM21" s="85"/>
-      <c r="BN21" s="85"/>
-      <c r="BO21" s="85"/>
-      <c r="BP21" s="85"/>
-      <c r="BQ21" s="85"/>
-      <c r="BR21" s="85">
+      <c r="AM21" s="53"/>
+      <c r="AN21" s="53"/>
+      <c r="AO21" s="53"/>
+      <c r="AP21" s="53"/>
+      <c r="AQ21" s="53"/>
+      <c r="AR21" s="53"/>
+      <c r="AS21" s="53"/>
+      <c r="AT21" s="53"/>
+      <c r="AU21" s="53"/>
+      <c r="AV21" s="53"/>
+      <c r="AW21" s="53"/>
+      <c r="AX21" s="53"/>
+      <c r="AY21" s="53"/>
+      <c r="AZ21" s="53"/>
+      <c r="BA21" s="53"/>
+      <c r="BB21" s="53"/>
+      <c r="BC21" s="53"/>
+      <c r="BD21" s="53"/>
+      <c r="BE21" s="53"/>
+      <c r="BF21" s="53"/>
+      <c r="BG21" s="53"/>
+      <c r="BH21" s="53"/>
+      <c r="BI21" s="53"/>
+      <c r="BJ21" s="53"/>
+      <c r="BK21" s="53"/>
+      <c r="BL21" s="53"/>
+      <c r="BM21" s="53"/>
+      <c r="BN21" s="53"/>
+      <c r="BO21" s="53"/>
+      <c r="BP21" s="53"/>
+      <c r="BQ21" s="53"/>
+      <c r="BR21" s="53">
         <v>26</v>
       </c>
-      <c r="BS21" s="85"/>
-      <c r="BT21" s="85"/>
-      <c r="BU21" s="85"/>
-      <c r="BV21" s="85"/>
-      <c r="BW21" s="85"/>
-      <c r="BX21" s="85"/>
-      <c r="BY21" s="85"/>
-      <c r="BZ21" s="85">
+      <c r="BS21" s="53"/>
+      <c r="BT21" s="53"/>
+      <c r="BU21" s="53"/>
+      <c r="BV21" s="53"/>
+      <c r="BW21" s="53"/>
+      <c r="BX21" s="53"/>
+      <c r="BY21" s="53"/>
+      <c r="BZ21" s="53">
         <v>137</v>
       </c>
-      <c r="CA21" s="85"/>
-      <c r="CB21" s="85"/>
-      <c r="CC21" s="85"/>
-      <c r="CD21" s="85"/>
-      <c r="CE21" s="85"/>
-      <c r="CF21" s="85"/>
-      <c r="CG21" s="85"/>
-      <c r="CH21" s="85">
+      <c r="CA21" s="53"/>
+      <c r="CB21" s="53"/>
+      <c r="CC21" s="53"/>
+      <c r="CD21" s="53"/>
+      <c r="CE21" s="53"/>
+      <c r="CF21" s="53"/>
+      <c r="CG21" s="53"/>
+      <c r="CH21" s="53">
         <v>8</v>
       </c>
-      <c r="CI21" s="85"/>
-      <c r="CJ21" s="85"/>
-      <c r="CK21" s="85"/>
-      <c r="CL21" s="85"/>
-      <c r="CM21" s="85"/>
-      <c r="CN21" s="85"/>
-      <c r="CO21" s="85"/>
+      <c r="CI21" s="53"/>
+      <c r="CJ21" s="53"/>
+      <c r="CK21" s="53"/>
+      <c r="CL21" s="53"/>
+      <c r="CM21" s="53"/>
+      <c r="CN21" s="53"/>
+      <c r="CO21" s="53"/>
     </row>
     <row r="22" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
@@ -4437,90 +4443,90 @@
       </c>
       <c r="AK22" s="10"/>
       <c r="AM22" t="s">
+        <v>193</v>
+      </c>
+      <c r="BR22" t="s">
         <v>194</v>
       </c>
-      <c r="BR22" t="s">
-        <v>195</v>
-      </c>
       <c r="BZ22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="CI22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H23" s="55">
+      <c r="H23" s="81">
         <v>18</v>
       </c>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="61"/>
-      <c r="U23" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="61"/>
-      <c r="AC23" s="59" t="s">
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="81"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="AD23" s="55"/>
-      <c r="AE23" s="55"/>
-      <c r="AF23" s="55"/>
-      <c r="AG23" s="55"/>
-      <c r="AH23" s="55"/>
-      <c r="AI23" s="55"/>
-      <c r="AJ23" s="56"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="78"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="V23" s="78"/>
+      <c r="W23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="78"/>
+      <c r="Z23" s="78"/>
+      <c r="AA23" s="78"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD23" s="81"/>
+      <c r="AE23" s="81"/>
+      <c r="AF23" s="81"/>
+      <c r="AG23" s="81"/>
+      <c r="AH23" s="81"/>
+      <c r="AI23" s="81"/>
+      <c r="AJ23" s="82"/>
       <c r="AK23" s="10"/>
       <c r="AM23" t="s">
-        <v>198</v>
-      </c>
-      <c r="BR23" s="85" t="s">
         <v>197</v>
       </c>
-      <c r="BS23" s="85"/>
-      <c r="BT23" s="85"/>
-      <c r="BU23" s="85"/>
-      <c r="BV23" s="85"/>
-      <c r="BW23" s="85"/>
-      <c r="BX23" s="85"/>
-      <c r="BY23" s="85"/>
-      <c r="BZ23" s="85">
+      <c r="BR23" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="BS23" s="53"/>
+      <c r="BT23" s="53"/>
+      <c r="BU23" s="53"/>
+      <c r="BV23" s="53"/>
+      <c r="BW23" s="53"/>
+      <c r="BX23" s="53"/>
+      <c r="BY23" s="53"/>
+      <c r="BZ23" s="53">
         <v>16</v>
       </c>
-      <c r="CA23" s="85"/>
-      <c r="CB23" s="85"/>
-      <c r="CC23" s="85"/>
-      <c r="CD23" s="85"/>
-      <c r="CE23" s="85"/>
-      <c r="CF23" s="85"/>
-      <c r="CG23" s="85"/>
-      <c r="CH23" s="85" t="s">
-        <v>196</v>
-      </c>
-      <c r="CI23" s="85"/>
-      <c r="CJ23" s="85"/>
-      <c r="CK23" s="85"/>
-      <c r="CL23" s="85"/>
-      <c r="CM23" s="85"/>
-      <c r="CN23" s="85"/>
-      <c r="CO23" s="85"/>
+      <c r="CA23" s="53"/>
+      <c r="CB23" s="53"/>
+      <c r="CC23" s="53"/>
+      <c r="CD23" s="53"/>
+      <c r="CE23" s="53"/>
+      <c r="CF23" s="53"/>
+      <c r="CG23" s="53"/>
+      <c r="CH23" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="CI23" s="53"/>
+      <c r="CJ23" s="53"/>
+      <c r="CK23" s="53"/>
+      <c r="CL23" s="53"/>
+      <c r="CM23" s="53"/>
+      <c r="CN23" s="53"/>
+      <c r="CO23" s="53"/>
     </row>
     <row r="24" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
@@ -4616,46 +4622,46 @@
       <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H25" s="55">
+      <c r="H25" s="81">
         <v>18</v>
       </c>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="60" t="s">
+      <c r="I25" s="81"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="79"/>
+      <c r="AC25" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="61"/>
-      <c r="U25" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="V25" s="54"/>
-      <c r="W25" s="54"/>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="54"/>
-      <c r="Z25" s="54"/>
-      <c r="AA25" s="54"/>
-      <c r="AB25" s="61"/>
-      <c r="AC25" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD25" s="54"/>
-      <c r="AE25" s="54"/>
-      <c r="AF25" s="54"/>
-      <c r="AG25" s="54"/>
-      <c r="AH25" s="54"/>
-      <c r="AI25" s="54"/>
-      <c r="AJ25" s="61"/>
+      <c r="AD25" s="78"/>
+      <c r="AE25" s="78"/>
+      <c r="AF25" s="78"/>
+      <c r="AG25" s="78"/>
+      <c r="AH25" s="78"/>
+      <c r="AI25" s="78"/>
+      <c r="AJ25" s="79"/>
       <c r="AK25" s="10"/>
       <c r="AM25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:102" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4784,48 +4790,48 @@
       <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H28" s="55">
+      <c r="H28" s="81">
         <v>18</v>
       </c>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="N28" s="54"/>
-      <c r="O28" s="54"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="54"/>
-      <c r="T28" s="61"/>
-      <c r="U28" s="59" t="s">
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="55"/>
-      <c r="Z28" s="55"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="56"/>
-      <c r="AC28" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD28" s="72"/>
-      <c r="AE28" s="72"/>
-      <c r="AF28" s="72"/>
-      <c r="AG28" s="72"/>
-      <c r="AH28" s="72"/>
-      <c r="AI28" s="72"/>
-      <c r="AJ28" s="73"/>
+      <c r="N28" s="78"/>
+      <c r="O28" s="78"/>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="79"/>
+      <c r="U28" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="V28" s="81"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
+      <c r="Y28" s="81"/>
+      <c r="Z28" s="81"/>
+      <c r="AA28" s="81"/>
+      <c r="AB28" s="82"/>
+      <c r="AC28" s="83" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD28" s="84"/>
+      <c r="AE28" s="84"/>
+      <c r="AF28" s="84"/>
+      <c r="AG28" s="84"/>
+      <c r="AH28" s="84"/>
+      <c r="AI28" s="84"/>
+      <c r="AJ28" s="85"/>
       <c r="AK28" s="10"/>
     </row>
     <row r="29" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H29" s="26">
         <v>0</v>
@@ -4890,61 +4896,61 @@
       <c r="AB29" s="27">
         <v>1</v>
       </c>
-      <c r="AC29" s="68" t="s">
+      <c r="AC29" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="AD29" s="69"/>
-      <c r="AE29" s="69"/>
-      <c r="AF29" s="69"/>
-      <c r="AG29" s="69"/>
-      <c r="AH29" s="69"/>
-      <c r="AI29" s="69"/>
-      <c r="AJ29" s="70"/>
+      <c r="AD29" s="95"/>
+      <c r="AE29" s="95"/>
+      <c r="AF29" s="95"/>
+      <c r="AG29" s="95"/>
+      <c r="AH29" s="95"/>
+      <c r="AI29" s="95"/>
+      <c r="AJ29" s="96"/>
       <c r="AK29" s="10"/>
     </row>
     <row r="30" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H30" s="54" t="s">
+      <c r="H30" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="N30" s="78"/>
+      <c r="O30" s="78"/>
+      <c r="P30" s="78"/>
+      <c r="Q30" s="78"/>
+      <c r="R30" s="78"/>
+      <c r="S30" s="78"/>
+      <c r="T30" s="79"/>
+      <c r="U30" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="61"/>
-      <c r="U30" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="61"/>
-      <c r="AC30" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD30" s="55"/>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="55"/>
-      <c r="AG30" s="55"/>
-      <c r="AH30" s="55"/>
-      <c r="AI30" s="55"/>
-      <c r="AJ30" s="56"/>
+      <c r="V30" s="78"/>
+      <c r="W30" s="78"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="78"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="78"/>
+      <c r="AB30" s="79"/>
+      <c r="AC30" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD30" s="81"/>
+      <c r="AE30" s="81"/>
+      <c r="AF30" s="81"/>
+      <c r="AG30" s="81"/>
+      <c r="AH30" s="81"/>
+      <c r="AI30" s="81"/>
+      <c r="AJ30" s="82"/>
       <c r="AK30" s="10"/>
     </row>
     <row r="31" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H31" s="29">
         <v>0</v>
@@ -5036,43 +5042,43 @@
       <c r="AK31" s="10"/>
     </row>
     <row r="32" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="H32" s="54" t="s">
+      <c r="H32" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="N32" s="89"/>
+      <c r="O32" s="89"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="90"/>
+      <c r="U32" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="V32" s="63"/>
-      <c r="W32" s="63"/>
-      <c r="X32" s="63"/>
-      <c r="Y32" s="63"/>
-      <c r="Z32" s="63"/>
-      <c r="AA32" s="63"/>
-      <c r="AB32" s="64"/>
-      <c r="AC32" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD32" s="66"/>
-      <c r="AE32" s="66"/>
-      <c r="AF32" s="66"/>
-      <c r="AG32" s="66"/>
-      <c r="AH32" s="66"/>
-      <c r="AI32" s="66"/>
-      <c r="AJ32" s="67"/>
+      <c r="V32" s="89"/>
+      <c r="W32" s="89"/>
+      <c r="X32" s="89"/>
+      <c r="Y32" s="89"/>
+      <c r="Z32" s="89"/>
+      <c r="AA32" s="89"/>
+      <c r="AB32" s="90"/>
+      <c r="AC32" s="91" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD32" s="92"/>
+      <c r="AE32" s="92"/>
+      <c r="AF32" s="92"/>
+      <c r="AG32" s="92"/>
+      <c r="AH32" s="92"/>
+      <c r="AI32" s="92"/>
+      <c r="AJ32" s="93"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -5083,28 +5089,47 @@
     <sortCondition ref="L3:L15"/>
   </sortState>
   <mergeCells count="78">
-    <mergeCell ref="BR23:BY23"/>
-    <mergeCell ref="BZ23:CG23"/>
-    <mergeCell ref="CH23:CO23"/>
-    <mergeCell ref="BR21:BY21"/>
-    <mergeCell ref="BZ21:CG21"/>
-    <mergeCell ref="CH21:CO21"/>
-    <mergeCell ref="AL14:BA14"/>
-    <mergeCell ref="CH8:CO8"/>
-    <mergeCell ref="AL21:BQ21"/>
-    <mergeCell ref="AT4:BY4"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="BR15:BY15"/>
-    <mergeCell ref="BZ15:CG15"/>
-    <mergeCell ref="U18:AB18"/>
-    <mergeCell ref="AL16:AS16"/>
-    <mergeCell ref="AT16:BA16"/>
-    <mergeCell ref="BJ16:BQ16"/>
-    <mergeCell ref="BB16:BI16"/>
-    <mergeCell ref="M7:T7"/>
-    <mergeCell ref="AV8:BE8"/>
-    <mergeCell ref="BF8:BQ8"/>
-    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="CH8:CW8"/>
+    <mergeCell ref="CH17:CW17"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="AL13:BQ13"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="AC30:AJ30"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="M30:T30"/>
+    <mergeCell ref="M32:T32"/>
+    <mergeCell ref="U32:AB32"/>
+    <mergeCell ref="AC32:AJ32"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="AC29:AJ29"/>
+    <mergeCell ref="AC23:AJ23"/>
+    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="AC19:AJ19"/>
+    <mergeCell ref="M23:T23"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="M28:T28"/>
+    <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="AC28:AJ28"/>
+    <mergeCell ref="AC25:AJ25"/>
+    <mergeCell ref="U25:AB25"/>
+    <mergeCell ref="CH15:CO15"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="AL1:CW1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="S1:AJ1"/>
+    <mergeCell ref="AL7:AS7"/>
+    <mergeCell ref="AL17:BQ17"/>
+    <mergeCell ref="BB14:BY14"/>
+    <mergeCell ref="U19:AB19"/>
+    <mergeCell ref="M19:T19"/>
+    <mergeCell ref="AL8:AU8"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="BR8:CG8"/>
+    <mergeCell ref="AL12:AS12"/>
+    <mergeCell ref="AL15:BQ15"/>
     <mergeCell ref="AL11:AS11"/>
     <mergeCell ref="CP15:CW15"/>
     <mergeCell ref="M9:T9"/>
@@ -5121,46 +5146,27 @@
     <mergeCell ref="U16:AB16"/>
     <mergeCell ref="U17:AB17"/>
     <mergeCell ref="U14:AB14"/>
-    <mergeCell ref="CH15:CO15"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="AL1:CW1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:R1"/>
-    <mergeCell ref="S1:AJ1"/>
-    <mergeCell ref="AL7:AS7"/>
-    <mergeCell ref="AL17:BQ17"/>
-    <mergeCell ref="BB14:BY14"/>
-    <mergeCell ref="U19:AB19"/>
-    <mergeCell ref="M19:T19"/>
-    <mergeCell ref="AL8:AU8"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="BR8:CG8"/>
-    <mergeCell ref="AL12:AS12"/>
-    <mergeCell ref="AL15:BQ15"/>
-    <mergeCell ref="AC19:AJ19"/>
-    <mergeCell ref="M23:T23"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="M28:T28"/>
-    <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="AC28:AJ28"/>
-    <mergeCell ref="AC25:AJ25"/>
-    <mergeCell ref="U25:AB25"/>
-    <mergeCell ref="CH17:CW17"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="AL13:BQ13"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="AC30:AJ30"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="M30:T30"/>
-    <mergeCell ref="M32:T32"/>
-    <mergeCell ref="U32:AB32"/>
-    <mergeCell ref="AC32:AJ32"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="AC29:AJ29"/>
-    <mergeCell ref="AC23:AJ23"/>
-    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="AL14:BA14"/>
+    <mergeCell ref="AL21:BQ21"/>
+    <mergeCell ref="AT4:BY4"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="BR15:BY15"/>
+    <mergeCell ref="BZ15:CG15"/>
+    <mergeCell ref="U18:AB18"/>
+    <mergeCell ref="AL16:AS16"/>
+    <mergeCell ref="AT16:BA16"/>
+    <mergeCell ref="BJ16:BQ16"/>
+    <mergeCell ref="BB16:BI16"/>
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="AV8:BE8"/>
+    <mergeCell ref="BF8:BQ8"/>
+    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="BR23:BY23"/>
+    <mergeCell ref="BZ23:CG23"/>
+    <mergeCell ref="CH23:CO23"/>
+    <mergeCell ref="BR21:BY21"/>
+    <mergeCell ref="BZ21:CG21"/>
+    <mergeCell ref="CH21:CO21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5419,226 +5425,226 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" t="s">
-        <v>131</v>
-      </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
         <v>132</v>
       </c>
-      <c r="F3" t="s">
-        <v>133</v>
-      </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
         <v>134</v>
       </c>
-      <c r="F4" t="s">
-        <v>135</v>
-      </c>
       <c r="G4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" t="s">
         <v>164</v>
-      </c>
-      <c r="H4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" t="s">
         <v>136</v>
       </c>
-      <c r="F5" t="s">
-        <v>137</v>
-      </c>
       <c r="G5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" t="s">
         <v>166</v>
-      </c>
-      <c r="H5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
         <v>138</v>
       </c>
-      <c r="F6" t="s">
-        <v>139</v>
-      </c>
       <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" t="s">
         <v>168</v>
-      </c>
-      <c r="H6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
         <v>140</v>
       </c>
-      <c r="F7" t="s">
-        <v>141</v>
-      </c>
       <c r="G7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" t="s">
         <v>170</v>
-      </c>
-      <c r="H7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" t="s">
         <v>142</v>
       </c>
-      <c r="F8" t="s">
-        <v>143</v>
-      </c>
       <c r="G8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H8" t="s">
         <v>172</v>
-      </c>
-      <c r="H8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" t="s">
         <v>144</v>
       </c>
-      <c r="F9" t="s">
-        <v>145</v>
-      </c>
       <c r="G9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" t="s">
         <v>174</v>
-      </c>
-      <c r="H9" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" t="s">
         <v>146</v>
       </c>
-      <c r="F10" t="s">
-        <v>147</v>
-      </c>
       <c r="G10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" t="s">
         <v>176</v>
-      </c>
-      <c r="H10" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" t="s">
         <v>148</v>
       </c>
-      <c r="F11" t="s">
-        <v>149</v>
-      </c>
       <c r="G11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" t="s">
         <v>178</v>
-      </c>
-      <c r="H11" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
         <v>150</v>
       </c>
-      <c r="F12" t="s">
-        <v>151</v>
-      </c>
       <c r="G12" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" t="s">
         <v>180</v>
-      </c>
-      <c r="H12" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" t="s">
         <v>152</v>
       </c>
-      <c r="F13" t="s">
-        <v>153</v>
-      </c>
       <c r="G13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13" t="s">
         <v>182</v>
-      </c>
-      <c r="H13" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" t="s">
         <v>154</v>
       </c>
-      <c r="F14" t="s">
-        <v>155</v>
-      </c>
       <c r="G14" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" t="s">
         <v>184</v>
-      </c>
-      <c r="H14" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" t="s">
         <v>156</v>
       </c>
-      <c r="F15" t="s">
-        <v>157</v>
-      </c>
       <c r="G15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" t="s">
         <v>186</v>
-      </c>
-      <c r="H15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" t="s">
         <v>158</v>
       </c>
-      <c r="F16" t="s">
-        <v>159</v>
-      </c>
       <c r="G16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H16" t="s">
         <v>188</v>
-      </c>
-      <c r="H16" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" t="s">
         <v>160</v>
       </c>
-      <c r="F17" t="s">
-        <v>161</v>
-      </c>
       <c r="G17" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" t="s">
         <v>190</v>
-      </c>
-      <c r="H17" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Start/stop Sensor eingebaut -automatisches Einlesen der Config vorbereitet
</commit_message>
<xml_diff>
--- a/04_Busprotokoll/CAN-Messages.xlsx
+++ b/04_Busprotokoll/CAN-Messages.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="160" windowWidth="24240" windowHeight="15040"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="MessageTypen" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">MessageTypen!$A$1:$AJ$19</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1118,13 +1118,104 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1133,19 +1224,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1175,100 +1266,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1570,151 +1570,151 @@
   <dimension ref="A1:CX32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AJ1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="76.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="36" width="1.83203125" customWidth="1"/>
-    <col min="37" max="37" width="0.6640625" style="8" customWidth="1"/>
-    <col min="38" max="101" width="1.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="36" width="1.85546875" customWidth="1"/>
+    <col min="37" max="37" width="0.7109375" style="8" customWidth="1"/>
+    <col min="38" max="101" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" ht="15" thickBot="1">
-      <c r="A1" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="95"/>
+    <row r="1" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="76"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="103"/>
-      <c r="W1" s="103"/>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="103"/>
-      <c r="AC1" s="103"/>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="103"/>
-      <c r="AI1" s="103"/>
-      <c r="AJ1" s="103"/>
-      <c r="AK1" s="102"/>
-      <c r="AL1" s="77" t="s">
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="77"/>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="77"/>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="77"/>
-      <c r="BF1" s="77"/>
-      <c r="BG1" s="77"/>
-      <c r="BH1" s="77"/>
-      <c r="BI1" s="77"/>
-      <c r="BJ1" s="77"/>
-      <c r="BK1" s="77"/>
-      <c r="BL1" s="77"/>
-      <c r="BM1" s="77"/>
-      <c r="BN1" s="77"/>
-      <c r="BO1" s="77"/>
-      <c r="BP1" s="77"/>
-      <c r="BQ1" s="77"/>
-      <c r="BR1" s="77"/>
-      <c r="BS1" s="77"/>
-      <c r="BT1" s="77"/>
-      <c r="BU1" s="77"/>
-      <c r="BV1" s="77"/>
-      <c r="BW1" s="77"/>
-      <c r="BX1" s="77"/>
-      <c r="BY1" s="77"/>
-      <c r="BZ1" s="77"/>
-      <c r="CA1" s="77"/>
-      <c r="CB1" s="77"/>
-      <c r="CC1" s="77"/>
-      <c r="CD1" s="77"/>
-      <c r="CE1" s="77"/>
-      <c r="CF1" s="77"/>
-      <c r="CG1" s="77"/>
-      <c r="CH1" s="77"/>
-      <c r="CI1" s="77"/>
-      <c r="CJ1" s="77"/>
-      <c r="CK1" s="77"/>
-      <c r="CL1" s="77"/>
-      <c r="CM1" s="77"/>
-      <c r="CN1" s="77"/>
-      <c r="CO1" s="77"/>
-      <c r="CP1" s="77"/>
-      <c r="CQ1" s="77"/>
-      <c r="CR1" s="77"/>
-      <c r="CS1" s="77"/>
-      <c r="CT1" s="77"/>
-      <c r="CU1" s="77"/>
-      <c r="CV1" s="77"/>
-      <c r="CW1" s="77"/>
+      <c r="AM1" s="73"/>
+      <c r="AN1" s="73"/>
+      <c r="AO1" s="73"/>
+      <c r="AP1" s="73"/>
+      <c r="AQ1" s="73"/>
+      <c r="AR1" s="73"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="73"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="73"/>
+      <c r="AW1" s="73"/>
+      <c r="AX1" s="73"/>
+      <c r="AY1" s="73"/>
+      <c r="AZ1" s="73"/>
+      <c r="BA1" s="73"/>
+      <c r="BB1" s="73"/>
+      <c r="BC1" s="73"/>
+      <c r="BD1" s="73"/>
+      <c r="BE1" s="73"/>
+      <c r="BF1" s="73"/>
+      <c r="BG1" s="73"/>
+      <c r="BH1" s="73"/>
+      <c r="BI1" s="73"/>
+      <c r="BJ1" s="73"/>
+      <c r="BK1" s="73"/>
+      <c r="BL1" s="73"/>
+      <c r="BM1" s="73"/>
+      <c r="BN1" s="73"/>
+      <c r="BO1" s="73"/>
+      <c r="BP1" s="73"/>
+      <c r="BQ1" s="73"/>
+      <c r="BR1" s="73"/>
+      <c r="BS1" s="73"/>
+      <c r="BT1" s="73"/>
+      <c r="BU1" s="73"/>
+      <c r="BV1" s="73"/>
+      <c r="BW1" s="73"/>
+      <c r="BX1" s="73"/>
+      <c r="BY1" s="73"/>
+      <c r="BZ1" s="73"/>
+      <c r="CA1" s="73"/>
+      <c r="CB1" s="73"/>
+      <c r="CC1" s="73"/>
+      <c r="CD1" s="73"/>
+      <c r="CE1" s="73"/>
+      <c r="CF1" s="73"/>
+      <c r="CG1" s="73"/>
+      <c r="CH1" s="73"/>
+      <c r="CI1" s="73"/>
+      <c r="CJ1" s="73"/>
+      <c r="CK1" s="73"/>
+      <c r="CL1" s="73"/>
+      <c r="CM1" s="73"/>
+      <c r="CN1" s="73"/>
+      <c r="CO1" s="73"/>
+      <c r="CP1" s="73"/>
+      <c r="CQ1" s="73"/>
+      <c r="CR1" s="73"/>
+      <c r="CS1" s="73"/>
+      <c r="CT1" s="73"/>
+      <c r="CU1" s="73"/>
+      <c r="CV1" s="73"/>
+      <c r="CW1" s="73"/>
       <c r="CX1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:102">
-      <c r="A2" s="101" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="101" t="s">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="55" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -2007,20 +2007,20 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:102">
-      <c r="A3" s="100" t="s">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="54" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="10">
@@ -2127,20 +2127,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:102">
-      <c r="A4" s="96" t="s">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="52" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
@@ -2233,50 +2233,50 @@
       <c r="AJ4" s="40">
         <v>1</v>
       </c>
-      <c r="AL4" s="78" t="s">
+      <c r="AL4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="AM4" s="52"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="52"/>
-      <c r="AP4" s="52"/>
-      <c r="AQ4" s="52"/>
-      <c r="AR4" s="52"/>
-      <c r="AS4" s="52"/>
-      <c r="AT4" s="92" t="s">
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="AU4" s="92"/>
-      <c r="AV4" s="92"/>
-      <c r="AW4" s="92"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="92"/>
-      <c r="AZ4" s="92"/>
-      <c r="BA4" s="92"/>
-      <c r="BB4" s="92"/>
-      <c r="BC4" s="92"/>
-      <c r="BD4" s="92"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="92"/>
-      <c r="BG4" s="92"/>
-      <c r="BH4" s="92"/>
-      <c r="BI4" s="92"/>
-      <c r="BJ4" s="92"/>
-      <c r="BK4" s="92"/>
-      <c r="BL4" s="92"/>
-      <c r="BM4" s="92"/>
-      <c r="BN4" s="92"/>
-      <c r="BO4" s="92"/>
-      <c r="BP4" s="92"/>
-      <c r="BQ4" s="92"/>
-      <c r="BR4" s="92"/>
-      <c r="BS4" s="92"/>
-      <c r="BT4" s="92"/>
-      <c r="BU4" s="92"/>
-      <c r="BV4" s="92"/>
-      <c r="BW4" s="92"/>
-      <c r="BX4" s="92"/>
-      <c r="BY4" s="92"/>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="62"/>
+      <c r="AY4" s="62"/>
+      <c r="AZ4" s="62"/>
+      <c r="BA4" s="62"/>
+      <c r="BB4" s="62"/>
+      <c r="BC4" s="62"/>
+      <c r="BD4" s="62"/>
+      <c r="BE4" s="62"/>
+      <c r="BF4" s="62"/>
+      <c r="BG4" s="62"/>
+      <c r="BH4" s="62"/>
+      <c r="BI4" s="62"/>
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="62"/>
+      <c r="BM4" s="62"/>
+      <c r="BN4" s="62"/>
+      <c r="BO4" s="62"/>
+      <c r="BP4" s="62"/>
+      <c r="BQ4" s="62"/>
+      <c r="BR4" s="62"/>
+      <c r="BS4" s="62"/>
+      <c r="BT4" s="62"/>
+      <c r="BU4" s="62"/>
+      <c r="BV4" s="62"/>
+      <c r="BW4" s="62"/>
+      <c r="BX4" s="62"/>
+      <c r="BY4" s="62"/>
       <c r="CG4" s="17"/>
       <c r="CI4" s="3"/>
       <c r="CO4" s="17"/>
@@ -2286,20 +2286,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:102" hidden="1">
-      <c r="A5" s="96" t="s">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="52" t="s">
         <v>116</v>
       </c>
       <c r="G5" t="s">
@@ -2409,20 +2409,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:102" hidden="1">
-      <c r="A6" s="97" t="s">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="53" t="s">
         <v>124</v>
       </c>
       <c r="F6" s="31"/>
@@ -2572,20 +2572,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:102" hidden="1">
-      <c r="A7" s="96" t="s">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="52" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
@@ -2606,16 +2606,16 @@
       <c r="L7" s="11">
         <v>0</v>
       </c>
-      <c r="M7" s="84" t="s">
+      <c r="M7" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="84"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
       <c r="U7" s="13">
         <v>0</v>
       </c>
@@ -2664,16 +2664,16 @@
       <c r="AJ7" s="40">
         <v>1</v>
       </c>
-      <c r="AL7" s="78" t="s">
+      <c r="AL7" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="AM7" s="52"/>
-      <c r="AN7" s="52"/>
-      <c r="AO7" s="52"/>
-      <c r="AP7" s="52"/>
-      <c r="AQ7" s="52"/>
-      <c r="AR7" s="52"/>
-      <c r="AS7" s="52"/>
+      <c r="AM7" s="66"/>
+      <c r="AN7" s="66"/>
+      <c r="AO7" s="66"/>
+      <c r="AP7" s="66"/>
+      <c r="AQ7" s="66"/>
+      <c r="AR7" s="66"/>
+      <c r="AS7" s="66"/>
       <c r="AU7" s="3"/>
       <c r="BA7" s="17"/>
       <c r="BE7" s="3"/>
@@ -2690,20 +2690,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:102" hidden="1">
-      <c r="A8" s="96" t="s">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="52" t="s">
         <v>16</v>
       </c>
       <c r="G8" t="s">
@@ -2724,16 +2724,16 @@
       <c r="L8" s="11">
         <v>1</v>
       </c>
-      <c r="M8" s="84" t="s">
+      <c r="M8" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="84"/>
-      <c r="S8" s="84"/>
-      <c r="T8" s="84"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
       <c r="U8" s="13">
         <v>0</v>
       </c>
@@ -2782,98 +2782,98 @@
       <c r="AJ8" s="40">
         <v>1</v>
       </c>
-      <c r="AL8" s="81" t="s">
+      <c r="AL8" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="AM8" s="82"/>
-      <c r="AN8" s="82"/>
-      <c r="AO8" s="82"/>
-      <c r="AP8" s="82"/>
-      <c r="AQ8" s="82"/>
-      <c r="AR8" s="82"/>
-      <c r="AS8" s="82"/>
-      <c r="AT8" s="82"/>
-      <c r="AU8" s="82"/>
-      <c r="AV8" s="94" t="s">
+      <c r="AM8" s="81"/>
+      <c r="AN8" s="81"/>
+      <c r="AO8" s="81"/>
+      <c r="AP8" s="81"/>
+      <c r="AQ8" s="81"/>
+      <c r="AR8" s="81"/>
+      <c r="AS8" s="81"/>
+      <c r="AT8" s="81"/>
+      <c r="AU8" s="81"/>
+      <c r="AV8" s="64" t="s">
         <v>199</v>
       </c>
-      <c r="AW8" s="94"/>
-      <c r="AX8" s="94"/>
-      <c r="AY8" s="94"/>
-      <c r="AZ8" s="94"/>
-      <c r="BA8" s="94"/>
-      <c r="BB8" s="94"/>
-      <c r="BC8" s="94"/>
-      <c r="BD8" s="94"/>
-      <c r="BE8" s="94"/>
-      <c r="BF8" s="53" t="s">
+      <c r="AW8" s="64"/>
+      <c r="AX8" s="64"/>
+      <c r="AY8" s="64"/>
+      <c r="AZ8" s="64"/>
+      <c r="BA8" s="64"/>
+      <c r="BB8" s="64"/>
+      <c r="BC8" s="64"/>
+      <c r="BD8" s="64"/>
+      <c r="BE8" s="64"/>
+      <c r="BF8" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="BG8" s="53"/>
-      <c r="BH8" s="53"/>
-      <c r="BI8" s="53"/>
-      <c r="BJ8" s="53"/>
-      <c r="BK8" s="53"/>
-      <c r="BL8" s="53"/>
-      <c r="BM8" s="53"/>
-      <c r="BN8" s="53"/>
-      <c r="BO8" s="53"/>
-      <c r="BP8" s="53"/>
-      <c r="BQ8" s="53"/>
-      <c r="BR8" s="83" t="s">
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65"/>
+      <c r="BL8" s="65"/>
+      <c r="BM8" s="65"/>
+      <c r="BN8" s="65"/>
+      <c r="BO8" s="65"/>
+      <c r="BP8" s="65"/>
+      <c r="BQ8" s="65"/>
+      <c r="BR8" s="82" t="s">
         <v>127</v>
       </c>
-      <c r="BS8" s="83"/>
-      <c r="BT8" s="83"/>
-      <c r="BU8" s="83"/>
-      <c r="BV8" s="83"/>
-      <c r="BW8" s="83"/>
-      <c r="BX8" s="83"/>
-      <c r="BY8" s="83"/>
-      <c r="BZ8" s="83"/>
-      <c r="CA8" s="83"/>
-      <c r="CB8" s="83"/>
-      <c r="CC8" s="83"/>
-      <c r="CD8" s="83"/>
-      <c r="CE8" s="83"/>
-      <c r="CF8" s="83"/>
-      <c r="CG8" s="83"/>
-      <c r="CH8" s="52" t="s">
+      <c r="BS8" s="82"/>
+      <c r="BT8" s="82"/>
+      <c r="BU8" s="82"/>
+      <c r="BV8" s="82"/>
+      <c r="BW8" s="82"/>
+      <c r="BX8" s="82"/>
+      <c r="BY8" s="82"/>
+      <c r="BZ8" s="82"/>
+      <c r="CA8" s="82"/>
+      <c r="CB8" s="82"/>
+      <c r="CC8" s="82"/>
+      <c r="CD8" s="82"/>
+      <c r="CE8" s="82"/>
+      <c r="CF8" s="82"/>
+      <c r="CG8" s="82"/>
+      <c r="CH8" s="66" t="s">
         <v>200</v>
       </c>
-      <c r="CI8" s="52"/>
-      <c r="CJ8" s="52"/>
-      <c r="CK8" s="52"/>
-      <c r="CL8" s="52"/>
-      <c r="CM8" s="52"/>
-      <c r="CN8" s="52"/>
-      <c r="CO8" s="52"/>
-      <c r="CP8" s="52"/>
-      <c r="CQ8" s="52"/>
-      <c r="CR8" s="52"/>
-      <c r="CS8" s="52"/>
-      <c r="CT8" s="52"/>
-      <c r="CU8" s="52"/>
-      <c r="CV8" s="52"/>
-      <c r="CW8" s="52"/>
+      <c r="CI8" s="66"/>
+      <c r="CJ8" s="66"/>
+      <c r="CK8" s="66"/>
+      <c r="CL8" s="66"/>
+      <c r="CM8" s="66"/>
+      <c r="CN8" s="66"/>
+      <c r="CO8" s="66"/>
+      <c r="CP8" s="66"/>
+      <c r="CQ8" s="66"/>
+      <c r="CR8" s="66"/>
+      <c r="CS8" s="66"/>
+      <c r="CT8" s="66"/>
+      <c r="CU8" s="66"/>
+      <c r="CV8" s="66"/>
+      <c r="CW8" s="66"/>
       <c r="CX8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:102" hidden="1">
-      <c r="A9" s="97" t="s">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="53" t="s">
         <v>126</v>
       </c>
       <c r="F9" s="31"/>
@@ -2895,16 +2895,16 @@
       <c r="L9" s="33">
         <v>0</v>
       </c>
-      <c r="M9" s="84" t="s">
+      <c r="M9" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="84"/>
-      <c r="T9" s="84"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
       <c r="U9" s="34">
         <v>0</v>
       </c>
@@ -3009,20 +3009,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:102" hidden="1">
-      <c r="A10" s="97" t="s">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="53" t="s">
         <v>125</v>
       </c>
       <c r="F10" s="31"/>
@@ -3172,20 +3172,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:102">
-      <c r="A11" s="96" t="s">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="96" t="s">
+      <c r="C11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="52" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
@@ -3206,16 +3206,16 @@
       <c r="L11" s="11">
         <v>0</v>
       </c>
-      <c r="M11" s="84" t="s">
+      <c r="M11" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="N11" s="84"/>
-      <c r="O11" s="84"/>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="84"/>
-      <c r="R11" s="84"/>
-      <c r="S11" s="84"/>
-      <c r="T11" s="84"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
       <c r="U11" s="13">
         <v>0</v>
       </c>
@@ -3264,16 +3264,16 @@
       <c r="AJ11" s="40">
         <v>1</v>
       </c>
-      <c r="AL11" s="78" t="s">
+      <c r="AL11" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="AM11" s="52"/>
-      <c r="AN11" s="52"/>
-      <c r="AO11" s="52"/>
-      <c r="AP11" s="52"/>
-      <c r="AQ11" s="52"/>
-      <c r="AR11" s="52"/>
-      <c r="AS11" s="52"/>
+      <c r="AM11" s="66"/>
+      <c r="AN11" s="66"/>
+      <c r="AO11" s="66"/>
+      <c r="AP11" s="66"/>
+      <c r="AQ11" s="66"/>
+      <c r="AR11" s="66"/>
+      <c r="AS11" s="66"/>
       <c r="AU11" s="3"/>
       <c r="BA11" s="17"/>
       <c r="BE11" s="3"/>
@@ -3290,20 +3290,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:102">
-      <c r="A12" s="96" t="s">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="96" t="s">
+      <c r="E12" s="52" t="s">
         <v>15</v>
       </c>
       <c r="G12" t="s">
@@ -3396,16 +3396,16 @@
       <c r="AJ12" s="47">
         <v>1</v>
       </c>
-      <c r="AL12" s="78" t="s">
+      <c r="AL12" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="AM12" s="52"/>
-      <c r="AN12" s="52"/>
-      <c r="AO12" s="52"/>
-      <c r="AP12" s="52"/>
-      <c r="AQ12" s="52"/>
-      <c r="AR12" s="52"/>
-      <c r="AS12" s="52"/>
+      <c r="AM12" s="66"/>
+      <c r="AN12" s="66"/>
+      <c r="AO12" s="66"/>
+      <c r="AP12" s="66"/>
+      <c r="AQ12" s="66"/>
+      <c r="AR12" s="66"/>
+      <c r="AS12" s="66"/>
       <c r="AU12" s="3"/>
       <c r="BA12" s="17"/>
       <c r="BE12" s="3"/>
@@ -3422,20 +3422,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:102">
-      <c r="A13" s="96" t="s">
+    <row r="13" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="96" t="s">
+      <c r="C13" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E13" s="52" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="22"/>
@@ -3530,40 +3530,40 @@
         <v>1</v>
       </c>
       <c r="AK13" s="48"/>
-      <c r="AL13" s="57" t="s">
+      <c r="AL13" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="AM13" s="58"/>
-      <c r="AN13" s="58"/>
-      <c r="AO13" s="58"/>
-      <c r="AP13" s="58"/>
-      <c r="AQ13" s="58"/>
-      <c r="AR13" s="58"/>
-      <c r="AS13" s="58"/>
-      <c r="AT13" s="58"/>
-      <c r="AU13" s="58"/>
-      <c r="AV13" s="58"/>
-      <c r="AW13" s="58"/>
-      <c r="AX13" s="58"/>
-      <c r="AY13" s="58"/>
-      <c r="AZ13" s="58"/>
-      <c r="BA13" s="58"/>
-      <c r="BB13" s="58"/>
-      <c r="BC13" s="58"/>
-      <c r="BD13" s="58"/>
-      <c r="BE13" s="58"/>
-      <c r="BF13" s="58"/>
-      <c r="BG13" s="58"/>
-      <c r="BH13" s="58"/>
-      <c r="BI13" s="58"/>
-      <c r="BJ13" s="58"/>
-      <c r="BK13" s="58"/>
-      <c r="BL13" s="58"/>
-      <c r="BM13" s="58"/>
-      <c r="BN13" s="58"/>
-      <c r="BO13" s="58"/>
-      <c r="BP13" s="58"/>
-      <c r="BQ13" s="58"/>
+      <c r="AM13" s="94"/>
+      <c r="AN13" s="94"/>
+      <c r="AO13" s="94"/>
+      <c r="AP13" s="94"/>
+      <c r="AQ13" s="94"/>
+      <c r="AR13" s="94"/>
+      <c r="AS13" s="94"/>
+      <c r="AT13" s="94"/>
+      <c r="AU13" s="94"/>
+      <c r="AV13" s="94"/>
+      <c r="AW13" s="94"/>
+      <c r="AX13" s="94"/>
+      <c r="AY13" s="94"/>
+      <c r="AZ13" s="94"/>
+      <c r="BA13" s="94"/>
+      <c r="BB13" s="94"/>
+      <c r="BC13" s="94"/>
+      <c r="BD13" s="94"/>
+      <c r="BE13" s="94"/>
+      <c r="BF13" s="94"/>
+      <c r="BG13" s="94"/>
+      <c r="BH13" s="94"/>
+      <c r="BI13" s="94"/>
+      <c r="BJ13" s="94"/>
+      <c r="BK13" s="94"/>
+      <c r="BL13" s="94"/>
+      <c r="BM13" s="94"/>
+      <c r="BN13" s="94"/>
+      <c r="BO13" s="94"/>
+      <c r="BP13" s="94"/>
+      <c r="BQ13" s="94"/>
       <c r="BR13" s="22"/>
       <c r="BS13" s="22"/>
       <c r="BT13" s="22"/>
@@ -3600,20 +3600,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:102">
-      <c r="A14" s="96" t="s">
+    <row r="14" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="52" t="s">
         <v>123</v>
       </c>
       <c r="G14" t="s">
@@ -3658,16 +3658,16 @@
       <c r="T14" s="14">
         <v>1</v>
       </c>
-      <c r="U14" s="87" t="s">
+      <c r="U14" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="V14" s="87"/>
-      <c r="W14" s="87"/>
-      <c r="X14" s="87"/>
-      <c r="Y14" s="87"/>
-      <c r="Z14" s="87"/>
-      <c r="AA14" s="87"/>
-      <c r="AB14" s="87"/>
+      <c r="V14" s="69"/>
+      <c r="W14" s="69"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
       <c r="AC14" s="12">
         <v>0</v>
       </c>
@@ -3692,50 +3692,50 @@
       <c r="AJ14" s="40">
         <v>1</v>
       </c>
-      <c r="AL14" s="78" t="s">
+      <c r="AL14" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="AM14" s="90"/>
-      <c r="AN14" s="90"/>
-      <c r="AO14" s="90"/>
-      <c r="AP14" s="90"/>
-      <c r="AQ14" s="90"/>
-      <c r="AR14" s="90"/>
-      <c r="AS14" s="90"/>
-      <c r="AT14" s="90"/>
-      <c r="AU14" s="90"/>
-      <c r="AV14" s="90"/>
-      <c r="AW14" s="90"/>
-      <c r="AX14" s="90"/>
-      <c r="AY14" s="90"/>
-      <c r="AZ14" s="90"/>
-      <c r="BA14" s="90"/>
-      <c r="BB14" s="53" t="s">
+      <c r="AM14" s="60"/>
+      <c r="AN14" s="60"/>
+      <c r="AO14" s="60"/>
+      <c r="AP14" s="60"/>
+      <c r="AQ14" s="60"/>
+      <c r="AR14" s="60"/>
+      <c r="AS14" s="60"/>
+      <c r="AT14" s="60"/>
+      <c r="AU14" s="60"/>
+      <c r="AV14" s="60"/>
+      <c r="AW14" s="60"/>
+      <c r="AX14" s="60"/>
+      <c r="AY14" s="60"/>
+      <c r="AZ14" s="60"/>
+      <c r="BA14" s="60"/>
+      <c r="BB14" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="BC14" s="53"/>
-      <c r="BD14" s="53"/>
-      <c r="BE14" s="53"/>
-      <c r="BF14" s="53"/>
-      <c r="BG14" s="53"/>
-      <c r="BH14" s="53"/>
-      <c r="BI14" s="53"/>
-      <c r="BJ14" s="53"/>
-      <c r="BK14" s="53"/>
-      <c r="BL14" s="53"/>
-      <c r="BM14" s="53"/>
-      <c r="BN14" s="53"/>
-      <c r="BO14" s="53"/>
-      <c r="BP14" s="53"/>
-      <c r="BQ14" s="53"/>
-      <c r="BR14" s="53"/>
-      <c r="BS14" s="53"/>
-      <c r="BT14" s="53"/>
-      <c r="BU14" s="53"/>
-      <c r="BV14" s="53"/>
-      <c r="BW14" s="53"/>
-      <c r="BX14" s="53"/>
-      <c r="BY14" s="53"/>
+      <c r="BC14" s="65"/>
+      <c r="BD14" s="65"/>
+      <c r="BE14" s="65"/>
+      <c r="BF14" s="65"/>
+      <c r="BG14" s="65"/>
+      <c r="BH14" s="65"/>
+      <c r="BI14" s="65"/>
+      <c r="BJ14" s="65"/>
+      <c r="BK14" s="65"/>
+      <c r="BL14" s="65"/>
+      <c r="BM14" s="65"/>
+      <c r="BN14" s="65"/>
+      <c r="BO14" s="65"/>
+      <c r="BP14" s="65"/>
+      <c r="BQ14" s="65"/>
+      <c r="BR14" s="65"/>
+      <c r="BS14" s="65"/>
+      <c r="BT14" s="65"/>
+      <c r="BU14" s="65"/>
+      <c r="BV14" s="65"/>
+      <c r="BW14" s="65"/>
+      <c r="BX14" s="65"/>
+      <c r="BY14" s="65"/>
       <c r="CG14" s="17"/>
       <c r="CI14" s="3"/>
       <c r="CO14" s="17"/>
@@ -3745,20 +3745,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:102">
-      <c r="A15" s="96" t="s">
+    <row r="15" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="96" t="s">
+      <c r="D15" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="52" t="s">
         <v>11</v>
       </c>
       <c r="F15" t="s">
@@ -3806,118 +3806,118 @@
       <c r="T15" s="14">
         <v>1</v>
       </c>
-      <c r="U15" s="87" t="s">
+      <c r="U15" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="V15" s="87"/>
-      <c r="W15" s="87"/>
-      <c r="X15" s="87"/>
-      <c r="Y15" s="87"/>
-      <c r="Z15" s="87"/>
-      <c r="AA15" s="87"/>
-      <c r="AB15" s="87"/>
-      <c r="AC15" s="88" t="s">
+      <c r="V15" s="69"/>
+      <c r="W15" s="69"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="AD15" s="89"/>
-      <c r="AE15" s="89"/>
-      <c r="AF15" s="89"/>
-      <c r="AG15" s="89"/>
-      <c r="AH15" s="89"/>
-      <c r="AI15" s="89"/>
-      <c r="AJ15" s="89"/>
-      <c r="AL15" s="78" t="s">
+      <c r="AD15" s="71"/>
+      <c r="AE15" s="71"/>
+      <c r="AF15" s="71"/>
+      <c r="AG15" s="71"/>
+      <c r="AH15" s="71"/>
+      <c r="AI15" s="71"/>
+      <c r="AJ15" s="71"/>
+      <c r="AL15" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="AM15" s="52"/>
-      <c r="AN15" s="52"/>
-      <c r="AO15" s="52"/>
-      <c r="AP15" s="52"/>
-      <c r="AQ15" s="52"/>
-      <c r="AR15" s="52"/>
-      <c r="AS15" s="52"/>
-      <c r="AT15" s="52"/>
-      <c r="AU15" s="52"/>
-      <c r="AV15" s="52"/>
-      <c r="AW15" s="52"/>
-      <c r="AX15" s="52"/>
-      <c r="AY15" s="52"/>
-      <c r="AZ15" s="52"/>
-      <c r="BA15" s="52"/>
-      <c r="BB15" s="52"/>
-      <c r="BC15" s="52"/>
-      <c r="BD15" s="52"/>
-      <c r="BE15" s="52"/>
-      <c r="BF15" s="52"/>
-      <c r="BG15" s="52"/>
-      <c r="BH15" s="52"/>
-      <c r="BI15" s="52"/>
-      <c r="BJ15" s="52"/>
-      <c r="BK15" s="52"/>
-      <c r="BL15" s="52"/>
-      <c r="BM15" s="52"/>
-      <c r="BN15" s="52"/>
-      <c r="BO15" s="52"/>
-      <c r="BP15" s="52"/>
-      <c r="BQ15" s="52"/>
-      <c r="BR15" s="75" t="s">
+      <c r="AM15" s="66"/>
+      <c r="AN15" s="66"/>
+      <c r="AO15" s="66"/>
+      <c r="AP15" s="66"/>
+      <c r="AQ15" s="66"/>
+      <c r="AR15" s="66"/>
+      <c r="AS15" s="66"/>
+      <c r="AT15" s="66"/>
+      <c r="AU15" s="66"/>
+      <c r="AV15" s="66"/>
+      <c r="AW15" s="66"/>
+      <c r="AX15" s="66"/>
+      <c r="AY15" s="66"/>
+      <c r="AZ15" s="66"/>
+      <c r="BA15" s="66"/>
+      <c r="BB15" s="66"/>
+      <c r="BC15" s="66"/>
+      <c r="BD15" s="66"/>
+      <c r="BE15" s="66"/>
+      <c r="BF15" s="66"/>
+      <c r="BG15" s="66"/>
+      <c r="BH15" s="66"/>
+      <c r="BI15" s="66"/>
+      <c r="BJ15" s="66"/>
+      <c r="BK15" s="66"/>
+      <c r="BL15" s="66"/>
+      <c r="BM15" s="66"/>
+      <c r="BN15" s="66"/>
+      <c r="BO15" s="66"/>
+      <c r="BP15" s="66"/>
+      <c r="BQ15" s="66"/>
+      <c r="BR15" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="BS15" s="75"/>
-      <c r="BT15" s="75"/>
-      <c r="BU15" s="75"/>
-      <c r="BV15" s="75"/>
-      <c r="BW15" s="75"/>
-      <c r="BX15" s="75"/>
-      <c r="BY15" s="75"/>
-      <c r="BZ15" s="75" t="s">
+      <c r="BS15" s="57"/>
+      <c r="BT15" s="57"/>
+      <c r="BU15" s="57"/>
+      <c r="BV15" s="57"/>
+      <c r="BW15" s="57"/>
+      <c r="BX15" s="57"/>
+      <c r="BY15" s="57"/>
+      <c r="BZ15" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="CA15" s="75"/>
-      <c r="CB15" s="75"/>
-      <c r="CC15" s="75"/>
-      <c r="CD15" s="75"/>
-      <c r="CE15" s="75"/>
-      <c r="CF15" s="75"/>
-      <c r="CG15" s="75"/>
-      <c r="CH15" s="75" t="s">
+      <c r="CA15" s="57"/>
+      <c r="CB15" s="57"/>
+      <c r="CC15" s="57"/>
+      <c r="CD15" s="57"/>
+      <c r="CE15" s="57"/>
+      <c r="CF15" s="57"/>
+      <c r="CG15" s="57"/>
+      <c r="CH15" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="CI15" s="75"/>
-      <c r="CJ15" s="75"/>
-      <c r="CK15" s="75"/>
-      <c r="CL15" s="75"/>
-      <c r="CM15" s="75"/>
-      <c r="CN15" s="75"/>
-      <c r="CO15" s="75"/>
-      <c r="CP15" s="75" t="s">
+      <c r="CI15" s="57"/>
+      <c r="CJ15" s="57"/>
+      <c r="CK15" s="57"/>
+      <c r="CL15" s="57"/>
+      <c r="CM15" s="57"/>
+      <c r="CN15" s="57"/>
+      <c r="CO15" s="57"/>
+      <c r="CP15" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="CQ15" s="75"/>
-      <c r="CR15" s="75"/>
-      <c r="CS15" s="75"/>
-      <c r="CT15" s="75"/>
-      <c r="CU15" s="75"/>
-      <c r="CV15" s="75"/>
-      <c r="CW15" s="75"/>
+      <c r="CQ15" s="57"/>
+      <c r="CR15" s="57"/>
+      <c r="CS15" s="57"/>
+      <c r="CT15" s="57"/>
+      <c r="CU15" s="57"/>
+      <c r="CV15" s="57"/>
+      <c r="CW15" s="57"/>
       <c r="CX15" s="30" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:102">
-      <c r="A16" s="96" t="s">
+    <row r="16" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="96" t="s">
+      <c r="E16" s="52" t="s">
         <v>7</v>
       </c>
       <c r="G16" t="s">
@@ -3962,124 +3962,124 @@
       <c r="T16" s="14">
         <v>1</v>
       </c>
-      <c r="U16" s="87" t="s">
+      <c r="U16" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="V16" s="87"/>
-      <c r="W16" s="87"/>
-      <c r="X16" s="87"/>
-      <c r="Y16" s="87"/>
-      <c r="Z16" s="87"/>
-      <c r="AA16" s="87"/>
-      <c r="AB16" s="87"/>
-      <c r="AC16" s="88" t="s">
+      <c r="V16" s="69"/>
+      <c r="W16" s="69"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="69"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="69"/>
+      <c r="AC16" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="AD16" s="89"/>
-      <c r="AE16" s="89"/>
-      <c r="AF16" s="89"/>
-      <c r="AG16" s="89"/>
-      <c r="AH16" s="89"/>
-      <c r="AI16" s="89"/>
-      <c r="AJ16" s="89"/>
-      <c r="AL16" s="75" t="s">
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="71"/>
+      <c r="AF16" s="71"/>
+      <c r="AG16" s="71"/>
+      <c r="AH16" s="71"/>
+      <c r="AI16" s="71"/>
+      <c r="AJ16" s="71"/>
+      <c r="AL16" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="AM16" s="75"/>
-      <c r="AN16" s="75"/>
-      <c r="AO16" s="75"/>
-      <c r="AP16" s="75"/>
-      <c r="AQ16" s="75"/>
-      <c r="AR16" s="75"/>
-      <c r="AS16" s="75"/>
-      <c r="AT16" s="75" t="s">
+      <c r="AM16" s="57"/>
+      <c r="AN16" s="57"/>
+      <c r="AO16" s="57"/>
+      <c r="AP16" s="57"/>
+      <c r="AQ16" s="57"/>
+      <c r="AR16" s="57"/>
+      <c r="AS16" s="57"/>
+      <c r="AT16" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="AU16" s="75"/>
-      <c r="AV16" s="75"/>
-      <c r="AW16" s="75"/>
-      <c r="AX16" s="75"/>
-      <c r="AY16" s="75"/>
-      <c r="AZ16" s="75"/>
-      <c r="BA16" s="75"/>
-      <c r="BB16" s="75" t="s">
+      <c r="AU16" s="57"/>
+      <c r="AV16" s="57"/>
+      <c r="AW16" s="57"/>
+      <c r="AX16" s="57"/>
+      <c r="AY16" s="57"/>
+      <c r="AZ16" s="57"/>
+      <c r="BA16" s="57"/>
+      <c r="BB16" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="BC16" s="75"/>
-      <c r="BD16" s="75"/>
-      <c r="BE16" s="75"/>
-      <c r="BF16" s="75"/>
-      <c r="BG16" s="75"/>
-      <c r="BH16" s="75"/>
-      <c r="BI16" s="75"/>
-      <c r="BJ16" s="75" t="s">
+      <c r="BC16" s="57"/>
+      <c r="BD16" s="57"/>
+      <c r="BE16" s="57"/>
+      <c r="BF16" s="57"/>
+      <c r="BG16" s="57"/>
+      <c r="BH16" s="57"/>
+      <c r="BI16" s="57"/>
+      <c r="BJ16" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="BK16" s="75"/>
-      <c r="BL16" s="75"/>
-      <c r="BM16" s="75"/>
-      <c r="BN16" s="75"/>
-      <c r="BO16" s="75"/>
-      <c r="BP16" s="75"/>
-      <c r="BQ16" s="75"/>
-      <c r="BR16" s="75" t="s">
+      <c r="BK16" s="57"/>
+      <c r="BL16" s="57"/>
+      <c r="BM16" s="57"/>
+      <c r="BN16" s="57"/>
+      <c r="BO16" s="57"/>
+      <c r="BP16" s="57"/>
+      <c r="BQ16" s="57"/>
+      <c r="BR16" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="BS16" s="75"/>
-      <c r="BT16" s="75"/>
-      <c r="BU16" s="75"/>
-      <c r="BV16" s="75"/>
-      <c r="BW16" s="75"/>
-      <c r="BX16" s="75"/>
-      <c r="BY16" s="75"/>
-      <c r="BZ16" s="75" t="s">
+      <c r="BS16" s="57"/>
+      <c r="BT16" s="57"/>
+      <c r="BU16" s="57"/>
+      <c r="BV16" s="57"/>
+      <c r="BW16" s="57"/>
+      <c r="BX16" s="57"/>
+      <c r="BY16" s="57"/>
+      <c r="BZ16" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="CA16" s="75"/>
-      <c r="CB16" s="75"/>
-      <c r="CC16" s="75"/>
-      <c r="CD16" s="75"/>
-      <c r="CE16" s="75"/>
-      <c r="CF16" s="75"/>
-      <c r="CG16" s="75"/>
-      <c r="CH16" s="75" t="s">
+      <c r="CA16" s="57"/>
+      <c r="CB16" s="57"/>
+      <c r="CC16" s="57"/>
+      <c r="CD16" s="57"/>
+      <c r="CE16" s="57"/>
+      <c r="CF16" s="57"/>
+      <c r="CG16" s="57"/>
+      <c r="CH16" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="CI16" s="75"/>
-      <c r="CJ16" s="75"/>
-      <c r="CK16" s="75"/>
-      <c r="CL16" s="75"/>
-      <c r="CM16" s="75"/>
-      <c r="CN16" s="75"/>
-      <c r="CO16" s="75"/>
-      <c r="CP16" s="75" t="s">
+      <c r="CI16" s="57"/>
+      <c r="CJ16" s="57"/>
+      <c r="CK16" s="57"/>
+      <c r="CL16" s="57"/>
+      <c r="CM16" s="57"/>
+      <c r="CN16" s="57"/>
+      <c r="CO16" s="57"/>
+      <c r="CP16" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="CQ16" s="75"/>
-      <c r="CR16" s="75"/>
-      <c r="CS16" s="75"/>
-      <c r="CT16" s="75"/>
-      <c r="CU16" s="75"/>
-      <c r="CV16" s="75"/>
-      <c r="CW16" s="75"/>
+      <c r="CQ16" s="57"/>
+      <c r="CR16" s="57"/>
+      <c r="CS16" s="57"/>
+      <c r="CT16" s="57"/>
+      <c r="CU16" s="57"/>
+      <c r="CV16" s="57"/>
+      <c r="CW16" s="57"/>
       <c r="CX16" s="20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:102" ht="13" customHeight="1">
-      <c r="A17" s="96" t="s">
+    <row r="17" spans="1:102" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="96" t="s">
+      <c r="C17" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="96" t="s">
+      <c r="D17" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="96" t="s">
+      <c r="E17" s="52" t="s">
         <v>6</v>
       </c>
       <c r="G17" t="s">
@@ -4124,103 +4124,103 @@
       <c r="T17" s="14">
         <v>1</v>
       </c>
-      <c r="U17" s="87" t="s">
+      <c r="U17" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="V17" s="87"/>
-      <c r="W17" s="87"/>
-      <c r="X17" s="87"/>
-      <c r="Y17" s="87"/>
-      <c r="Z17" s="87"/>
-      <c r="AA17" s="87"/>
-      <c r="AB17" s="87"/>
-      <c r="AC17" s="88" t="s">
+      <c r="V17" s="69"/>
+      <c r="W17" s="69"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="69"/>
+      <c r="Z17" s="69"/>
+      <c r="AA17" s="69"/>
+      <c r="AB17" s="69"/>
+      <c r="AC17" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="AD17" s="89"/>
-      <c r="AE17" s="89"/>
-      <c r="AF17" s="89"/>
-      <c r="AG17" s="89"/>
-      <c r="AH17" s="89"/>
-      <c r="AI17" s="89"/>
-      <c r="AJ17" s="89"/>
-      <c r="AL17" s="78" t="s">
+      <c r="AD17" s="71"/>
+      <c r="AE17" s="71"/>
+      <c r="AF17" s="71"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AL17" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="52"/>
-      <c r="AO17" s="52"/>
-      <c r="AP17" s="52"/>
-      <c r="AQ17" s="52"/>
-      <c r="AR17" s="52"/>
-      <c r="AS17" s="52"/>
-      <c r="AT17" s="52"/>
-      <c r="AU17" s="52"/>
-      <c r="AV17" s="52"/>
-      <c r="AW17" s="52"/>
-      <c r="AX17" s="52"/>
-      <c r="AY17" s="52"/>
-      <c r="AZ17" s="52"/>
-      <c r="BA17" s="52"/>
-      <c r="BB17" s="52"/>
-      <c r="BC17" s="52"/>
-      <c r="BD17" s="52"/>
-      <c r="BE17" s="52"/>
-      <c r="BF17" s="52"/>
-      <c r="BG17" s="52"/>
-      <c r="BH17" s="52"/>
-      <c r="BI17" s="52"/>
-      <c r="BJ17" s="52"/>
-      <c r="BK17" s="52"/>
-      <c r="BL17" s="52"/>
-      <c r="BM17" s="52"/>
-      <c r="BN17" s="52"/>
-      <c r="BO17" s="52"/>
-      <c r="BP17" s="52"/>
-      <c r="BQ17" s="52"/>
-      <c r="BR17" s="85" t="s">
+      <c r="AM17" s="66"/>
+      <c r="AN17" s="66"/>
+      <c r="AO17" s="66"/>
+      <c r="AP17" s="66"/>
+      <c r="AQ17" s="66"/>
+      <c r="AR17" s="66"/>
+      <c r="AS17" s="66"/>
+      <c r="AT17" s="66"/>
+      <c r="AU17" s="66"/>
+      <c r="AV17" s="66"/>
+      <c r="AW17" s="66"/>
+      <c r="AX17" s="66"/>
+      <c r="AY17" s="66"/>
+      <c r="AZ17" s="66"/>
+      <c r="BA17" s="66"/>
+      <c r="BB17" s="66"/>
+      <c r="BC17" s="66"/>
+      <c r="BD17" s="66"/>
+      <c r="BE17" s="66"/>
+      <c r="BF17" s="66"/>
+      <c r="BG17" s="66"/>
+      <c r="BH17" s="66"/>
+      <c r="BI17" s="66"/>
+      <c r="BJ17" s="66"/>
+      <c r="BK17" s="66"/>
+      <c r="BL17" s="66"/>
+      <c r="BM17" s="66"/>
+      <c r="BN17" s="66"/>
+      <c r="BO17" s="66"/>
+      <c r="BP17" s="66"/>
+      <c r="BQ17" s="66"/>
+      <c r="BR17" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="BS17" s="85"/>
-      <c r="BT17" s="85"/>
-      <c r="BU17" s="85"/>
-      <c r="BV17" s="85"/>
-      <c r="BW17" s="85"/>
-      <c r="BX17" s="85"/>
-      <c r="BY17" s="85"/>
-      <c r="BZ17" s="86" t="s">
+      <c r="BS17" s="67"/>
+      <c r="BT17" s="67"/>
+      <c r="BU17" s="67"/>
+      <c r="BV17" s="67"/>
+      <c r="BW17" s="67"/>
+      <c r="BX17" s="67"/>
+      <c r="BY17" s="67"/>
+      <c r="BZ17" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="CA17" s="86"/>
-      <c r="CB17" s="86"/>
-      <c r="CC17" s="86"/>
-      <c r="CD17" s="86"/>
-      <c r="CE17" s="86"/>
-      <c r="CF17" s="86"/>
-      <c r="CG17" s="86"/>
-      <c r="CH17" s="53" t="s">
+      <c r="CA17" s="68"/>
+      <c r="CB17" s="68"/>
+      <c r="CC17" s="68"/>
+      <c r="CD17" s="68"/>
+      <c r="CE17" s="68"/>
+      <c r="CF17" s="68"/>
+      <c r="CG17" s="68"/>
+      <c r="CH17" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="CI17" s="53"/>
-      <c r="CJ17" s="53"/>
-      <c r="CK17" s="53"/>
-      <c r="CL17" s="53"/>
-      <c r="CM17" s="53"/>
-      <c r="CN17" s="53"/>
-      <c r="CO17" s="53"/>
-      <c r="CP17" s="53"/>
-      <c r="CQ17" s="53"/>
-      <c r="CR17" s="53"/>
-      <c r="CS17" s="53"/>
-      <c r="CT17" s="53"/>
-      <c r="CU17" s="53"/>
-      <c r="CV17" s="53"/>
-      <c r="CW17" s="53"/>
+      <c r="CI17" s="65"/>
+      <c r="CJ17" s="65"/>
+      <c r="CK17" s="65"/>
+      <c r="CL17" s="65"/>
+      <c r="CM17" s="65"/>
+      <c r="CN17" s="65"/>
+      <c r="CO17" s="65"/>
+      <c r="CP17" s="65"/>
+      <c r="CQ17" s="65"/>
+      <c r="CR17" s="65"/>
+      <c r="CS17" s="65"/>
+      <c r="CT17" s="65"/>
+      <c r="CU17" s="65"/>
+      <c r="CV17" s="65"/>
+      <c r="CW17" s="65"/>
       <c r="CX17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:102" s="31" customFormat="1" hidden="1">
+    <row r="18" spans="1:102" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>24</v>
       </c>
@@ -4278,16 +4278,16 @@
       <c r="T18" s="38">
         <v>1</v>
       </c>
-      <c r="U18" s="93" t="s">
+      <c r="U18" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="V18" s="93"/>
-      <c r="W18" s="93"/>
-      <c r="X18" s="93"/>
-      <c r="Y18" s="93"/>
-      <c r="Z18" s="93"/>
-      <c r="AA18" s="93"/>
-      <c r="AB18" s="93"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
       <c r="AC18" s="12">
         <v>0</v>
       </c>
@@ -4327,46 +4327,46 @@
       <c r="CS18" s="35"/>
       <c r="CW18" s="36"/>
     </row>
-    <row r="19" spans="1:102" ht="15" thickBot="1">
+    <row r="19" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="76" t="s">
+      <c r="I19" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="76"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="80" t="s">
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="80"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="80"/>
-      <c r="R19" s="80"/>
-      <c r="S19" s="80"/>
-      <c r="T19" s="80"/>
-      <c r="U19" s="79" t="s">
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79"/>
+      <c r="R19" s="79"/>
+      <c r="S19" s="79"/>
+      <c r="T19" s="79"/>
+      <c r="U19" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="V19" s="79"/>
-      <c r="W19" s="79"/>
-      <c r="X19" s="79"/>
-      <c r="Y19" s="79"/>
-      <c r="Z19" s="79"/>
-      <c r="AA19" s="79"/>
-      <c r="AB19" s="79"/>
-      <c r="AC19" s="71" t="s">
+      <c r="V19" s="78"/>
+      <c r="W19" s="78"/>
+      <c r="X19" s="78"/>
+      <c r="Y19" s="78"/>
+      <c r="Z19" s="78"/>
+      <c r="AA19" s="78"/>
+      <c r="AB19" s="78"/>
+      <c r="AC19" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="AD19" s="71"/>
-      <c r="AE19" s="71"/>
-      <c r="AF19" s="71"/>
-      <c r="AG19" s="71"/>
-      <c r="AH19" s="71"/>
-      <c r="AI19" s="71"/>
-      <c r="AJ19" s="71"/>
+      <c r="AD19" s="86"/>
+      <c r="AE19" s="86"/>
+      <c r="AF19" s="86"/>
+      <c r="AG19" s="86"/>
+      <c r="AH19" s="86"/>
+      <c r="AI19" s="86"/>
+      <c r="AJ19" s="86"/>
       <c r="AK19" s="42"/>
       <c r="AS19" s="17"/>
       <c r="AU19" s="3"/>
@@ -4382,76 +4382,76 @@
       <c r="CS19" s="3"/>
       <c r="CW19" s="17"/>
     </row>
-    <row r="21" spans="1:102">
+    <row r="21" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AL21" s="91">
+      <c r="AL21" s="61">
         <v>1098</v>
       </c>
-      <c r="AM21" s="75"/>
-      <c r="AN21" s="75"/>
-      <c r="AO21" s="75"/>
-      <c r="AP21" s="75"/>
-      <c r="AQ21" s="75"/>
-      <c r="AR21" s="75"/>
-      <c r="AS21" s="75"/>
-      <c r="AT21" s="75"/>
-      <c r="AU21" s="75"/>
-      <c r="AV21" s="75"/>
-      <c r="AW21" s="75"/>
-      <c r="AX21" s="75"/>
-      <c r="AY21" s="75"/>
-      <c r="AZ21" s="75"/>
-      <c r="BA21" s="75"/>
-      <c r="BB21" s="75"/>
-      <c r="BC21" s="75"/>
-      <c r="BD21" s="75"/>
-      <c r="BE21" s="75"/>
-      <c r="BF21" s="75"/>
-      <c r="BG21" s="75"/>
-      <c r="BH21" s="75"/>
-      <c r="BI21" s="75"/>
-      <c r="BJ21" s="75"/>
-      <c r="BK21" s="75"/>
-      <c r="BL21" s="75"/>
-      <c r="BM21" s="75"/>
-      <c r="BN21" s="75"/>
-      <c r="BO21" s="75"/>
-      <c r="BP21" s="75"/>
-      <c r="BQ21" s="75"/>
-      <c r="BR21" s="75">
+      <c r="AM21" s="57"/>
+      <c r="AN21" s="57"/>
+      <c r="AO21" s="57"/>
+      <c r="AP21" s="57"/>
+      <c r="AQ21" s="57"/>
+      <c r="AR21" s="57"/>
+      <c r="AS21" s="57"/>
+      <c r="AT21" s="57"/>
+      <c r="AU21" s="57"/>
+      <c r="AV21" s="57"/>
+      <c r="AW21" s="57"/>
+      <c r="AX21" s="57"/>
+      <c r="AY21" s="57"/>
+      <c r="AZ21" s="57"/>
+      <c r="BA21" s="57"/>
+      <c r="BB21" s="57"/>
+      <c r="BC21" s="57"/>
+      <c r="BD21" s="57"/>
+      <c r="BE21" s="57"/>
+      <c r="BF21" s="57"/>
+      <c r="BG21" s="57"/>
+      <c r="BH21" s="57"/>
+      <c r="BI21" s="57"/>
+      <c r="BJ21" s="57"/>
+      <c r="BK21" s="57"/>
+      <c r="BL21" s="57"/>
+      <c r="BM21" s="57"/>
+      <c r="BN21" s="57"/>
+      <c r="BO21" s="57"/>
+      <c r="BP21" s="57"/>
+      <c r="BQ21" s="57"/>
+      <c r="BR21" s="57">
         <v>26</v>
       </c>
-      <c r="BS21" s="75"/>
-      <c r="BT21" s="75"/>
-      <c r="BU21" s="75"/>
-      <c r="BV21" s="75"/>
-      <c r="BW21" s="75"/>
-      <c r="BX21" s="75"/>
-      <c r="BY21" s="75"/>
-      <c r="BZ21" s="75">
+      <c r="BS21" s="57"/>
+      <c r="BT21" s="57"/>
+      <c r="BU21" s="57"/>
+      <c r="BV21" s="57"/>
+      <c r="BW21" s="57"/>
+      <c r="BX21" s="57"/>
+      <c r="BY21" s="57"/>
+      <c r="BZ21" s="57">
         <v>137</v>
       </c>
-      <c r="CA21" s="75"/>
-      <c r="CB21" s="75"/>
-      <c r="CC21" s="75"/>
-      <c r="CD21" s="75"/>
-      <c r="CE21" s="75"/>
-      <c r="CF21" s="75"/>
-      <c r="CG21" s="75"/>
-      <c r="CH21" s="75">
+      <c r="CA21" s="57"/>
+      <c r="CB21" s="57"/>
+      <c r="CC21" s="57"/>
+      <c r="CD21" s="57"/>
+      <c r="CE21" s="57"/>
+      <c r="CF21" s="57"/>
+      <c r="CG21" s="57"/>
+      <c r="CH21" s="57">
         <v>8</v>
       </c>
-      <c r="CI21" s="75"/>
-      <c r="CJ21" s="75"/>
-      <c r="CK21" s="75"/>
-      <c r="CL21" s="75"/>
-      <c r="CM21" s="75"/>
-      <c r="CN21" s="75"/>
-      <c r="CO21" s="75"/>
-    </row>
-    <row r="22" spans="1:102">
+      <c r="CI21" s="57"/>
+      <c r="CJ21" s="57"/>
+      <c r="CK21" s="57"/>
+      <c r="CL21" s="57"/>
+      <c r="CM21" s="57"/>
+      <c r="CN21" s="57"/>
+      <c r="CO21" s="57"/>
+    </row>
+    <row r="22" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>77</v>
       </c>
@@ -4556,80 +4556,80 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:102">
-      <c r="H23" s="55">
+    <row r="23" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="H23" s="88">
         <v>18</v>
       </c>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="60" t="s">
+      <c r="I23" s="88"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="61"/>
-      <c r="U23" s="60" t="s">
+      <c r="N23" s="84"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="84"/>
+      <c r="S23" s="84"/>
+      <c r="T23" s="85"/>
+      <c r="U23" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="61"/>
-      <c r="AC23" s="59" t="s">
+      <c r="V23" s="84"/>
+      <c r="W23" s="84"/>
+      <c r="X23" s="84"/>
+      <c r="Y23" s="84"/>
+      <c r="Z23" s="84"/>
+      <c r="AA23" s="84"/>
+      <c r="AB23" s="85"/>
+      <c r="AC23" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="AD23" s="55"/>
-      <c r="AE23" s="55"/>
-      <c r="AF23" s="55"/>
-      <c r="AG23" s="55"/>
-      <c r="AH23" s="55"/>
-      <c r="AI23" s="55"/>
-      <c r="AJ23" s="56"/>
+      <c r="AD23" s="88"/>
+      <c r="AE23" s="88"/>
+      <c r="AF23" s="88"/>
+      <c r="AG23" s="88"/>
+      <c r="AH23" s="88"/>
+      <c r="AI23" s="88"/>
+      <c r="AJ23" s="89"/>
       <c r="AK23" s="9"/>
       <c r="AM23" t="s">
         <v>197</v>
       </c>
-      <c r="BR23" s="75" t="s">
+      <c r="BR23" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="BS23" s="75"/>
-      <c r="BT23" s="75"/>
-      <c r="BU23" s="75"/>
-      <c r="BV23" s="75"/>
-      <c r="BW23" s="75"/>
-      <c r="BX23" s="75"/>
-      <c r="BY23" s="75"/>
-      <c r="BZ23" s="75">
+      <c r="BS23" s="57"/>
+      <c r="BT23" s="57"/>
+      <c r="BU23" s="57"/>
+      <c r="BV23" s="57"/>
+      <c r="BW23" s="57"/>
+      <c r="BX23" s="57"/>
+      <c r="BY23" s="57"/>
+      <c r="BZ23" s="57">
         <v>16</v>
       </c>
-      <c r="CA23" s="75"/>
-      <c r="CB23" s="75"/>
-      <c r="CC23" s="75"/>
-      <c r="CD23" s="75"/>
-      <c r="CE23" s="75"/>
-      <c r="CF23" s="75"/>
-      <c r="CG23" s="75"/>
-      <c r="CH23" s="75" t="s">
+      <c r="CA23" s="57"/>
+      <c r="CB23" s="57"/>
+      <c r="CC23" s="57"/>
+      <c r="CD23" s="57"/>
+      <c r="CE23" s="57"/>
+      <c r="CF23" s="57"/>
+      <c r="CG23" s="57"/>
+      <c r="CH23" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="CI23" s="75"/>
-      <c r="CJ23" s="75"/>
-      <c r="CK23" s="75"/>
-      <c r="CL23" s="75"/>
-      <c r="CM23" s="75"/>
-      <c r="CN23" s="75"/>
-      <c r="CO23" s="75"/>
-    </row>
-    <row r="24" spans="1:102">
+      <c r="CI23" s="57"/>
+      <c r="CJ23" s="57"/>
+      <c r="CK23" s="57"/>
+      <c r="CL23" s="57"/>
+      <c r="CM23" s="57"/>
+      <c r="CN23" s="57"/>
+      <c r="CO23" s="57"/>
+    </row>
+    <row r="24" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>78</v>
       </c>
@@ -4722,50 +4722,50 @@
       </c>
       <c r="AK24" s="9"/>
     </row>
-    <row r="25" spans="1:102">
-      <c r="H25" s="55">
+    <row r="25" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="H25" s="88">
         <v>18</v>
       </c>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="60" t="s">
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="61"/>
-      <c r="U25" s="60" t="s">
+      <c r="N25" s="84"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="84"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="V25" s="54"/>
-      <c r="W25" s="54"/>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="54"/>
-      <c r="Z25" s="54"/>
-      <c r="AA25" s="54"/>
-      <c r="AB25" s="61"/>
-      <c r="AC25" s="60" t="s">
+      <c r="V25" s="84"/>
+      <c r="W25" s="84"/>
+      <c r="X25" s="84"/>
+      <c r="Y25" s="84"/>
+      <c r="Z25" s="84"/>
+      <c r="AA25" s="84"/>
+      <c r="AB25" s="85"/>
+      <c r="AC25" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="AD25" s="54"/>
-      <c r="AE25" s="54"/>
-      <c r="AF25" s="54"/>
-      <c r="AG25" s="54"/>
-      <c r="AH25" s="54"/>
-      <c r="AI25" s="54"/>
-      <c r="AJ25" s="61"/>
+      <c r="AD25" s="84"/>
+      <c r="AE25" s="84"/>
+      <c r="AF25" s="84"/>
+      <c r="AG25" s="84"/>
+      <c r="AH25" s="84"/>
+      <c r="AI25" s="84"/>
+      <c r="AJ25" s="85"/>
       <c r="AK25" s="9"/>
       <c r="AM25" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:102" ht="2.25" customHeight="1">
+    <row r="26" spans="1:102" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H26" s="25"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
@@ -4797,7 +4797,7 @@
       <c r="AJ26" s="26"/>
       <c r="AK26" s="9"/>
     </row>
-    <row r="27" spans="1:102">
+    <row r="27" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
         <v>79</v>
       </c>
@@ -4890,47 +4890,47 @@
       </c>
       <c r="AK27" s="9"/>
     </row>
-    <row r="28" spans="1:102">
-      <c r="H28" s="55">
+    <row r="28" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="H28" s="88">
         <v>18</v>
       </c>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="60" t="s">
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="N28" s="54"/>
-      <c r="O28" s="54"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="54"/>
-      <c r="T28" s="61"/>
-      <c r="U28" s="59" t="s">
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="84"/>
+      <c r="Q28" s="84"/>
+      <c r="R28" s="84"/>
+      <c r="S28" s="84"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="55"/>
-      <c r="Z28" s="55"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="56"/>
-      <c r="AC28" s="72" t="s">
+      <c r="V28" s="88"/>
+      <c r="W28" s="88"/>
+      <c r="X28" s="88"/>
+      <c r="Y28" s="88"/>
+      <c r="Z28" s="88"/>
+      <c r="AA28" s="88"/>
+      <c r="AB28" s="89"/>
+      <c r="AC28" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="AD28" s="73"/>
-      <c r="AE28" s="73"/>
-      <c r="AF28" s="73"/>
-      <c r="AG28" s="73"/>
-      <c r="AH28" s="73"/>
-      <c r="AI28" s="73"/>
-      <c r="AJ28" s="74"/>
+      <c r="AD28" s="91"/>
+      <c r="AE28" s="91"/>
+      <c r="AF28" s="91"/>
+      <c r="AG28" s="91"/>
+      <c r="AH28" s="91"/>
+      <c r="AI28" s="91"/>
+      <c r="AJ28" s="92"/>
       <c r="AK28" s="9"/>
     </row>
-    <row r="29" spans="1:102">
+    <row r="29" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>86</v>
       </c>
@@ -4997,59 +4997,59 @@
       <c r="AB29" s="26">
         <v>1</v>
       </c>
-      <c r="AC29" s="68" t="s">
+      <c r="AC29" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="AD29" s="69"/>
-      <c r="AE29" s="69"/>
-      <c r="AF29" s="69"/>
-      <c r="AG29" s="69"/>
-      <c r="AH29" s="69"/>
-      <c r="AI29" s="69"/>
-      <c r="AJ29" s="70"/>
+      <c r="AD29" s="102"/>
+      <c r="AE29" s="102"/>
+      <c r="AF29" s="102"/>
+      <c r="AG29" s="102"/>
+      <c r="AH29" s="102"/>
+      <c r="AI29" s="102"/>
+      <c r="AJ29" s="103"/>
       <c r="AK29" s="9"/>
     </row>
-    <row r="30" spans="1:102">
-      <c r="H30" s="54" t="s">
+    <row r="30" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="H30" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="60" t="s">
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="61"/>
-      <c r="U30" s="60" t="s">
+      <c r="N30" s="84"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="84"/>
+      <c r="Q30" s="84"/>
+      <c r="R30" s="84"/>
+      <c r="S30" s="84"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="54"/>
-      <c r="Y30" s="54"/>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="61"/>
-      <c r="AC30" s="59" t="s">
+      <c r="V30" s="84"/>
+      <c r="W30" s="84"/>
+      <c r="X30" s="84"/>
+      <c r="Y30" s="84"/>
+      <c r="Z30" s="84"/>
+      <c r="AA30" s="84"/>
+      <c r="AB30" s="85"/>
+      <c r="AC30" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="AD30" s="55"/>
-      <c r="AE30" s="55"/>
-      <c r="AF30" s="55"/>
-      <c r="AG30" s="55"/>
-      <c r="AH30" s="55"/>
-      <c r="AI30" s="55"/>
-      <c r="AJ30" s="56"/>
+      <c r="AD30" s="88"/>
+      <c r="AE30" s="88"/>
+      <c r="AF30" s="88"/>
+      <c r="AG30" s="88"/>
+      <c r="AH30" s="88"/>
+      <c r="AI30" s="88"/>
+      <c r="AJ30" s="89"/>
       <c r="AK30" s="9"/>
     </row>
-    <row r="31" spans="1:102">
+    <row r="31" spans="1:102" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>85</v>
       </c>
@@ -5142,44 +5142,44 @@
       </c>
       <c r="AK31" s="9"/>
     </row>
-    <row r="32" spans="1:102">
-      <c r="H32" s="54" t="s">
+    <row r="32" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="H32" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="62" t="s">
+      <c r="I32" s="88"/>
+      <c r="J32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="62" t="s">
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="96"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="97"/>
+      <c r="U32" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="V32" s="63"/>
-      <c r="W32" s="63"/>
-      <c r="X32" s="63"/>
-      <c r="Y32" s="63"/>
-      <c r="Z32" s="63"/>
-      <c r="AA32" s="63"/>
-      <c r="AB32" s="64"/>
-      <c r="AC32" s="65" t="s">
+      <c r="V32" s="96"/>
+      <c r="W32" s="96"/>
+      <c r="X32" s="96"/>
+      <c r="Y32" s="96"/>
+      <c r="Z32" s="96"/>
+      <c r="AA32" s="96"/>
+      <c r="AB32" s="97"/>
+      <c r="AC32" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="AD32" s="66"/>
-      <c r="AE32" s="66"/>
-      <c r="AF32" s="66"/>
-      <c r="AG32" s="66"/>
-      <c r="AH32" s="66"/>
-      <c r="AI32" s="66"/>
-      <c r="AJ32" s="67"/>
+      <c r="AD32" s="99"/>
+      <c r="AE32" s="99"/>
+      <c r="AF32" s="99"/>
+      <c r="AG32" s="99"/>
+      <c r="AH32" s="99"/>
+      <c r="AI32" s="99"/>
+      <c r="AJ32" s="100"/>
     </row>
   </sheetData>
   <sortState ref="A3:AK15">
@@ -5190,28 +5190,46 @@
     <sortCondition ref="L3:L15"/>
   </sortState>
   <mergeCells count="78">
-    <mergeCell ref="BR23:BY23"/>
-    <mergeCell ref="BZ23:CG23"/>
-    <mergeCell ref="CH23:CO23"/>
-    <mergeCell ref="BR21:BY21"/>
-    <mergeCell ref="BZ21:CG21"/>
-    <mergeCell ref="CH21:CO21"/>
-    <mergeCell ref="BZ15:CG15"/>
-    <mergeCell ref="U18:AB18"/>
-    <mergeCell ref="AL16:AS16"/>
-    <mergeCell ref="AT16:BA16"/>
-    <mergeCell ref="BJ16:BQ16"/>
-    <mergeCell ref="BB16:BI16"/>
-    <mergeCell ref="AL14:BA14"/>
-    <mergeCell ref="AL21:BQ21"/>
-    <mergeCell ref="AT4:BY4"/>
-    <mergeCell ref="M8:T8"/>
-    <mergeCell ref="BR15:BY15"/>
-    <mergeCell ref="M7:T7"/>
-    <mergeCell ref="AV8:BE8"/>
-    <mergeCell ref="BF8:BQ8"/>
-    <mergeCell ref="M11:T11"/>
-    <mergeCell ref="AL11:AS11"/>
+    <mergeCell ref="CH17:CW17"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="AL13:BQ13"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="AC30:AJ30"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="M30:T30"/>
+    <mergeCell ref="M32:T32"/>
+    <mergeCell ref="U32:AB32"/>
+    <mergeCell ref="AC32:AJ32"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="AC29:AJ29"/>
+    <mergeCell ref="AC23:AJ23"/>
+    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="AC19:AJ19"/>
+    <mergeCell ref="M23:T23"/>
+    <mergeCell ref="M25:T25"/>
+    <mergeCell ref="M28:T28"/>
+    <mergeCell ref="U28:AB28"/>
+    <mergeCell ref="AC28:AJ28"/>
+    <mergeCell ref="AC25:AJ25"/>
+    <mergeCell ref="U25:AB25"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="AL1:CW1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="S1:AJ1"/>
+    <mergeCell ref="AL7:AS7"/>
+    <mergeCell ref="AL17:BQ17"/>
+    <mergeCell ref="BB14:BY14"/>
+    <mergeCell ref="U19:AB19"/>
+    <mergeCell ref="M19:T19"/>
+    <mergeCell ref="AL8:AU8"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="BR8:CG8"/>
+    <mergeCell ref="AL12:AS12"/>
+    <mergeCell ref="AL15:BQ15"/>
+    <mergeCell ref="CH8:CW8"/>
     <mergeCell ref="CP15:CW15"/>
     <mergeCell ref="M9:T9"/>
     <mergeCell ref="BR17:BY17"/>
@@ -5228,46 +5246,28 @@
     <mergeCell ref="U17:AB17"/>
     <mergeCell ref="U14:AB14"/>
     <mergeCell ref="CH15:CO15"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="AL1:CW1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:R1"/>
-    <mergeCell ref="S1:AJ1"/>
-    <mergeCell ref="AL7:AS7"/>
-    <mergeCell ref="AL17:BQ17"/>
-    <mergeCell ref="BB14:BY14"/>
-    <mergeCell ref="U19:AB19"/>
-    <mergeCell ref="M19:T19"/>
-    <mergeCell ref="AL8:AU8"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="BR8:CG8"/>
-    <mergeCell ref="AL12:AS12"/>
-    <mergeCell ref="AL15:BQ15"/>
-    <mergeCell ref="U23:AB23"/>
-    <mergeCell ref="AC19:AJ19"/>
-    <mergeCell ref="M23:T23"/>
-    <mergeCell ref="M25:T25"/>
-    <mergeCell ref="M28:T28"/>
-    <mergeCell ref="U28:AB28"/>
-    <mergeCell ref="AC28:AJ28"/>
-    <mergeCell ref="AC25:AJ25"/>
-    <mergeCell ref="U25:AB25"/>
-    <mergeCell ref="CH8:CW8"/>
-    <mergeCell ref="CH17:CW17"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="AL13:BQ13"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="AC30:AJ30"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="M30:T30"/>
-    <mergeCell ref="M32:T32"/>
-    <mergeCell ref="U32:AB32"/>
-    <mergeCell ref="AC32:AJ32"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="AC29:AJ29"/>
-    <mergeCell ref="AC23:AJ23"/>
+    <mergeCell ref="AL14:BA14"/>
+    <mergeCell ref="AL21:BQ21"/>
+    <mergeCell ref="AT4:BY4"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="BR15:BY15"/>
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="AV8:BE8"/>
+    <mergeCell ref="BF8:BQ8"/>
+    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="AL11:AS11"/>
+    <mergeCell ref="BZ15:CG15"/>
+    <mergeCell ref="U18:AB18"/>
+    <mergeCell ref="AL16:AS16"/>
+    <mergeCell ref="AT16:BA16"/>
+    <mergeCell ref="BJ16:BQ16"/>
+    <mergeCell ref="BB16:BI16"/>
+    <mergeCell ref="BR23:BY23"/>
+    <mergeCell ref="BZ23:CG23"/>
+    <mergeCell ref="CH23:CO23"/>
+    <mergeCell ref="BR21:BY21"/>
+    <mergeCell ref="BZ21:CG21"/>
+    <mergeCell ref="CH21:CO21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.79000000000000015" bottom="0.79000000000000015" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -5288,24 +5288,24 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>40</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -5533,9 +5533,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>129</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>131</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>133</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>135</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>137</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>139</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>141</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>143</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>145</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>147</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>149</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>151</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>153</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>155</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>157</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>159</v>
       </c>

</xml_diff>